<commit_message>
back to initial content
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="355">
   <si>
     <t>parameter</t>
   </si>
@@ -1082,9 +1082,6 @@
   </si>
   <si>
     <t>proportion of data points used in the loess regressions of the rate by age; groups: district, year, sex</t>
-  </si>
-  <si>
-    <t>asdfasdfasdfasdfasdf</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1689,7 +1686,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>355</v>
+        <v>23</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
new parameters for dao (relocation on immigration*)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="361">
   <si>
     <t>parameter</t>
   </si>
@@ -904,9 +904,6 @@
     <t>when immigration* is above this threshold: proportion with district (and year, age, origin), below without district (but with year, age, origin). Value must be higher than rei_ims_thres_o.</t>
   </si>
   <si>
-    <t>when immigration* is above this threshold: proportion with oritin (and year, age), below without origin (but with year, age). Value must be lower than rei_ims_thres_d.</t>
-  </si>
-  <si>
     <t>ree_ems_span_yao</t>
   </si>
   <si>
@@ -1082,6 +1079,27 @@
   </si>
   <si>
     <t>proportion of data points used in the loess regressions of the rate by age; groups: district, year, sex</t>
+  </si>
+  <si>
+    <t>rei_ims_span_dao</t>
+  </si>
+  <si>
+    <t>rei_rel_span_dao</t>
+  </si>
+  <si>
+    <t>proportion of data points used in the loess regressions of immigration* by age; groups: district, origin</t>
+  </si>
+  <si>
+    <t>proportion of data points used in the loess regressions of relocation by age; groups: district, origin</t>
+  </si>
+  <si>
+    <t>rei_ims_thres_y</t>
+  </si>
+  <si>
+    <t>when immigration* is above this threshold: proportion with origin (and year, age), below without origin (but with year, age). Value must be lower than rei_ims_thres_d.</t>
+  </si>
+  <si>
+    <t>when immigration* is above this threshold: proportion with year (and district, age, origin), below without year (but with district, age, origin).</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1298,6 +1316,10 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1617,11 +1639,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J143"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2506,7 +2528,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>107</v>
@@ -2538,7 +2560,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>107</v>
@@ -2570,7 +2592,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>107</v>
@@ -2602,7 +2624,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>107</v>
@@ -2634,7 +2656,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>107</v>
@@ -2649,7 +2671,7 @@
         <v>24</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H32" s="10">
         <v>2011</v>
@@ -2666,7 +2688,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>107</v>
@@ -2681,7 +2703,7 @@
         <v>24</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H33" s="10">
         <v>2020</v>
@@ -3365,7 +3387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>22</v>
       </c>
@@ -4697,68 +4719,68 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="11" t="s">
+    <row r="97" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="B97" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C97" s="6" t="s">
+      <c r="B97" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="C97" s="35" t="s">
         <v>241</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="35">
         <v>0.15</v>
       </c>
-      <c r="E97" s="11" t="s">
+      <c r="E97" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F97" s="11" t="s">
+      <c r="F97" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G97" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="H97" s="6">
+      <c r="G97" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="H97" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="I97" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="J97" s="35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B98" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="C98" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D98" s="35">
         <v>0.15</v>
       </c>
-      <c r="I97" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="J97" s="6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D98" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="E98" s="11" t="s">
+      <c r="E98" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="F98" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G98" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="H98" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="I98" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="J98" s="6">
-        <v>0.15</v>
+      <c r="G98" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="H98" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="I98" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="J98" s="35">
+        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4766,13 +4788,13 @@
         <v>236</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D99" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E99" s="11" t="s">
         <v>93</v>
@@ -4781,16 +4803,16 @@
         <v>66</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H99" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I99" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J99" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4798,13 +4820,13 @@
         <v>236</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D100" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>93</v>
@@ -4813,16 +4835,16 @@
         <v>66</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H100" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I100" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J100" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="101" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4830,31 +4852,31 @@
         <v>236</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D101" s="6">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G101" s="11" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="H101" s="6">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="I101" s="6">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="J101" s="6">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="102" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4862,22 +4884,22 @@
         <v>236</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D102" s="6">
         <v>0.1</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
       <c r="H102" s="6">
         <v>0.1</v>
@@ -4894,127 +4916,127 @@
         <v>236</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D103" s="6">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>93</v>
+        <v>250</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G103" s="11" t="s">
-        <v>251</v>
+        <v>294</v>
       </c>
       <c r="H103" s="6">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="I103" s="6">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="J103" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>268</v>
+        <v>291</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D104" s="12">
-        <v>20</v>
+        <v>249</v>
+      </c>
+      <c r="D104" s="6">
+        <v>0.1</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>49</v>
+        <v>250</v>
       </c>
       <c r="F104" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G104" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="H104" s="12">
-        <v>20</v>
-      </c>
-      <c r="I104" s="12">
-        <v>20</v>
-      </c>
-      <c r="J104" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A105" s="11" t="s">
+      <c r="G104" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="H104" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I104" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J104" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="B105" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D105" s="12">
-        <v>20</v>
-      </c>
-      <c r="E105" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F105" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G105" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H105" s="12">
-        <v>20</v>
-      </c>
-      <c r="I105" s="12">
-        <v>20</v>
-      </c>
-      <c r="J105" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B105" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="C105" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="D105" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="E105" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="F105" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G105" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="H105" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="I105" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="J105" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D106" s="12">
-        <v>13</v>
+        <v>241</v>
+      </c>
+      <c r="D106" s="6">
+        <v>0.3</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F106" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="H106" s="12">
-        <v>13</v>
-      </c>
-      <c r="I106" s="12">
-        <v>13</v>
-      </c>
-      <c r="J106" s="12">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H106" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I106" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J106" s="6">
+        <v>0.3</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -5022,223 +5044,223 @@
         <v>236</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>107</v>
+        <v>256</v>
       </c>
       <c r="D107" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>49</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G107" s="13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H107" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I107" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J107" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D108" s="12">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>49</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G108" s="13" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H108" s="12">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="I108" s="12">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J108" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B109" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D109" s="12">
+        <v>13</v>
+      </c>
+      <c r="E109" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F109" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G109" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="H109" s="12">
+        <v>13</v>
+      </c>
+      <c r="I109" s="12">
+        <v>13</v>
+      </c>
+      <c r="J109" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A110" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D110" s="12">
+        <v>0</v>
+      </c>
+      <c r="E110" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G110" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H110" s="12">
+        <v>0</v>
+      </c>
+      <c r="I110" s="12">
+        <v>0</v>
+      </c>
+      <c r="J110" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D111" s="12">
+        <v>100</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G111" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="H111" s="12">
+        <v>100</v>
+      </c>
+      <c r="I111" s="12">
+        <v>100</v>
+      </c>
+      <c r="J111" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B112" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="C112" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D112" s="6">
         <v>0.15</v>
       </c>
-      <c r="E109" s="11" t="s">
+      <c r="E112" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="F112" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G109" s="11" t="s">
+      <c r="G112" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="H109" s="6">
+      <c r="H112" s="6">
         <v>0.15</v>
       </c>
-      <c r="I109" s="6">
+      <c r="I112" s="6">
         <v>0.15</v>
       </c>
-      <c r="J109" s="6">
+      <c r="J112" s="6">
         <v>0.15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A110" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B110" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="D110" s="29">
-        <v>70</v>
-      </c>
-      <c r="E110" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F110" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G110" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="H110" s="29">
-        <v>70</v>
-      </c>
-      <c r="I110" s="29">
-        <v>70</v>
-      </c>
-      <c r="J110" s="29">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A111" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B111" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D111" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E111" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F111" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G111" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="H111" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="I111" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="J111" s="14">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A112" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B112" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D112" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E112" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F112" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G112" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="H112" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="I112" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="J112" s="14">
-        <v>0.2</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="B113" s="27" t="s">
-        <v>296</v>
+      <c r="B113" s="14" t="s">
+        <v>285</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D113" s="14">
-        <v>0.15</v>
+        <v>235</v>
+      </c>
+      <c r="D113" s="29">
+        <v>70</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F113" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G113" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="H113" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="I113" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="J113" s="14">
-        <v>0.15</v>
+        <v>24</v>
+      </c>
+      <c r="G113" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="H113" s="29">
+        <v>70</v>
+      </c>
+      <c r="I113" s="29">
+        <v>70</v>
+      </c>
+      <c r="J113" s="29">
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
@@ -5246,13 +5268,13 @@
         <v>274</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="C114" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D114" s="14">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E114" s="27" t="s">
         <v>93</v>
@@ -5261,16 +5283,16 @@
         <v>66</v>
       </c>
       <c r="G114" s="27" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="H114" s="14">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="I114" s="14">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="J114" s="14">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
@@ -5278,13 +5300,13 @@
         <v>274</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D115" s="14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E115" s="27" t="s">
         <v>93</v>
@@ -5293,16 +5315,16 @@
         <v>66</v>
       </c>
       <c r="G115" s="27" t="s">
-        <v>289</v>
+        <v>243</v>
       </c>
       <c r="H115" s="14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I115" s="14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J115" s="14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
@@ -5310,13 +5332,13 @@
         <v>274</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D116" s="14">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E116" s="27" t="s">
         <v>93</v>
@@ -5325,16 +5347,16 @@
         <v>66</v>
       </c>
       <c r="G116" s="27" t="s">
-        <v>247</v>
+        <v>288</v>
       </c>
       <c r="H116" s="14">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I116" s="14">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J116" s="14">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
@@ -5342,31 +5364,31 @@
         <v>274</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D117" s="14">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="E117" s="27" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="F117" s="27" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G117" s="27" t="s">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="H117" s="14">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="I117" s="14">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
       <c r="J117" s="14">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
@@ -5374,22 +5396,22 @@
         <v>274</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D118" s="14">
         <v>0.1</v>
       </c>
       <c r="E118" s="27" t="s">
-        <v>250</v>
+        <v>93</v>
       </c>
       <c r="F118" s="27" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G118" s="27" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="H118" s="14">
         <v>0.1</v>
@@ -5406,13 +5428,13 @@
         <v>274</v>
       </c>
       <c r="B119" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C119" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D119" s="14">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E119" s="27" t="s">
         <v>93</v>
@@ -5421,112 +5443,112 @@
         <v>66</v>
       </c>
       <c r="G119" s="27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H119" s="14">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="I119" s="14">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="J119" s="14">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="27" t="s">
         <v>274</v>
       </c>
       <c r="B120" s="27" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D120" s="29">
-        <v>20</v>
+        <v>248</v>
+      </c>
+      <c r="D120" s="14">
+        <v>0.8</v>
       </c>
       <c r="E120" s="27" t="s">
-        <v>49</v>
+        <v>250</v>
       </c>
       <c r="F120" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G120" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="H120" s="29">
-        <v>20</v>
-      </c>
-      <c r="I120" s="29">
-        <v>20</v>
-      </c>
-      <c r="J120" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="G120" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="H120" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="I120" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="J120" s="14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
         <v>274</v>
       </c>
       <c r="B121" s="27" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D121" s="29">
-        <v>20</v>
+        <v>249</v>
+      </c>
+      <c r="D121" s="14">
+        <v>0.1</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>49</v>
+        <v>250</v>
       </c>
       <c r="F121" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G121" s="28" t="s">
-        <v>301</v>
-      </c>
-      <c r="H121" s="29">
-        <v>20</v>
-      </c>
-      <c r="I121" s="29">
-        <v>20</v>
-      </c>
-      <c r="J121" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G121" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="H121" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="I121" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="J121" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="s">
         <v>274</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D122" s="29">
-        <v>13</v>
+        <v>241</v>
+      </c>
+      <c r="D122" s="14">
+        <v>0.3</v>
       </c>
       <c r="E122" s="27" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F122" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G122" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="H122" s="29">
-        <v>13</v>
-      </c>
-      <c r="I122" s="29">
-        <v>13</v>
-      </c>
-      <c r="J122" s="29">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="G122" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="H122" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="I122" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="J122" s="14">
+        <v>0.3</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -5534,237 +5556,237 @@
         <v>274</v>
       </c>
       <c r="B123" s="27" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>107</v>
+        <v>256</v>
       </c>
       <c r="D123" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E123" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F123" s="27" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G123" s="28" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="H123" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I123" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J123" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
         <v>274</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C124" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D124" s="29">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E124" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F124" s="27" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G124" s="28" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H124" s="29">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="I124" s="29">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J124" s="29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
         <v>274</v>
       </c>
       <c r="B125" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D125" s="29">
+        <v>13</v>
+      </c>
+      <c r="E125" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F125" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G125" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="H125" s="29">
+        <v>13</v>
+      </c>
+      <c r="I125" s="29">
+        <v>13</v>
+      </c>
+      <c r="J125" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A126" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B126" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D126" s="29">
+        <v>0</v>
+      </c>
+      <c r="E126" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F126" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G126" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="H126" s="29">
+        <v>0</v>
+      </c>
+      <c r="I126" s="29">
+        <v>0</v>
+      </c>
+      <c r="J126" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A127" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B127" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D127" s="29">
+        <v>100</v>
+      </c>
+      <c r="E127" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F127" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G127" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="H127" s="29">
+        <v>100</v>
+      </c>
+      <c r="I127" s="29">
+        <v>100</v>
+      </c>
+      <c r="J127" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A128" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B128" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="C125" s="14" t="s">
+      <c r="C128" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="D125" s="14">
+      <c r="D128" s="14">
         <v>0.15</v>
       </c>
-      <c r="E125" s="27" t="s">
+      <c r="E128" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F125" s="27" t="s">
+      <c r="F128" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G125" s="27" t="s">
+      <c r="G128" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="H125" s="14">
+      <c r="H128" s="14">
         <v>0.15</v>
       </c>
-      <c r="I125" s="14">
+      <c r="I128" s="14">
         <v>0.15</v>
       </c>
-      <c r="J125" s="14">
+      <c r="J128" s="14">
         <v>0.15</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A126" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="D126" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E126" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F126" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G126" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="H126" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I126" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J126" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="B127" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="D127" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="E127" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F127" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G127" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="H127" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="I127" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="J127" s="6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A128" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D128" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E128" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F128" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G128" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="H128" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I128" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J128" s="6">
-        <v>0.5</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="C129" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B129" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="D129" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>321</v>
+        <v>93</v>
       </c>
       <c r="F129" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G129" s="11" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="H129" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I129" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J129" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B130" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C130" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B130" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="D130" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>93</v>
@@ -5773,91 +5795,91 @@
         <v>24</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H130" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I130" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J130" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D131" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="F131" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G131" s="11" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="H131" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="I131" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="J131" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>314</v>
+        <v>107</v>
       </c>
       <c r="D132" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>93</v>
+        <v>320</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G132" s="11" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="H132" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I132" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J132" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C133" s="6" t="s">
         <v>313</v>
-      </c>
-      <c r="B133" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>314</v>
       </c>
       <c r="D133" s="6">
         <v>0.1</v>
@@ -5869,7 +5891,7 @@
         <v>24</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="H133" s="6">
         <v>0.1</v>
@@ -5883,112 +5905,112 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="C134" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B134" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>334</v>
-      </c>
       <c r="D134" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F134" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="H134" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I134" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="J134" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="C135" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B135" s="11" t="s">
-        <v>335</v>
-      </c>
-      <c r="C135" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="D135" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F135" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="H135" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="I135" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="J135" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B136" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C136" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B136" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="D136" s="6">
-        <v>7</v>
+        <v>0.1</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F136" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G136" s="11" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H136" s="6">
-        <v>13</v>
+        <v>0.1</v>
       </c>
       <c r="I136" s="6">
-        <v>13</v>
+        <v>0.1</v>
       </c>
       <c r="J136" s="6">
-        <v>13</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>107</v>
+        <v>333</v>
       </c>
       <c r="D137" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>49</v>
@@ -5997,158 +6019,158 @@
         <v>24</v>
       </c>
       <c r="G137" s="11" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H137" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I137" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J137" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>314</v>
+        <v>107</v>
       </c>
       <c r="D138" s="6">
-        <v>0.05</v>
+        <v>20</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F138" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="H138" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="I138" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="J138" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>314</v>
+        <v>107</v>
       </c>
       <c r="D139" s="6">
-        <v>0.05</v>
+        <v>7</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F139" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H139" s="6">
-        <v>0.15</v>
+        <v>13</v>
       </c>
       <c r="I139" s="6">
-        <v>0.15</v>
+        <v>13</v>
       </c>
       <c r="J139" s="6">
-        <v>0.15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>314</v>
+        <v>107</v>
       </c>
       <c r="D140" s="6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E140" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F140" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="H140" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I140" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J140" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B141" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B141" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="D141" s="6">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E141" s="11" t="s">
-        <v>350</v>
+        <v>93</v>
       </c>
       <c r="F141" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="H141" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="I141" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J141" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B142" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="C142" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B142" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="D142" s="6">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E142" s="11" t="s">
         <v>93</v>
@@ -6157,30 +6179,30 @@
         <v>24</v>
       </c>
       <c r="G142" s="11" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="H142" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I142" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J142" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="C143" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="B143" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>314</v>
-      </c>
       <c r="D143" s="6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E143" s="11" t="s">
         <v>93</v>
@@ -6189,7 +6211,7 @@
         <v>24</v>
       </c>
       <c r="G143" s="11" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H143" s="6">
         <v>0.1</v>
@@ -6198,6 +6220,102 @@
         <v>0.1</v>
       </c>
       <c r="J143" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A144" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D144" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E144" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="F144" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G144" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="H144" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I144" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J144" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A145" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D145" s="6">
+        <v>1</v>
+      </c>
+      <c r="E145" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F145" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G145" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="H145" s="6">
+        <v>0</v>
+      </c>
+      <c r="I145" s="6">
+        <v>0</v>
+      </c>
+      <c r="J145" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A146" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="B146" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D146" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E146" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F146" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G146" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="H146" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I146" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J146" s="6">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
relocation: new model (dao)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1642,8 +1642,8 @@
   <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4986,7 +4986,7 @@
         <v>249</v>
       </c>
       <c r="D105" s="35">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="E105" s="32" t="s">
         <v>250</v>

</xml_diff>

<commit_message>
relocations: without parameters for old models (yao, ya)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="351">
   <si>
     <t>parameter</t>
   </si>
@@ -751,15 +751,9 @@
     <t>proportion of data points used in the loess regressions of relocation by age; groups: district, year, origin</t>
   </si>
   <si>
-    <t>proportion of data points used in the loess regressions of immigration* by age; groups: year, origin</t>
-  </si>
-  <si>
     <t>proportion of data points used in the loess regressions of relocation by age; groups: year, origin</t>
   </si>
   <si>
-    <t>proportion of data points used in the loess regressions of immigration* by age; groups: year</t>
-  </si>
-  <si>
     <t>proportion of data points used in the loess regressions of relocation by age; groups: year</t>
   </si>
   <si>
@@ -805,21 +799,6 @@
     <t>rei_rel_span_dyao</t>
   </si>
   <si>
-    <t>rei_ims_span_yao</t>
-  </si>
-  <si>
-    <t>rei_rel_span_yao</t>
-  </si>
-  <si>
-    <t>rei_ims_span_ya</t>
-  </si>
-  <si>
-    <t>rei_rel_span_ya</t>
-  </si>
-  <si>
-    <t>rei_ims_thres_d</t>
-  </si>
-  <si>
     <t>rei_prop_span</t>
   </si>
   <si>
@@ -892,18 +871,12 @@
     <t>when immigration* is above this threshold: proportion with district (and year, age, origin), below without district (but with year, age, origin). Value must be higher than ree_thres_o.</t>
   </si>
   <si>
-    <t>rei_ims_thres_o</t>
-  </si>
-  <si>
     <t>ree_ems_thres_d</t>
   </si>
   <si>
     <t>ree_ems_thres_o</t>
   </si>
   <si>
-    <t>when immigration* is above this threshold: proportion with district (and year, age, origin), below without district (but with year, age, origin). Value must be higher than rei_ims_thres_o.</t>
-  </si>
-  <si>
     <t>ree_ems_span_yao</t>
   </si>
   <si>
@@ -1094,9 +1067,6 @@
   </si>
   <si>
     <t>rei_ims_thres_y</t>
-  </si>
-  <si>
-    <t>when immigration* is above this threshold: proportion with origin (and year, age), below without origin (but with year, age). Value must be lower than rei_ims_thres_d.</t>
   </si>
   <si>
     <t>when immigration* is above this threshold: proportion with year (and district, age, origin), below without year (but with district, age, origin).</t>
@@ -1218,7 +1188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1316,10 +1286,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1639,11 +1605,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J146"/>
+  <dimension ref="A1:J140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2528,7 +2494,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>107</v>
@@ -2560,7 +2526,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>107</v>
@@ -2592,7 +2558,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>107</v>
@@ -2624,7 +2590,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>107</v>
@@ -2656,7 +2622,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>107</v>
@@ -2671,7 +2637,7 @@
         <v>24</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="H32" s="10">
         <v>2011</v>
@@ -2688,7 +2654,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>107</v>
@@ -2703,7 +2669,7 @@
         <v>24</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="H33" s="10">
         <v>2020</v>
@@ -4628,7 +4594,7 @@
         <v>236</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>235</v>
@@ -4660,7 +4626,7 @@
         <v>236</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>241</v>
@@ -4692,7 +4658,7 @@
         <v>236</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>241</v>
@@ -4719,68 +4685,68 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="32" t="s">
+    <row r="97" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="B97" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="C97" s="35" t="s">
+      <c r="B97" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="D97" s="35">
-        <v>0.15</v>
-      </c>
-      <c r="E97" s="32" t="s">
+      <c r="D97" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="E97" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F97" s="32" t="s">
+      <c r="F97" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G97" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="H97" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="I97" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="J97" s="35">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="32" t="s">
+      <c r="G97" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="H97" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="I97" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="J97" s="6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="B98" s="32" t="s">
-        <v>355</v>
-      </c>
-      <c r="C98" s="35" t="s">
+      <c r="B98" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="D98" s="35">
-        <v>0.15</v>
-      </c>
-      <c r="E98" s="32" t="s">
+      <c r="D98" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="E98" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F98" s="32" t="s">
+      <c r="F98" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G98" s="32" t="s">
-        <v>357</v>
-      </c>
-      <c r="H98" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="I98" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="J98" s="35">
-        <v>0.1</v>
+      <c r="G98" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="H98" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="I98" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="J98" s="6">
+        <v>0.12</v>
       </c>
     </row>
     <row r="99" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4788,31 +4754,31 @@
         <v>236</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>262</v>
+        <v>349</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D99" s="6">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>93</v>
+        <v>248</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>244</v>
+        <v>350</v>
       </c>
       <c r="H99" s="6">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="I99" s="6">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="J99" s="6">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4820,13 +4786,13 @@
         <v>236</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D100" s="6">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>93</v>
@@ -4835,176 +4801,176 @@
         <v>66</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="H100" s="6">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="I100" s="6">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="J100" s="6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D101" s="6">
-        <v>0.1</v>
+        <v>254</v>
+      </c>
+      <c r="D101" s="12">
+        <v>20</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G101" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="H101" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I101" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J101" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G101" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="H101" s="12">
+        <v>20</v>
+      </c>
+      <c r="I101" s="12">
+        <v>20</v>
+      </c>
+      <c r="J101" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D102" s="6">
-        <v>0.1</v>
+        <v>107</v>
+      </c>
+      <c r="D102" s="12">
+        <v>20</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G102" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="H102" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I102" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J102" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="G102" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="H102" s="12">
+        <v>20</v>
+      </c>
+      <c r="I102" s="12">
+        <v>20</v>
+      </c>
+      <c r="J102" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="D103" s="6">
-        <v>0.8</v>
+        <v>107</v>
+      </c>
+      <c r="D103" s="12">
+        <v>13</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="F103" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G103" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="H103" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="I103" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="J103" s="6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G103" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="H103" s="12">
+        <v>13</v>
+      </c>
+      <c r="I103" s="12">
+        <v>13</v>
+      </c>
+      <c r="J103" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>291</v>
+        <v>264</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="D104" s="6">
-        <v>0.1</v>
+        <v>107</v>
+      </c>
+      <c r="D104" s="12">
+        <v>0</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G104" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="H104" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I104" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J104" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G104" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="H104" s="12">
+        <v>0</v>
+      </c>
+      <c r="I104" s="12">
+        <v>0</v>
+      </c>
+      <c r="J104" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="B105" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="C105" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="D105" s="35">
-        <v>0.4</v>
-      </c>
-      <c r="E105" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="F105" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="G105" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="H105" s="35">
-        <v>0.8</v>
-      </c>
-      <c r="I105" s="35">
-        <v>0.8</v>
-      </c>
-      <c r="J105" s="35">
-        <v>0.8</v>
+      <c r="B105" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D105" s="12">
+        <v>100</v>
+      </c>
+      <c r="E105" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G105" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H105" s="12">
+        <v>100</v>
+      </c>
+      <c r="I105" s="12">
+        <v>100</v>
+      </c>
+      <c r="J105" s="12">
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5012,13 +4978,13 @@
         <v>236</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D106" s="6">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E106" s="11" t="s">
         <v>93</v>
@@ -5027,318 +4993,318 @@
         <v>66</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="H106" s="6">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="I106" s="6">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="J106" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A107" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B107" s="11" t="s">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D107" s="29">
+        <v>70</v>
+      </c>
+      <c r="E107" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F107" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G107" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="H107" s="29">
+        <v>70</v>
+      </c>
+      <c r="I107" s="29">
+        <v>70</v>
+      </c>
+      <c r="J107" s="29">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B108" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D108" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E108" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F108" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G108" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="H108" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I108" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="J108" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B109" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="C107" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D107" s="12">
-        <v>20</v>
-      </c>
-      <c r="E107" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F107" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G107" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="H107" s="12">
-        <v>20</v>
-      </c>
-      <c r="I107" s="12">
-        <v>20</v>
-      </c>
-      <c r="J107" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A108" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B108" s="11" t="s">
+      <c r="C109" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D109" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E109" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F109" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G109" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="H109" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="I109" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="J109" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B110" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D110" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="E110" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F110" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G110" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="H110" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="I110" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="J110" s="14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B111" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="C108" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D108" s="12">
-        <v>20</v>
-      </c>
-      <c r="E108" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F108" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G108" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H108" s="12">
-        <v>20</v>
-      </c>
-      <c r="I108" s="12">
-        <v>20</v>
-      </c>
-      <c r="J108" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A109" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C109" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D109" s="12">
-        <v>13</v>
-      </c>
-      <c r="E109" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F109" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G109" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="H109" s="12">
-        <v>13</v>
-      </c>
-      <c r="I109" s="12">
-        <v>13</v>
-      </c>
-      <c r="J109" s="12">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A110" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D110" s="12">
-        <v>0</v>
-      </c>
-      <c r="E110" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F110" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G110" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="H110" s="12">
-        <v>0</v>
-      </c>
-      <c r="I110" s="12">
-        <v>0</v>
-      </c>
-      <c r="J110" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A111" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D111" s="12">
-        <v>100</v>
-      </c>
-      <c r="E111" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F111" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G111" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="H111" s="12">
-        <v>100</v>
-      </c>
-      <c r="I111" s="12">
-        <v>100</v>
-      </c>
-      <c r="J111" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C112" s="6" t="s">
+      <c r="C111" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D111" s="14">
         <v>0.15</v>
       </c>
-      <c r="E112" s="11" t="s">
+      <c r="E111" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F112" s="11" t="s">
+      <c r="F111" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G112" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="H112" s="6">
+      <c r="G111" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="H111" s="14">
         <v>0.15</v>
       </c>
-      <c r="I112" s="6">
+      <c r="I111" s="14">
         <v>0.15</v>
       </c>
-      <c r="J112" s="6">
+      <c r="J111" s="14">
         <v>0.15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B112" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D112" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E112" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F112" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G112" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="H112" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="I112" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="J112" s="14">
+        <v>0.1</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>285</v>
+        <v>267</v>
+      </c>
+      <c r="B113" s="27" t="s">
+        <v>270</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="D113" s="29">
-        <v>70</v>
+        <v>241</v>
+      </c>
+      <c r="D113" s="14">
+        <v>0.1</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F113" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G113" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="H113" s="29">
-        <v>70</v>
-      </c>
-      <c r="I113" s="29">
-        <v>70</v>
-      </c>
-      <c r="J113" s="29">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="G113" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="H113" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="I113" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="J113" s="14">
+        <v>0.1</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="27" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D114" s="14">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>93</v>
+        <v>248</v>
       </c>
       <c r="F114" s="27" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G114" s="27" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H114" s="14">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="I114" s="14">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="J114" s="14">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D115" s="14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E115" s="27" t="s">
-        <v>93</v>
+        <v>248</v>
       </c>
       <c r="F115" s="27" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G115" s="27" t="s">
-        <v>243</v>
+        <v>289</v>
       </c>
       <c r="H115" s="14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I115" s="14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="J115" s="14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="27" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D116" s="14">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E116" s="27" t="s">
         <v>93</v>
@@ -5347,190 +5313,190 @@
         <v>66</v>
       </c>
       <c r="G116" s="27" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="H116" s="14">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="I116" s="14">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="J116" s="14">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B117" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D117" s="29">
+        <v>20</v>
+      </c>
+      <c r="E117" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F117" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G117" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="H117" s="29">
+        <v>20</v>
+      </c>
+      <c r="I117" s="29">
+        <v>20</v>
+      </c>
+      <c r="J117" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A118" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B118" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D118" s="29">
+        <v>20</v>
+      </c>
+      <c r="E118" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F118" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G118" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="H118" s="29">
+        <v>20</v>
+      </c>
+      <c r="I118" s="29">
+        <v>20</v>
+      </c>
+      <c r="J118" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A119" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B119" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="B117" s="27" t="s">
+      <c r="C119" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D119" s="29">
+        <v>13</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F119" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G119" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="H119" s="29">
+        <v>13</v>
+      </c>
+      <c r="I119" s="29">
+        <v>13</v>
+      </c>
+      <c r="J119" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A120" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B120" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D120" s="29">
+        <v>0</v>
+      </c>
+      <c r="E120" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F120" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G120" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="H120" s="29">
+        <v>0</v>
+      </c>
+      <c r="I120" s="29">
+        <v>0</v>
+      </c>
+      <c r="J120" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A121" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B121" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="C117" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D117" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="E117" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F117" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G117" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="H117" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="I117" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="J117" s="14">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A118" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B118" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D118" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="E118" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F118" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G118" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="H118" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="I118" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="J118" s="14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A119" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B119" s="27" t="s">
-        <v>277</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D119" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="E119" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F119" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G119" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="H119" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="I119" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="J119" s="14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A120" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B120" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="D120" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="E120" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="F120" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G120" s="27" t="s">
-        <v>290</v>
-      </c>
-      <c r="H120" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="I120" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="J120" s="14">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B121" s="27" t="s">
-        <v>293</v>
-      </c>
       <c r="C121" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="D121" s="14">
-        <v>0.1</v>
+        <v>107</v>
+      </c>
+      <c r="D121" s="29">
+        <v>100</v>
       </c>
       <c r="E121" s="27" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="F121" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G121" s="27" t="s">
-        <v>298</v>
-      </c>
-      <c r="H121" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="I121" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="J121" s="14">
-        <v>0.1</v>
+        <v>61</v>
+      </c>
+      <c r="G121" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="H121" s="29">
+        <v>100</v>
+      </c>
+      <c r="I121" s="29">
+        <v>100</v>
+      </c>
+      <c r="J121" s="29">
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C122" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D122" s="14">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E122" s="27" t="s">
         <v>93</v>
@@ -5539,219 +5505,219 @@
         <v>66</v>
       </c>
       <c r="G122" s="27" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="H122" s="14">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="I122" s="14">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="J122" s="14">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A123" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B123" s="27" t="s">
-        <v>279</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="D123" s="29">
-        <v>20</v>
-      </c>
-      <c r="E123" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F123" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G123" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="H123" s="29">
-        <v>20</v>
-      </c>
-      <c r="I123" s="29">
-        <v>20</v>
-      </c>
-      <c r="J123" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A124" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B124" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D124" s="29">
-        <v>20</v>
-      </c>
-      <c r="E124" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F124" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G124" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="H124" s="29">
-        <v>20</v>
-      </c>
-      <c r="I124" s="29">
-        <v>20</v>
-      </c>
-      <c r="J124" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A125" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B125" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D125" s="29">
-        <v>13</v>
-      </c>
-      <c r="E125" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F125" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G125" s="28" t="s">
-        <v>301</v>
-      </c>
-      <c r="H125" s="29">
-        <v>13</v>
-      </c>
-      <c r="I125" s="29">
-        <v>13</v>
-      </c>
-      <c r="J125" s="29">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A126" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B126" s="27" t="s">
-        <v>282</v>
-      </c>
-      <c r="C126" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D126" s="29">
-        <v>0</v>
-      </c>
-      <c r="E126" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F126" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="G126" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="H126" s="29">
-        <v>0</v>
-      </c>
-      <c r="I126" s="29">
-        <v>0</v>
-      </c>
-      <c r="J126" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A127" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B127" s="27" t="s">
-        <v>283</v>
-      </c>
-      <c r="C127" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D127" s="29">
-        <v>100</v>
-      </c>
-      <c r="E127" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F127" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="G127" s="28" t="s">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="H127" s="29">
-        <v>100</v>
-      </c>
-      <c r="I127" s="29">
-        <v>100</v>
-      </c>
-      <c r="J127" s="29">
-        <v>100</v>
+      <c r="B123" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D123" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="H123" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I123" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J123" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D124" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E124" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F124" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G124" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="H124" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="I124" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="J124" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A125" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D125" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="H125" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I125" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J125" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B126" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D126" s="6">
+        <v>0</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="F126" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G126" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="H126" s="6">
+        <v>0</v>
+      </c>
+      <c r="I126" s="6">
+        <v>0</v>
+      </c>
+      <c r="J126" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A127" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D127" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E127" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="H127" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I127" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J127" s="6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A128" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B128" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="C128" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D128" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="E128" s="27" t="s">
+      <c r="A128" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D128" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E128" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F128" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G128" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="H128" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="I128" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="J128" s="14">
-        <v>0.15</v>
+      <c r="F128" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="H128" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I128" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J128" s="6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D129" s="6">
         <v>0.1</v>
@@ -5763,30 +5729,30 @@
         <v>24</v>
       </c>
       <c r="G129" s="11" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="H129" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I129" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J129" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D130" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E130" s="11" t="s">
         <v>93</v>
@@ -5795,158 +5761,158 @@
         <v>24</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="H130" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I130" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J130" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="D131" s="6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F131" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G131" s="11" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="H131" s="6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="I131" s="6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="J131" s="6">
-        <v>0.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="C132" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D132" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>320</v>
+        <v>49</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G132" s="11" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="H132" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I132" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J132" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>313</v>
+        <v>107</v>
       </c>
       <c r="D133" s="6">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F133" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="H133" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="I133" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="J133" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>313</v>
+        <v>107</v>
       </c>
       <c r="D134" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F134" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="H134" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I134" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J134" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D135" s="6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E135" s="11" t="s">
         <v>93</v>
@@ -5955,30 +5921,30 @@
         <v>24</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="H135" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I135" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J135" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D136" s="6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>93</v>
@@ -5987,33 +5953,33 @@
         <v>24</v>
       </c>
       <c r="G136" s="11" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="H136" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I136" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J136" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>333</v>
+        <v>304</v>
       </c>
       <c r="D137" s="6">
-        <v>20</v>
+        <v>0.05</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F137" s="11" t="s">
         <v>24</v>
@@ -6022,300 +5988,108 @@
         <v>337</v>
       </c>
       <c r="H137" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I137" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="J137" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D138" s="6">
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>49</v>
+        <v>340</v>
       </c>
       <c r="F138" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="H138" s="6">
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="I138" s="6">
-        <v>20</v>
+        <v>0.5</v>
       </c>
       <c r="J138" s="6">
-        <v>20</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D139" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F139" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H139" s="6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I139" s="6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J139" s="6">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>107</v>
+        <v>304</v>
       </c>
       <c r="D140" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E140" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F140" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="H140" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I140" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J140" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B141" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D141" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="E141" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F141" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G141" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H141" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I141" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J141" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A142" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B142" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D142" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="E142" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F142" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G142" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="H142" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="I142" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="J142" s="6">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A143" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B143" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D143" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="E143" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F143" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G143" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="H143" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I143" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J143" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A144" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B144" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D144" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E144" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="F144" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G144" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="H144" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I144" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J144" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A145" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B145" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="C145" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D145" s="6">
-        <v>1</v>
-      </c>
-      <c r="E145" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F145" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G145" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="H145" s="6">
-        <v>0</v>
-      </c>
-      <c r="I145" s="6">
-        <v>0</v>
-      </c>
-      <c r="J145" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A146" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="B146" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="C146" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D146" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E146" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F146" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G146" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="H146" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I146" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J146" s="6">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
relocations: new model (dao instead of yao/ya)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="343">
   <si>
     <t>parameter</t>
   </si>
@@ -751,12 +751,6 @@
     <t>proportion of data points used in the loess regressions of relocation by age; groups: district, year, origin</t>
   </si>
   <si>
-    <t>proportion of data points used in the loess regressions of relocation by age; groups: year, origin</t>
-  </si>
-  <si>
-    <t>proportion of data points used in the loess regressions of relocation by age; groups: year</t>
-  </si>
-  <si>
     <t>similar to umz.anz.rate.heimat</t>
   </si>
   <si>
@@ -826,12 +820,6 @@
     <t>ree_rel_span_dyao</t>
   </si>
   <si>
-    <t>ree_rel_span_yao</t>
-  </si>
-  <si>
-    <t>ree_rel_span_ya</t>
-  </si>
-  <si>
     <t>ree_prop_span</t>
   </si>
   <si>
@@ -862,33 +850,9 @@
     <t>proportion of data points used in the loess regressions of emigration* by age; groups: district, year, origin</t>
   </si>
   <si>
-    <t>proportion of data points used in the loess regressions of emigration* by age; groups: year, origin</t>
-  </si>
-  <si>
-    <t>proportion of data points used in the loess regressions of emigration* by age; groups: year</t>
-  </si>
-  <si>
-    <t>when immigration* is above this threshold: proportion with district (and year, age, origin), below without district (but with year, age, origin). Value must be higher than ree_thres_o.</t>
-  </si>
-  <si>
-    <t>ree_ems_thres_d</t>
-  </si>
-  <si>
-    <t>ree_ems_thres_o</t>
-  </si>
-  <si>
-    <t>ree_ems_span_yao</t>
-  </si>
-  <si>
     <t>ree_ems_span_dyao</t>
   </si>
   <si>
-    <t>ree_ems_span_ya</t>
-  </si>
-  <si>
-    <t>when emigration* is above this threshold: proportion with oritin (and year, age), below without origin (but with year, age). Value must be lower than ree_thres_d.</t>
-  </si>
-  <si>
     <t>relocation proportion on emigration*: trend in addition to the mean; 20% means, 20% of the difference between trend and mean is added to the mean.</t>
   </si>
   <si>
@@ -1070,6 +1034,18 @@
   </si>
   <si>
     <t>when immigration* is above this threshold: proportion with year (and district, age, origin), below without year (but with district, age, origin).</t>
+  </si>
+  <si>
+    <t>ree_ems_span_dao</t>
+  </si>
+  <si>
+    <t>ree_rel_span_dao</t>
+  </si>
+  <si>
+    <t>proportion of data points used in the loess regressions of emigration* by age; groups: district, origin</t>
+  </si>
+  <si>
+    <t>ree_ems_thres_y</t>
   </si>
 </sst>
 </file>
@@ -1605,11 +1581,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2494,7 +2470,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>107</v>
@@ -2526,7 +2502,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>107</v>
@@ -2558,7 +2534,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>107</v>
@@ -2590,7 +2566,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>107</v>
@@ -2622,7 +2598,7 @@
         <v>21</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>107</v>
@@ -2637,7 +2613,7 @@
         <v>24</v>
       </c>
       <c r="G32" s="31" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="H32" s="10">
         <v>2011</v>
@@ -2654,7 +2630,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>107</v>
@@ -2669,7 +2645,7 @@
         <v>24</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="H33" s="10">
         <v>2020</v>
@@ -4594,7 +4570,7 @@
         <v>236</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>235</v>
@@ -4626,7 +4602,7 @@
         <v>236</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>241</v>
@@ -4658,7 +4634,7 @@
         <v>236</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>241</v>
@@ -4690,7 +4666,7 @@
         <v>236</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>241</v>
@@ -4705,7 +4681,7 @@
         <v>66</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="H97" s="6">
         <v>0.12</v>
@@ -4722,7 +4698,7 @@
         <v>236</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>241</v>
@@ -4737,7 +4713,7 @@
         <v>66</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="H98" s="6">
         <v>0.12</v>
@@ -4754,22 +4730,22 @@
         <v>236</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D99" s="6">
         <v>0.4</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F99" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="H99" s="6">
         <v>0.4</v>
@@ -4786,7 +4762,7 @@
         <v>236</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>241</v>
@@ -4801,7 +4777,7 @@
         <v>66</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H100" s="6">
         <v>0.3</v>
@@ -4818,10 +4794,10 @@
         <v>236</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D101" s="12">
         <v>20</v>
@@ -4833,7 +4809,7 @@
         <v>24</v>
       </c>
       <c r="G101" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H101" s="12">
         <v>20</v>
@@ -4850,7 +4826,7 @@
         <v>236</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>107</v>
@@ -4865,7 +4841,7 @@
         <v>24</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H102" s="12">
         <v>20</v>
@@ -4882,7 +4858,7 @@
         <v>236</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>107</v>
@@ -4897,7 +4873,7 @@
         <v>24</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H103" s="12">
         <v>13</v>
@@ -4914,7 +4890,7 @@
         <v>236</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>107</v>
@@ -4929,7 +4905,7 @@
         <v>61</v>
       </c>
       <c r="G104" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H104" s="12">
         <v>0</v>
@@ -4946,7 +4922,7 @@
         <v>236</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>107</v>
@@ -4961,7 +4937,7 @@
         <v>61</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H105" s="12">
         <v>100</v>
@@ -4978,7 +4954,7 @@
         <v>236</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>241</v>
@@ -4993,7 +4969,7 @@
         <v>66</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H106" s="6">
         <v>0.15</v>
@@ -5007,10 +4983,10 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C107" s="14" t="s">
         <v>235</v>
@@ -5025,7 +5001,7 @@
         <v>24</v>
       </c>
       <c r="G107" s="28" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="H107" s="29">
         <v>70</v>
@@ -5039,10 +5015,10 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B108" s="27" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C108" s="14" t="s">
         <v>241</v>
@@ -5057,7 +5033,7 @@
         <v>66</v>
       </c>
       <c r="G108" s="27" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H108" s="14">
         <v>0.2</v>
@@ -5071,10 +5047,10 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B109" s="27" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>241</v>
@@ -5103,16 +5079,16 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B110" s="27" t="s">
-        <v>286</v>
+        <v>339</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D110" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="E110" s="27" t="s">
         <v>93</v>
@@ -5121,30 +5097,30 @@
         <v>66</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>281</v>
+        <v>341</v>
       </c>
       <c r="H110" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="I110" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="J110" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B111" s="27" t="s">
-        <v>269</v>
+        <v>340</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D111" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="E111" s="27" t="s">
         <v>93</v>
@@ -5153,62 +5129,62 @@
         <v>66</v>
       </c>
       <c r="G111" s="27" t="s">
-        <v>244</v>
+        <v>336</v>
       </c>
       <c r="H111" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="I111" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="J111" s="14">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B112" s="27" t="s">
-        <v>288</v>
+        <v>342</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D112" s="14">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>93</v>
+        <v>246</v>
       </c>
       <c r="F112" s="27" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G112" s="27" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="H112" s="14">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="I112" s="14">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="J112" s="14">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="B113" s="27" t="s">
         <v>267</v>
-      </c>
-      <c r="B113" s="27" t="s">
-        <v>270</v>
       </c>
       <c r="C113" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D113" s="14">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E113" s="27" t="s">
         <v>93</v>
@@ -5217,350 +5193,350 @@
         <v>66</v>
       </c>
       <c r="G113" s="27" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H113" s="14">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I113" s="14">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J113" s="14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A114" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="D114" s="14">
-        <v>0.8</v>
+        <v>252</v>
+      </c>
+      <c r="D114" s="29">
+        <v>20</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>248</v>
+        <v>49</v>
       </c>
       <c r="F114" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G114" s="27" t="s">
-        <v>283</v>
-      </c>
-      <c r="H114" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="I114" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="J114" s="14">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G114" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="H114" s="29">
+        <v>20</v>
+      </c>
+      <c r="I114" s="29">
+        <v>20</v>
+      </c>
+      <c r="J114" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="D115" s="14">
-        <v>0.1</v>
+        <v>107</v>
+      </c>
+      <c r="D115" s="29">
+        <v>20</v>
       </c>
       <c r="E115" s="27" t="s">
-        <v>248</v>
+        <v>49</v>
       </c>
       <c r="F115" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G115" s="27" t="s">
-        <v>289</v>
-      </c>
-      <c r="H115" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="I115" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="J115" s="14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G115" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="H115" s="29">
+        <v>20</v>
+      </c>
+      <c r="I115" s="29">
+        <v>20</v>
+      </c>
+      <c r="J115" s="29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D116" s="14">
-        <v>0.3</v>
+        <v>107</v>
+      </c>
+      <c r="D116" s="29">
+        <v>13</v>
       </c>
       <c r="E116" s="27" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F116" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G116" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="H116" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="I116" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="J116" s="14">
-        <v>0.3</v>
+        <v>24</v>
+      </c>
+      <c r="G116" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="H116" s="29">
+        <v>13</v>
+      </c>
+      <c r="I116" s="29">
+        <v>13</v>
+      </c>
+      <c r="J116" s="29">
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>254</v>
+        <v>107</v>
       </c>
       <c r="D117" s="29">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E117" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F117" s="27" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G117" s="28" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="H117" s="29">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I117" s="29">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J117" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D118" s="29">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E118" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F118" s="27" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G118" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="H118" s="29">
+        <v>100</v>
+      </c>
+      <c r="I118" s="29">
+        <v>100</v>
+      </c>
+      <c r="J118" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A119" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="B119" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D119" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F119" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G119" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="H119" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="I119" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="J119" s="14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="H118" s="29">
-        <v>20</v>
-      </c>
-      <c r="I118" s="29">
-        <v>20</v>
-      </c>
-      <c r="J118" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A119" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B119" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D119" s="29">
-        <v>13</v>
-      </c>
-      <c r="E119" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F119" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G119" s="28" t="s">
+      <c r="B120" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C120" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="H119" s="29">
-        <v>13</v>
-      </c>
-      <c r="I119" s="29">
-        <v>13</v>
-      </c>
-      <c r="J119" s="29">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A120" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B120" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D120" s="29">
-        <v>0</v>
-      </c>
-      <c r="E120" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F120" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="G120" s="28" t="s">
+      <c r="D120" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G120" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="H120" s="29">
-        <v>0</v>
-      </c>
-      <c r="I120" s="29">
-        <v>0</v>
-      </c>
-      <c r="J120" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A121" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B121" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="C121" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D121" s="29">
-        <v>100</v>
-      </c>
-      <c r="E121" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F121" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="G121" s="28" t="s">
-        <v>294</v>
-      </c>
-      <c r="H121" s="29">
-        <v>100</v>
-      </c>
-      <c r="I121" s="29">
-        <v>100</v>
-      </c>
-      <c r="J121" s="29">
-        <v>100</v>
+      <c r="H120" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="I120" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J120" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D121" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="H121" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="I121" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="J121" s="6">
+        <v>0.15</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A122" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B122" s="27" t="s">
-        <v>277</v>
-      </c>
-      <c r="C122" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D122" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="E122" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F122" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G122" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="H122" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="I122" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="J122" s="14">
-        <v>0.15</v>
+      <c r="A122" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D122" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F122" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="H122" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I122" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J122" s="6">
+        <v>0.5</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>304</v>
+        <v>107</v>
       </c>
       <c r="D123" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>93</v>
+        <v>299</v>
       </c>
       <c r="F123" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="H123" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I123" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J123" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B124" s="11" t="s">
         <v>303</v>
       </c>
-      <c r="B124" s="11" t="s">
-        <v>307</v>
-      </c>
       <c r="C124" s="6" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D124" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E124" s="11" t="s">
         <v>93</v>
@@ -5569,91 +5545,91 @@
         <v>24</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="H124" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I124" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J124" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="D125" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="F125" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G125" s="11" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="H125" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="I125" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J125" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="D126" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>311</v>
+        <v>93</v>
       </c>
       <c r="F126" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H126" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="I126" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J126" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D127" s="6">
         <v>0.1</v>
@@ -5665,7 +5641,7 @@
         <v>24</v>
       </c>
       <c r="G127" s="11" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H127" s="6">
         <v>0.1</v>
@@ -5679,112 +5655,112 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D128" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F128" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G128" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H128" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="I128" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="J128" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>304</v>
+        <v>107</v>
       </c>
       <c r="D129" s="6">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F129" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G129" s="11" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H129" s="6">
-        <v>0.15</v>
+        <v>20</v>
       </c>
       <c r="I129" s="6">
-        <v>0.15</v>
+        <v>20</v>
       </c>
       <c r="J129" s="6">
-        <v>0.15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>304</v>
+        <v>107</v>
       </c>
       <c r="D130" s="6">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F130" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="H130" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="I130" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="J130" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>324</v>
+        <v>107</v>
       </c>
       <c r="D131" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E131" s="11" t="s">
         <v>49</v>
@@ -5793,158 +5769,158 @@
         <v>24</v>
       </c>
       <c r="G131" s="11" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="H131" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I131" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J131" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="D132" s="6">
-        <v>20</v>
+        <v>0.05</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G132" s="11" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="H132" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I132" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="J132" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="D133" s="6">
-        <v>7</v>
+        <v>0.05</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F133" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H133" s="6">
-        <v>13</v>
+        <v>0.15</v>
       </c>
       <c r="I133" s="6">
-        <v>13</v>
+        <v>0.15</v>
       </c>
       <c r="J133" s="6">
-        <v>13</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="D134" s="6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F134" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="H134" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I134" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J134" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>304</v>
+        <v>107</v>
       </c>
       <c r="D135" s="6">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>93</v>
+        <v>328</v>
       </c>
       <c r="F135" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="H135" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="I135" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="J135" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>304</v>
+        <v>107</v>
       </c>
       <c r="D136" s="6">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E136" s="11" t="s">
         <v>93</v>
@@ -5953,30 +5929,30 @@
         <v>24</v>
       </c>
       <c r="G136" s="11" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="H136" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="I136" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J136" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D137" s="6">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>93</v>
@@ -5985,7 +5961,7 @@
         <v>24</v>
       </c>
       <c r="G137" s="11" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="H137" s="6">
         <v>0.1</v>
@@ -5994,102 +5970,6 @@
         <v>0.1</v>
       </c>
       <c r="J137" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B138" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D138" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="E138" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="F138" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G138" s="11" t="s">
-        <v>341</v>
-      </c>
-      <c r="H138" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="I138" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J138" s="6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B139" s="11" t="s">
-        <v>339</v>
-      </c>
-      <c r="C139" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D139" s="6">
-        <v>1</v>
-      </c>
-      <c r="E139" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F139" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G139" s="11" t="s">
-        <v>342</v>
-      </c>
-      <c r="H139" s="6">
-        <v>0</v>
-      </c>
-      <c r="I139" s="6">
-        <v>0</v>
-      </c>
-      <c r="J139" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="B140" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="C140" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="D140" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E140" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F140" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G140" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H140" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I140" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J140" s="6">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new parameters for capacity/reserves
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="368">
   <si>
     <t>parameter</t>
   </si>
@@ -1046,6 +1046,81 @@
   </si>
   <si>
     <t>ree_ems_thres_y</t>
+  </si>
+  <si>
+    <t>capacity and reserves</t>
+  </si>
+  <si>
+    <t>kareb.vf</t>
+  </si>
+  <si>
+    <t>car_sc</t>
+  </si>
+  <si>
+    <t>kareb.wohnant</t>
+  </si>
+  <si>
+    <t>kareb.areal</t>
+  </si>
+  <si>
+    <t>kareb.ausbau</t>
+  </si>
+  <si>
+    <t>kareb.ina.prozentpunkte</t>
+  </si>
+  <si>
+    <t>car_resi</t>
+  </si>
+  <si>
+    <t>car_plot</t>
+  </si>
+  <si>
+    <t>car_uti</t>
+  </si>
+  <si>
+    <t>kareb.ina.jahr</t>
+  </si>
+  <si>
+    <t>kareb.ina.lambda</t>
+  </si>
+  <si>
+    <t>car_lamda</t>
+  </si>
+  <si>
+    <t>car_y</t>
+  </si>
+  <si>
+    <t>car_pp</t>
+  </si>
+  <si>
+    <t>percent points</t>
+  </si>
+  <si>
+    <t>Proportion of staircases; for the conversion from total area to living area.</t>
+  </si>
+  <si>
+    <t>Proportion of plot construction ('slider'); 0% = without plot construction, 100% = with plot construction</t>
+  </si>
+  <si>
+    <t>Reference year of the usage values</t>
+  </si>
+  <si>
+    <t>lambda value of an exponential function exp(lambda * time since start of scenario); proportion of utilization per year</t>
+  </si>
+  <si>
+    <t>Residence portion ('slider'): -100% = minimum residential share according to the building regulation (BZO), 0% = real residential share, +100% = maximum residential share according to building regulation.</t>
+  </si>
+  <si>
+    <t>car_uti_input</t>
+  </si>
+  <si>
+    <t>degree of utilization used to calculate the input data</t>
+  </si>
+  <si>
+    <t>degree of utilization; linear influence on the capacity</t>
+  </si>
+  <si>
+    <t>usage: less or more percentage points (parameter between -100 and +100)</t>
   </si>
 </sst>
 </file>
@@ -1581,11 +1656,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G143" sqref="G143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1595,7 +1670,7 @@
     <col min="3" max="3" width="35.85546875" style="22" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="23" customWidth="1"/>
     <col min="5" max="5" width="18" style="21" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="19" style="21" customWidth="1"/>
     <col min="7" max="7" width="75.5703125" style="24" customWidth="1"/>
     <col min="8" max="10" width="6.7109375" style="23" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="5"/>
@@ -3329,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>22</v>
       </c>
@@ -5971,6 +6046,262 @@
       </c>
       <c r="J137" s="6">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A138" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B138" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="D138" s="29">
+        <v>25</v>
+      </c>
+      <c r="E138" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F138" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G138" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="H138" s="29">
+        <v>25</v>
+      </c>
+      <c r="I138" s="29">
+        <v>25</v>
+      </c>
+      <c r="J138" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A139" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B139" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C139" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="D139" s="29">
+        <v>0</v>
+      </c>
+      <c r="E139" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F139" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G139" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="H139" s="29">
+        <v>-25</v>
+      </c>
+      <c r="I139" s="29">
+        <v>0</v>
+      </c>
+      <c r="J139" s="29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A140" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B140" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="D140" s="29">
+        <v>50</v>
+      </c>
+      <c r="E140" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F140" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G140" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="H140" s="29">
+        <v>0</v>
+      </c>
+      <c r="I140" s="29">
+        <v>50</v>
+      </c>
+      <c r="J140" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B141" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="C141" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D141" s="29">
+        <v>85</v>
+      </c>
+      <c r="E141" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F141" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G141" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="H141" s="29">
+        <v>85</v>
+      </c>
+      <c r="I141" s="29">
+        <v>85</v>
+      </c>
+      <c r="J141" s="29">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A142" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B142" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="C142" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="D142" s="29">
+        <v>85</v>
+      </c>
+      <c r="E142" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F142" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G142" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="H142" s="29">
+        <v>75</v>
+      </c>
+      <c r="I142" s="29">
+        <v>85</v>
+      </c>
+      <c r="J142" s="29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A143" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B143" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="C143" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="D143" s="29">
+        <v>0</v>
+      </c>
+      <c r="E143" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="F143" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G143" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="H143" s="29">
+        <v>0</v>
+      </c>
+      <c r="I143" s="29">
+        <v>0</v>
+      </c>
+      <c r="J143" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A144" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B144" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="C144" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="D144" s="29">
+        <v>2044</v>
+      </c>
+      <c r="E144" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F144" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G144" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="H144" s="29">
+        <v>2044</v>
+      </c>
+      <c r="I144" s="29">
+        <v>2044</v>
+      </c>
+      <c r="J144" s="29">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A145" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B145" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="C145" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="D145" s="29">
+        <v>-0.04</v>
+      </c>
+      <c r="E145" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F145" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G145" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="H145" s="29">
+        <v>-0.04</v>
+      </c>
+      <c r="I145" s="29">
+        <v>-0.04</v>
+      </c>
+      <c r="J145" s="29">
+        <v>-0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new parameters for capacity
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1658,9 +1658,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:J145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G143" sqref="G143"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new parameter (round area)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="371">
   <si>
     <t>parameter</t>
   </si>
@@ -1121,6 +1121,15 @@
   </si>
   <si>
     <t>usage: less or more percentage points (parameter between -100 and +100)</t>
+  </si>
+  <si>
+    <t>round_area</t>
+  </si>
+  <si>
+    <t>digits (area)</t>
+  </si>
+  <si>
+    <t>rounding of area (e.g. ha in the capacity and reserve module)</t>
   </si>
 </sst>
 </file>
@@ -1656,11 +1665,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2860,36 +2869,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="12">
-        <v>15</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H38" s="12">
-        <v>15</v>
-      </c>
-      <c r="I38" s="12">
-        <v>15</v>
-      </c>
-      <c r="J38" s="12">
-        <v>15</v>
+    <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="26">
+        <v>4</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="H38" s="29">
+        <v>4</v>
+      </c>
+      <c r="I38" s="29">
+        <v>4</v>
+      </c>
+      <c r="J38" s="29">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2897,13 +2906,13 @@
         <v>22</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" s="12">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>36</v>
@@ -2912,48 +2921,48 @@
         <v>23</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H39" s="12">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="I39" s="12">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="J39" s="12">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="7">
-        <v>100</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H40" s="7">
-        <v>100</v>
-      </c>
-      <c r="I40" s="7">
-        <v>100</v>
-      </c>
-      <c r="J40" s="7">
-        <v>100</v>
+        <v>4</v>
+      </c>
+      <c r="D40" s="12">
+        <v>49</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="12">
+        <v>49</v>
+      </c>
+      <c r="I40" s="12">
+        <v>49</v>
+      </c>
+      <c r="J40" s="12">
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -2961,13 +2970,13 @@
         <v>22</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>35</v>
@@ -2976,16 +2985,16 @@
         <v>24</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H41" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I41" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J41" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -2993,13 +3002,13 @@
         <v>22</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D42" s="7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>35</v>
@@ -3008,48 +3017,48 @@
         <v>24</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H42" s="7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I42" s="7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J42" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H43" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I43" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J43" s="7">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3057,42 +3066,42 @@
         <v>22</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="12">
-        <v>20</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H44" s="12">
-        <v>20</v>
-      </c>
-      <c r="I44" s="12">
-        <v>20</v>
-      </c>
-      <c r="J44" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0</v>
+      </c>
+      <c r="I44" s="7">
+        <v>0</v>
+      </c>
+      <c r="J44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="12">
         <v>20</v>
@@ -3101,10 +3110,10 @@
         <v>49</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H45" s="12">
         <v>20</v>
@@ -3116,36 +3125,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D46" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H46" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I46" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J46" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3153,45 +3162,45 @@
         <v>22</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="D47" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="H47" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I47" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J47" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>87</v>
+      <c r="D48" s="12">
+        <v>0</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>49</v>
@@ -3200,48 +3209,48 @@
         <v>61</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H48" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J48" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="H48" s="12">
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <v>0</v>
+      </c>
+      <c r="J48" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D49" s="12">
-        <v>30</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>65</v>
+      <c r="D49" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="F49" s="11" t="s">
         <v>61</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H49" s="12">
-        <v>30</v>
-      </c>
-      <c r="I49" s="12">
-        <v>30</v>
-      </c>
-      <c r="J49" s="12">
-        <v>30</v>
+        <v>90</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3249,31 +3258,31 @@
         <v>22</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="D50" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="H50" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I50" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J50" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3281,39 +3290,39 @@
         <v>22</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="D51" s="12">
-        <v>20</v>
-      </c>
-      <c r="E51" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="H51" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I51" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J51" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>107</v>
@@ -3325,10 +3334,10 @@
         <v>49</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H52" s="12">
         <v>20</v>
@@ -3340,36 +3349,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D53" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H53" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I53" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J53" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3377,31 +3386,31 @@
         <v>22</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D54" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H54" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I54" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J54" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3409,13 +3418,13 @@
         <v>22</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D55" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>49</v>
@@ -3424,62 +3433,62 @@
         <v>61</v>
       </c>
       <c r="G55" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H55" s="12">
+        <v>0</v>
+      </c>
+      <c r="I55" s="12">
+        <v>0</v>
+      </c>
+      <c r="J55" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="12">
+        <v>100</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="H55" s="12">
+      <c r="H56" s="12">
         <v>100</v>
       </c>
-      <c r="I55" s="12">
+      <c r="I56" s="12">
         <v>100</v>
       </c>
-      <c r="J55" s="12">
+      <c r="J56" s="12">
         <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D56" s="14">
-        <v>30</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="H56" s="16">
-        <v>30</v>
-      </c>
-      <c r="I56" s="14">
-        <v>30</v>
-      </c>
-      <c r="J56" s="14">
-        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D57" s="19">
-        <v>99</v>
+      <c r="B57" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="14">
+        <v>30</v>
       </c>
       <c r="E57" s="14" t="s">
         <v>101</v>
@@ -3488,30 +3497,30 @@
         <v>24</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H57" s="19">
-        <v>99</v>
-      </c>
-      <c r="I57" s="19">
-        <v>99</v>
-      </c>
-      <c r="J57" s="19">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="H57" s="16">
+        <v>30</v>
+      </c>
+      <c r="I57" s="14">
+        <v>30</v>
+      </c>
+      <c r="J57" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>107</v>
+      <c r="B58" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="D58" s="19">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>101</v>
@@ -3520,30 +3529,30 @@
         <v>24</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="H58" s="19">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I58" s="19">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="J58" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D59" s="19">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E59" s="14" t="s">
         <v>101</v>
@@ -3551,28 +3560,28 @@
       <c r="F59" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G59" s="20" t="s">
-        <v>109</v>
+      <c r="G59" s="15" t="s">
+        <v>115</v>
       </c>
       <c r="H59" s="19">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="I59" s="19">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J59" s="19">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="17" t="s">
-        <v>116</v>
+      <c r="B60" s="32" t="s">
+        <v>108</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D60" s="19">
         <v>120</v>
@@ -3584,7 +3593,7 @@
         <v>24</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="H60" s="19">
         <v>120</v>
@@ -3601,39 +3610,45 @@
         <v>100</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D61" s="19">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
+        <v>117</v>
+      </c>
+      <c r="H61" s="19">
+        <v>120</v>
+      </c>
+      <c r="I61" s="19">
+        <v>120</v>
+      </c>
+      <c r="J61" s="19">
+        <v>120</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D62" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="14" t="s">
         <v>93</v>
@@ -3642,85 +3657,79 @@
         <v>61</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
       <c r="J62" s="19"/>
     </row>
-    <row r="63" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B63" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D63" s="19">
+        <v>3</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+    </row>
+    <row r="64" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" s="19">
+      <c r="C64" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="19">
         <v>0.8</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E64" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F63" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G63" s="20" t="s">
+      <c r="F64" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G64" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="H63" s="19">
+      <c r="H64" s="19">
         <v>0.8</v>
       </c>
-      <c r="I63" s="19">
+      <c r="I64" s="19">
         <v>0.8</v>
       </c>
-      <c r="J63" s="19">
+      <c r="J64" s="19">
         <v>0.8</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" s="12">
-        <v>20</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G64" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="H64" s="12">
-        <v>20</v>
-      </c>
-      <c r="I64" s="12">
-        <v>20</v>
-      </c>
-      <c r="J64" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>159</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D65" s="12">
         <v>20</v>
@@ -3732,7 +3741,7 @@
         <v>24</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H65" s="12">
         <v>20</v>
@@ -3744,36 +3753,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>159</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D66" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F66" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H66" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I66" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J66" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3781,31 +3790,31 @@
         <v>159</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="D67" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="H67" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I67" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J67" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3813,42 +3822,42 @@
         <v>159</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="D68" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>49</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="H68" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I68" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J68" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>159</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D69" s="12">
         <v>20</v>
@@ -3860,7 +3869,7 @@
         <v>24</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="H69" s="12">
         <v>20</v>
@@ -3872,36 +3881,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>159</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D70" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F70" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="H70" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I70" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J70" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3909,54 +3918,54 @@
         <v>159</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="D71" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H71" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I71" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J71" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B72" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>169</v>
+      <c r="B72" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="D72" s="12">
         <v>0</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="H72" s="12">
         <v>0</v>
@@ -3973,13 +3982,13 @@
         <v>159</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D73" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>101</v>
@@ -3988,48 +3997,48 @@
         <v>24</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H73" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="I73" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J73" s="12">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>171</v>
+      <c r="B74" s="32" t="s">
+        <v>168</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="D74" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="F74" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H74" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="I74" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="J74" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -4037,39 +4046,39 @@
         <v>159</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="C75" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C75" s="13" t="s">
         <v>107</v>
       </c>
       <c r="D75" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F75" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H75" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I75" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J75" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
         <v>159</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>107</v>
@@ -4084,7 +4093,7 @@
         <v>24</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H76" s="12">
         <v>20</v>
@@ -4096,36 +4105,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>159</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D77" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F77" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H77" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I77" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J77" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -4133,74 +4142,74 @@
         <v>159</v>
       </c>
       <c r="B78" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="12">
+        <v>13</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="H78" s="12">
+        <v>13</v>
+      </c>
+      <c r="I78" s="12">
+        <v>13</v>
+      </c>
+      <c r="J78" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D78" s="12">
-        <v>0</v>
-      </c>
-      <c r="E78" s="11" t="s">
+      <c r="C79" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="12">
+        <v>0</v>
+      </c>
+      <c r="E79" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F78" s="11" t="s">
+      <c r="F79" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G78" s="13" t="s">
+      <c r="G79" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="H78" s="12">
-        <v>0</v>
-      </c>
-      <c r="I78" s="12">
-        <v>0</v>
-      </c>
-      <c r="J78" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="B79" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D79" s="26">
-        <v>20</v>
-      </c>
-      <c r="E79" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="F79" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G79" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="H79" s="26">
-        <v>20</v>
-      </c>
-      <c r="I79" s="26">
-        <v>20</v>
-      </c>
-      <c r="J79" s="26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="H79" s="12">
+        <v>0</v>
+      </c>
+      <c r="I79" s="12">
+        <v>0</v>
+      </c>
+      <c r="J79" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D80" s="26">
         <v>20</v>
@@ -4212,7 +4221,7 @@
         <v>24</v>
       </c>
       <c r="G80" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H80" s="26">
         <v>20</v>
@@ -4224,36 +4233,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A81" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D81" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E81" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F81" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G81" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H81" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I81" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J81" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4261,31 +4270,31 @@
         <v>196</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>107</v>
+        <v>224</v>
       </c>
       <c r="D82" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E82" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G82" s="30" t="s">
-        <v>91</v>
+        <v>214</v>
       </c>
       <c r="H82" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I82" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J82" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4293,42 +4302,42 @@
         <v>196</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>225</v>
+        <v>107</v>
       </c>
       <c r="D83" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E83" s="25" t="s">
         <v>49</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G83" s="30" t="s">
-        <v>153</v>
+        <v>91</v>
       </c>
       <c r="H83" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I83" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J83" s="26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D84" s="26">
         <v>20</v>
@@ -4340,7 +4349,7 @@
         <v>24</v>
       </c>
       <c r="G84" s="30" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="H84" s="26">
         <v>20</v>
@@ -4352,36 +4361,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="C85" s="31" t="s">
-        <v>227</v>
+        <v>202</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="D85" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E85" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F85" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G85" s="30" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="H85" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I85" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J85" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4389,54 +4398,54 @@
         <v>196</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>204</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>107</v>
+        <v>203</v>
+      </c>
+      <c r="C86" s="31" t="s">
+        <v>227</v>
       </c>
       <c r="D86" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E86" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G86" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H86" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I86" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J86" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B87" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="C87" s="30" t="s">
-        <v>228</v>
+      <c r="B87" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="D87" s="26">
         <v>0</v>
       </c>
       <c r="E87" s="25" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G87" s="30" t="s">
-        <v>215</v>
+        <v>157</v>
       </c>
       <c r="H87" s="26">
         <v>0</v>
@@ -4453,13 +4462,13 @@
         <v>196</v>
       </c>
       <c r="B88" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C88" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D88" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E88" s="25" t="s">
         <v>101</v>
@@ -4468,48 +4477,48 @@
         <v>24</v>
       </c>
       <c r="G88" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H88" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="I88" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J88" s="26">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A89" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="B89" s="25" t="s">
-        <v>207</v>
+      <c r="B89" s="32" t="s">
+        <v>206</v>
       </c>
       <c r="C89" s="30" t="s">
-        <v>107</v>
+        <v>229</v>
       </c>
       <c r="D89" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E89" s="25" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="F89" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G89" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H89" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="I89" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="J89" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4517,39 +4526,39 @@
         <v>196</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C90" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C90" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D90" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E90" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F90" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G90" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H90" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I90" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="J90" s="26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>107</v>
@@ -4564,7 +4573,7 @@
         <v>24</v>
       </c>
       <c r="G91" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H91" s="26">
         <v>20</v>
@@ -4576,36 +4585,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A92" s="25" t="s">
         <v>196</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D92" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F92" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G92" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H92" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I92" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J92" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4613,95 +4622,95 @@
         <v>196</v>
       </c>
       <c r="B93" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D93" s="26">
+        <v>13</v>
+      </c>
+      <c r="E93" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F93" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G93" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="H93" s="26">
+        <v>13</v>
+      </c>
+      <c r="I93" s="26">
+        <v>13</v>
+      </c>
+      <c r="J93" s="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="C93" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D93" s="26">
-        <v>0</v>
-      </c>
-      <c r="E93" s="25" t="s">
+      <c r="C94" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D94" s="26">
+        <v>0</v>
+      </c>
+      <c r="E94" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F93" s="25" t="s">
+      <c r="F94" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G93" s="30" t="s">
+      <c r="G94" s="30" t="s">
         <v>221</v>
       </c>
-      <c r="H93" s="26">
-        <v>0</v>
-      </c>
-      <c r="I93" s="26">
-        <v>0</v>
-      </c>
-      <c r="J93" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C94" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D94" s="12">
-        <v>70</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F94" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G94" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="H94" s="12">
-        <v>70</v>
-      </c>
-      <c r="I94" s="12">
-        <v>70</v>
-      </c>
-      <c r="J94" s="12">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H94" s="26">
+        <v>0</v>
+      </c>
+      <c r="I94" s="26">
+        <v>0</v>
+      </c>
+      <c r="J94" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="B95" s="11" t="s">
-        <v>256</v>
+      <c r="B95" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D95" s="6">
-        <v>0.2</v>
+        <v>235</v>
+      </c>
+      <c r="D95" s="12">
+        <v>70</v>
       </c>
       <c r="E95" s="11" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="G95" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="H95" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="I95" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="J95" s="6">
-        <v>0.2</v>
+        <v>24</v>
+      </c>
+      <c r="G95" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="H95" s="12">
+        <v>70</v>
+      </c>
+      <c r="I95" s="12">
+        <v>70</v>
+      </c>
+      <c r="J95" s="12">
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4709,7 +4718,7 @@
         <v>236</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>241</v>
@@ -4724,7 +4733,7 @@
         <v>66</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H96" s="6">
         <v>0.2</v>
@@ -4741,13 +4750,13 @@
         <v>236</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>333</v>
+        <v>257</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>241</v>
       </c>
       <c r="D97" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>93</v>
@@ -4756,16 +4765,16 @@
         <v>66</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>335</v>
+        <v>243</v>
       </c>
       <c r="H97" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="I97" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="J97" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4773,7 +4782,7 @@
         <v>236</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>241</v>
@@ -4788,7 +4797,7 @@
         <v>66</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H98" s="6">
         <v>0.12</v>
@@ -4805,31 +4814,31 @@
         <v>236</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D99" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>246</v>
+        <v>93</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H99" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="I99" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="J99" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="100" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4837,74 +4846,74 @@
         <v>236</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>258</v>
+        <v>337</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D100" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E100" s="11" t="s">
-        <v>93</v>
+        <v>246</v>
       </c>
       <c r="F100" s="11" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G100" s="11" t="s">
-        <v>247</v>
+        <v>338</v>
       </c>
       <c r="H100" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I100" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="J100" s="6">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D101" s="12">
-        <v>20</v>
+        <v>241</v>
+      </c>
+      <c r="D101" s="6">
+        <v>0.3</v>
       </c>
       <c r="E101" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G101" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="H101" s="12">
-        <v>20</v>
-      </c>
-      <c r="I101" s="12">
-        <v>20</v>
-      </c>
-      <c r="J101" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="H101" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I101" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J101" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>107</v>
+        <v>252</v>
       </c>
       <c r="D102" s="12">
         <v>20</v>
@@ -4916,7 +4925,7 @@
         <v>24</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H102" s="12">
         <v>20</v>
@@ -4928,36 +4937,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D103" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F103" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H103" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I103" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J103" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -4965,31 +4974,31 @@
         <v>236</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D104" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G104" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H104" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I104" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J104" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -4997,13 +5006,13 @@
         <v>236</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D105" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E105" s="11" t="s">
         <v>49</v>
@@ -5012,112 +5021,112 @@
         <v>61</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H105" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I105" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J105" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B106" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D106" s="12">
+        <v>100</v>
+      </c>
+      <c r="E106" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F106" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G106" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="H106" s="12">
+        <v>100</v>
+      </c>
+      <c r="I106" s="12">
+        <v>100</v>
+      </c>
+      <c r="J106" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B107" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="C106" s="6" t="s">
+      <c r="C107" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D107" s="6">
         <v>0.15</v>
       </c>
-      <c r="E106" s="11" t="s">
+      <c r="E107" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="F107" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G106" s="11" t="s">
+      <c r="G107" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="H106" s="6">
+      <c r="H107" s="6">
         <v>0.15</v>
       </c>
-      <c r="I106" s="6">
+      <c r="I107" s="6">
         <v>0.15</v>
       </c>
-      <c r="J106" s="6">
+      <c r="J107" s="6">
         <v>0.15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A107" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="B107" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="C107" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="D107" s="29">
-        <v>70</v>
-      </c>
-      <c r="E107" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F107" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G107" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="H107" s="29">
-        <v>70</v>
-      </c>
-      <c r="I107" s="29">
-        <v>70</v>
-      </c>
-      <c r="J107" s="29">
-        <v>70</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="B108" s="27" t="s">
-        <v>277</v>
+      <c r="B108" s="14" t="s">
+        <v>274</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="D108" s="14">
-        <v>0.2</v>
+        <v>235</v>
+      </c>
+      <c r="D108" s="29">
+        <v>70</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G108" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="H108" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="I108" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="J108" s="14">
-        <v>0.2</v>
+        <v>24</v>
+      </c>
+      <c r="G108" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="H108" s="29">
+        <v>70</v>
+      </c>
+      <c r="I108" s="29">
+        <v>70</v>
+      </c>
+      <c r="J108" s="29">
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
@@ -5125,7 +5134,7 @@
         <v>265</v>
       </c>
       <c r="B109" s="27" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>241</v>
@@ -5140,7 +5149,7 @@
         <v>66</v>
       </c>
       <c r="G109" s="27" t="s">
-        <v>243</v>
+        <v>276</v>
       </c>
       <c r="H109" s="14">
         <v>0.2</v>
@@ -5157,13 +5166,13 @@
         <v>265</v>
       </c>
       <c r="B110" s="27" t="s">
-        <v>339</v>
+        <v>266</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D110" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E110" s="27" t="s">
         <v>93</v>
@@ -5172,16 +5181,16 @@
         <v>66</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>341</v>
+        <v>243</v>
       </c>
       <c r="H110" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="I110" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="J110" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
@@ -5189,7 +5198,7 @@
         <v>265</v>
       </c>
       <c r="B111" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>241</v>
@@ -5204,7 +5213,7 @@
         <v>66</v>
       </c>
       <c r="G111" s="27" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="H111" s="14">
         <v>0.12</v>
@@ -5221,31 +5230,31 @@
         <v>265</v>
       </c>
       <c r="B112" s="27" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D112" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>246</v>
+        <v>93</v>
       </c>
       <c r="F112" s="27" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G112" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H112" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="I112" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="J112" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
@@ -5253,74 +5262,74 @@
         <v>265</v>
       </c>
       <c r="B113" s="27" t="s">
-        <v>267</v>
+        <v>342</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D113" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>93</v>
+        <v>246</v>
       </c>
       <c r="F113" s="27" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G113" s="27" t="s">
-        <v>247</v>
+        <v>338</v>
       </c>
       <c r="H113" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I113" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="J113" s="14">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="27" t="s">
         <v>265</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="D114" s="29">
-        <v>20</v>
+        <v>241</v>
+      </c>
+      <c r="D114" s="14">
+        <v>0.3</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F114" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="G114" s="28" t="s">
-        <v>278</v>
-      </c>
-      <c r="H114" s="29">
-        <v>20</v>
-      </c>
-      <c r="I114" s="29">
-        <v>20</v>
-      </c>
-      <c r="J114" s="29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="G114" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="H114" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="I114" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="J114" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" s="27" t="s">
         <v>265</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>107</v>
+        <v>252</v>
       </c>
       <c r="D115" s="29">
         <v>20</v>
@@ -5332,7 +5341,7 @@
         <v>24</v>
       </c>
       <c r="G115" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H115" s="29">
         <v>20</v>
@@ -5344,36 +5353,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A116" s="27" t="s">
         <v>265</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D116" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E116" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F116" s="27" t="s">
         <v>24</v>
       </c>
       <c r="G116" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H116" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I116" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J116" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -5381,31 +5390,31 @@
         <v>265</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C117" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D117" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E117" s="27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F117" s="27" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="G117" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H117" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I117" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J117" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -5413,13 +5422,13 @@
         <v>265</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D118" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E118" s="27" t="s">
         <v>49</v>
@@ -5428,80 +5437,80 @@
         <v>61</v>
       </c>
       <c r="G118" s="28" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H118" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I118" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J118" s="29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
         <v>265</v>
       </c>
       <c r="B119" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D119" s="29">
+        <v>100</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F119" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G119" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="H119" s="29">
+        <v>100</v>
+      </c>
+      <c r="I119" s="29">
+        <v>100</v>
+      </c>
+      <c r="J119" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A120" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="B120" s="27" t="s">
         <v>273</v>
       </c>
-      <c r="C119" s="14" t="s">
+      <c r="C120" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="D119" s="14">
+      <c r="D120" s="14">
         <v>0.15</v>
       </c>
-      <c r="E119" s="27" t="s">
+      <c r="E120" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F119" s="27" t="s">
+      <c r="F120" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G119" s="27" t="s">
+      <c r="G120" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="H119" s="14">
+      <c r="H120" s="14">
         <v>0.15</v>
       </c>
-      <c r="I119" s="14">
+      <c r="I120" s="14">
         <v>0.15</v>
       </c>
-      <c r="J119" s="14">
+      <c r="J120" s="14">
         <v>0.15</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A120" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="D120" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="F120" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G120" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="H120" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="I120" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="J120" s="6">
-        <v>0.1</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
@@ -5509,13 +5518,13 @@
         <v>291</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>292</v>
       </c>
       <c r="D121" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E121" s="11" t="s">
         <v>93</v>
@@ -5524,16 +5533,16 @@
         <v>24</v>
       </c>
       <c r="G121" s="11" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="H121" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I121" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J121" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
@@ -5541,31 +5550,31 @@
         <v>291</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D122" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="F122" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G122" s="11" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H122" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="I122" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="J122" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
@@ -5573,31 +5582,31 @@
         <v>291</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>107</v>
+        <v>298</v>
       </c>
       <c r="D123" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>299</v>
+        <v>35</v>
       </c>
       <c r="F123" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H123" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I123" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J123" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
@@ -5605,31 +5614,31 @@
         <v>291</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>292</v>
+        <v>107</v>
       </c>
       <c r="D124" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>93</v>
+        <v>299</v>
       </c>
       <c r="F124" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H124" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I124" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J124" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
@@ -5637,7 +5646,7 @@
         <v>291</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>292</v>
@@ -5652,7 +5661,7 @@
         <v>24</v>
       </c>
       <c r="G125" s="11" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="H125" s="6">
         <v>0.1</v>
@@ -5669,7 +5678,7 @@
         <v>291</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>292</v>
@@ -5684,16 +5693,16 @@
         <v>24</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H126" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I126" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J126" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
@@ -5701,7 +5710,7 @@
         <v>291</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>292</v>
@@ -5716,16 +5725,16 @@
         <v>24</v>
       </c>
       <c r="G127" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H127" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I127" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J127" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
@@ -5733,31 +5742,31 @@
         <v>291</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="D128" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F128" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G128" s="11" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="H128" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I128" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="J128" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
@@ -5765,10 +5774,10 @@
         <v>291</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>107</v>
+        <v>312</v>
       </c>
       <c r="D129" s="6">
         <v>20</v>
@@ -5780,7 +5789,7 @@
         <v>24</v>
       </c>
       <c r="G129" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H129" s="6">
         <v>20</v>
@@ -5797,31 +5806,31 @@
         <v>291</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D130" s="6">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F130" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H130" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I130" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J130" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
@@ -5829,31 +5838,31 @@
         <v>291</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D131" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E131" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F131" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G131" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H131" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I131" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J131" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
@@ -5861,31 +5870,31 @@
         <v>291</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>292</v>
+        <v>107</v>
       </c>
       <c r="D132" s="6">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G132" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="H132" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I132" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J132" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
@@ -5893,7 +5902,7 @@
         <v>291</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C133" s="6" t="s">
         <v>292</v>
@@ -5908,16 +5917,16 @@
         <v>24</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H133" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I133" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J133" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
@@ -5925,7 +5934,7 @@
         <v>291</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C134" s="6" t="s">
         <v>292</v>
@@ -5940,16 +5949,16 @@
         <v>24</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H134" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="I134" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="J134" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
@@ -5957,31 +5966,31 @@
         <v>291</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="D135" s="6">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>328</v>
+        <v>93</v>
       </c>
       <c r="F135" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H135" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="I135" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J135" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
@@ -5989,31 +5998,31 @@
         <v>291</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C136" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D136" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>93</v>
+        <v>328</v>
       </c>
       <c r="F136" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G136" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H136" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I136" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J136" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
@@ -6021,13 +6030,13 @@
         <v>291</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>292</v>
+        <v>107</v>
       </c>
       <c r="D137" s="6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E137" s="11" t="s">
         <v>93</v>
@@ -6036,94 +6045,94 @@
         <v>24</v>
       </c>
       <c r="G137" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="H137" s="6">
+        <v>0</v>
+      </c>
+      <c r="I137" s="6">
+        <v>0</v>
+      </c>
+      <c r="J137" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A138" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B138" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D138" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E138" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F138" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G138" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="H137" s="6">
+      <c r="H138" s="6">
         <v>0.1</v>
       </c>
-      <c r="I137" s="6">
+      <c r="I138" s="6">
         <v>0.1</v>
       </c>
-      <c r="J137" s="6">
+      <c r="J138" s="6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="B138" s="27" t="s">
-        <v>345</v>
-      </c>
-      <c r="C138" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="D138" s="29">
-        <v>25</v>
-      </c>
-      <c r="E138" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="F138" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G138" s="28" t="s">
-        <v>359</v>
-      </c>
-      <c r="H138" s="29">
-        <v>25</v>
-      </c>
-      <c r="I138" s="29">
-        <v>25</v>
-      </c>
-      <c r="J138" s="29">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="27" t="s">
         <v>343</v>
       </c>
       <c r="B139" s="27" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D139" s="29">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E139" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F139" s="27" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G139" s="28" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H139" s="29">
-        <v>-25</v>
+        <v>25</v>
       </c>
       <c r="I139" s="29">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J139" s="29">
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A140" s="27" t="s">
         <v>343</v>
       </c>
       <c r="B140" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D140" s="29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E140" s="27" t="s">
         <v>49</v>
@@ -6132,30 +6141,30 @@
         <v>51</v>
       </c>
       <c r="G140" s="28" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="H140" s="29">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="I140" s="29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J140" s="29">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A141" s="27" t="s">
         <v>343</v>
       </c>
       <c r="B141" s="27" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>107</v>
+        <v>347</v>
       </c>
       <c r="D141" s="29">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="E141" s="27" t="s">
         <v>49</v>
@@ -6164,16 +6173,16 @@
         <v>51</v>
       </c>
       <c r="G141" s="28" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="H141" s="29">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="I141" s="29">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="J141" s="29">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
@@ -6181,10 +6190,10 @@
         <v>343</v>
       </c>
       <c r="B142" s="27" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>348</v>
+        <v>107</v>
       </c>
       <c r="D142" s="29">
         <v>85</v>
@@ -6196,16 +6205,16 @@
         <v>51</v>
       </c>
       <c r="G142" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H142" s="29">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="I142" s="29">
         <v>85</v>
       </c>
       <c r="J142" s="29">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
@@ -6213,31 +6222,31 @@
         <v>343</v>
       </c>
       <c r="B143" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D143" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E143" s="27" t="s">
-        <v>358</v>
+        <v>49</v>
       </c>
       <c r="F143" s="27" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G143" s="28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H143" s="29">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I143" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="J143" s="29">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
@@ -6245,62 +6254,94 @@
         <v>343</v>
       </c>
       <c r="B144" s="27" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D144" s="29">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="E144" s="27" t="s">
-        <v>36</v>
+        <v>358</v>
       </c>
       <c r="F144" s="27" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="G144" s="28" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="H144" s="29">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="I144" s="29">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="J144" s="29">
-        <v>2044</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="27" t="s">
         <v>343</v>
       </c>
       <c r="B145" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="C145" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="D145" s="29">
+        <v>2044</v>
+      </c>
+      <c r="E145" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F145" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G145" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="H145" s="29">
+        <v>2044</v>
+      </c>
+      <c r="I145" s="29">
+        <v>2044</v>
+      </c>
+      <c r="J145" s="29">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A146" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B146" s="27" t="s">
         <v>355</v>
       </c>
-      <c r="C145" s="14" t="s">
+      <c r="C146" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="D145" s="29">
+      <c r="D146" s="29">
         <v>-0.04</v>
       </c>
-      <c r="E145" s="27" t="s">
+      <c r="E146" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="F145" s="27" t="s">
+      <c r="F146" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="G145" s="28" t="s">
+      <c r="G146" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="H145" s="29">
+      <c r="H146" s="29">
         <v>-0.04</v>
       </c>
-      <c r="I145" s="29">
+      <c r="I146" s="29">
         <v>-0.04</v>
       </c>
-      <c r="J145" s="29">
+      <c r="J146" s="29">
         <v>-0.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new parameters (project list)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4780BE7-D0E1-441E-8D53-C45145421C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28668BC2-7FDB-498A-A3F9-F110A054EC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1916,11 +1916,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J175"/>
+  <dimension ref="A1:J173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7460,12 +7460,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F174" s="22"/>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F175" s="22"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new parameter (data source for percentage of cooperative housing)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587DE7C0-9F74-4DC1-92E2-73BFBA145E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="465">
   <si>
     <t>parameter</t>
   </si>
@@ -1401,12 +1400,24 @@
   </si>
   <si>
     <t>rounding of people</t>
+  </si>
+  <si>
+    <t>housing model</t>
+  </si>
+  <si>
+    <t>similar to wohn.modell.typ</t>
+  </si>
+  <si>
+    <t>car_coop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of cooperative housing can be used from capacity/reserves (car_coop = 100), or from the trends in the districts (car_coop = 0) or a mixture of both data sources. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1626,7 +1637,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1730,23 +1741,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1782,23 +1776,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1974,13 +1951,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J181"/>
+  <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7776,6 +7753,38 @@
         <v>100</v>
       </c>
     </row>
+    <row r="182" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A182" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="B182" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="D182" s="12">
+        <v>20</v>
+      </c>
+      <c r="E182" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F182" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G182" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="H182" s="12">
+        <v>20</v>
+      </c>
+      <c r="I182" s="12">
+        <v>20</v>
+      </c>
+      <c r="J182" s="12">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new parameter (housing module)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1411,7 +1411,7 @@
     <t>car_coop</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage of cooperative housing can be used from capacity/reserves (car_coop = 100), or from the trends in the districts (car_coop = 0) or a mixture of both data sources. </t>
+    <t>Percentage of cooperative housing can be used from capacity/reserves (car_coop = 100), or from the trends in the districts (car_coop = 0) or a mixture of both data sources. In other words: car_coop = percentage used from capacity/reserves.</t>
   </si>
 </sst>
 </file>
@@ -1956,8 +1956,8 @@
   <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C150" sqref="C150"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7753,7 +7753,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A182" s="11" t="s">
         <v>461</v>
       </c>

</xml_diff>

<commit_message>
new parameters (proportion of empty apartments)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C6949-79B1-45D3-A715-0CB19D6B8377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="470">
   <si>
     <t>parameter</t>
   </si>
@@ -1413,12 +1412,27 @@
   </si>
   <si>
     <t>Percentage of cooperative housing can be used from capacity/reserves (car_coop = 100), or from the trends in the districts (car_coop = 0) or a mixture of both data sources. In other words: car_coop = percentage used from capacity/reserves.</t>
+  </si>
+  <si>
+    <t>empty_coop</t>
+  </si>
+  <si>
+    <t>similar to wohn.modell.anteil.leerwhg</t>
+  </si>
+  <si>
+    <t>empty_private</t>
+  </si>
+  <si>
+    <t>Percentage of empty apartments (cooperative housing)</t>
+  </si>
+  <si>
+    <t>Percentage of empty apartments (private housing)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1638,7 +1652,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1742,23 +1756,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1794,23 +1791,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1986,13 +1966,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J182"/>
+  <dimension ref="A1:J184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C182" sqref="C182"/>
+      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7820,6 +7800,70 @@
         <v>20</v>
       </c>
     </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A183" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="B183" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="D183" s="12">
+        <v>0</v>
+      </c>
+      <c r="E183" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F183" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G183" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="H183" s="12">
+        <v>0</v>
+      </c>
+      <c r="I183" s="12">
+        <v>0</v>
+      </c>
+      <c r="J183" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A184" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="B184" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="D184" s="12">
+        <v>0</v>
+      </c>
+      <c r="E184" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F184" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G184" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="H184" s="12">
+        <v>0</v>
+      </c>
+      <c r="I184" s="12">
+        <v>0</v>
+      </c>
+      <c r="J184" s="12">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new parameters: less/more living space
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="476">
   <si>
     <t>parameter</t>
   </si>
@@ -1427,6 +1427,24 @@
   </si>
   <si>
     <t>Percentage of empty apartments (private housing)</t>
+  </si>
+  <si>
+    <t>demography and housing model</t>
+  </si>
+  <si>
+    <t>prop_less_ims</t>
+  </si>
+  <si>
+    <t>less living space available (according to reserves, compared to trend calcuation). Then immigration* is descreased, and emigration* increased. This parameter determines how much of the difference is compensated by changes of immigration* (the remainder is corrected with emigration*)</t>
+  </si>
+  <si>
+    <t>more living space available (according to reserves, compared to trend calcuation). Then immigration* is inscreased, and emigration* decreased. This parameter determines how much of the difference is compensated by changes of immigration* (the remainder is corrected with emigration*)</t>
+  </si>
+  <si>
+    <t>similar to mod.ant.zuz (in the previous model only one parameter for both situations: less or more living space available)</t>
+  </si>
+  <si>
+    <t>prop_more_ims</t>
   </si>
 </sst>
 </file>
@@ -1968,11 +1986,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:J184"/>
+  <dimension ref="A1:J186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A178" sqref="A178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7864,6 +7882,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="185" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A185" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="B185" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="C185" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="D185" s="29">
+        <v>80</v>
+      </c>
+      <c r="E185" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F185" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G185" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="H185" s="29">
+        <v>80</v>
+      </c>
+      <c r="I185" s="29">
+        <v>80</v>
+      </c>
+      <c r="J185" s="29">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A186" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="B186" s="27" t="s">
+        <v>475</v>
+      </c>
+      <c r="C186" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="D186" s="29">
+        <v>60</v>
+      </c>
+      <c r="E186" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F186" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G186" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="H186" s="29">
+        <v>60</v>
+      </c>
+      <c r="I186" s="29">
+        <v>60</v>
+      </c>
+      <c r="J186" s="29">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new parameter: capacity/reserves vs. project list
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19DFAF9-6846-4A6C-B93D-4B239D32DAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686CADA0-9110-4AA3-80C2-126AF03213AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="477">
   <si>
     <t>parameter</t>
   </si>
@@ -1443,6 +1443,12 @@
   </si>
   <si>
     <t>middle</t>
+  </si>
+  <si>
+    <t>car_trust</t>
+  </si>
+  <si>
+    <t>If the amount of people according to the project list exceeds the population according to capacity/reserves: trust the capacity/reserves number (parameter = 100%)? Or the project list (parameter = 0%)?</t>
   </si>
 </sst>
 </file>
@@ -2018,10 +2024,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -7317,33 +7323,33 @@
         <v>462</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
         <v>459</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>464</v>
+        <v>105</v>
       </c>
       <c r="D183" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E183" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F183" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G183" s="11" t="s">
         <v>47</v>
       </c>
       <c r="H183" s="11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I183" s="13" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.2">
@@ -7351,7 +7357,7 @@
         <v>459</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>464</v>
@@ -7372,36 +7378,36 @@
         <v>22</v>
       </c>
       <c r="I184" s="13" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A185" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B185" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="D185" s="12">
+        <v>0</v>
+      </c>
+      <c r="E185" s="12">
+        <v>0</v>
+      </c>
+      <c r="F185" s="12">
+        <v>0</v>
+      </c>
+      <c r="G185" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H185" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I185" s="13" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A185" s="27" t="s">
-        <v>468</v>
-      </c>
-      <c r="B185" s="27" t="s">
-        <v>472</v>
-      </c>
-      <c r="C185" s="28" t="s">
-        <v>471</v>
-      </c>
-      <c r="D185" s="29">
-        <v>90</v>
-      </c>
-      <c r="E185" s="29">
-        <v>90</v>
-      </c>
-      <c r="F185" s="29">
-        <v>90</v>
-      </c>
-      <c r="G185" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H185" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I185" s="28" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -7409,19 +7415,19 @@
         <v>468</v>
       </c>
       <c r="B186" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C186" s="28" t="s">
         <v>471</v>
       </c>
       <c r="D186" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E186" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F186" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G186" s="27" t="s">
         <v>47</v>
@@ -7430,6 +7436,35 @@
         <v>59</v>
       </c>
       <c r="I186" s="28" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A187" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="B187" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="C187" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="D187" s="29">
+        <v>50</v>
+      </c>
+      <c r="E187" s="29">
+        <v>50</v>
+      </c>
+      <c r="F187" s="29">
+        <v>50</v>
+      </c>
+      <c r="G187" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H187" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I187" s="28" t="s">
         <v>470</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new parameter: car vs. pro
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686CADA0-9110-4AA3-80C2-126AF03213AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853A2132-9926-46DD-8D27-6806D484B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2028,7 +2028,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
parameter changes (project list: submitted)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F06AC0F-71AB-45AE-AAAA-F2BF6B1DC155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C47818C-3F83-4EEE-A69F-396E47238F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -1573,7 +1573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1671,6 +1671,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2027,8 +2030,8 @@
   <dimension ref="A1:I187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I186" sqref="I186"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6988,8 +6991,8 @@
       <c r="D171" s="12">
         <v>10</v>
       </c>
-      <c r="E171" s="12">
-        <v>10</v>
+      <c r="E171" s="35">
+        <v>80</v>
       </c>
       <c r="F171" s="12">
         <v>10</v>
@@ -7133,7 +7136,7 @@
       <c r="D176" s="12">
         <v>20</v>
       </c>
-      <c r="E176" s="12">
+      <c r="E176" s="35">
         <v>20</v>
       </c>
       <c r="F176" s="12">

</xml_diff>

<commit_message>
new approach for project delay
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C47818C-3F83-4EEE-A69F-396E47238F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932EEBE-CABF-4ED1-A565-D625FD43CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -2030,8 +2030,8 @@
   <dimension ref="A1:I187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E171" sqref="E171"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6931,13 +6931,13 @@
         <v>415</v>
       </c>
       <c r="D169" s="12">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="E169" s="12">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="F169" s="12">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="G169" s="11" t="s">
         <v>117</v>
@@ -6960,13 +6960,13 @@
         <v>418</v>
       </c>
       <c r="D170" s="12">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="E170" s="12">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="F170" s="12">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="G170" s="11" t="s">
         <v>117</v>
@@ -6982,7 +6982,7 @@
       <c r="A171" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="B171" s="11" t="s">
+      <c r="B171" s="32" t="s">
         <v>421</v>
       </c>
       <c r="C171" s="6" t="s">
@@ -7136,7 +7136,7 @@
       <c r="D176" s="12">
         <v>20</v>
       </c>
-      <c r="E176" s="35">
+      <c r="E176" s="12">
         <v>20</v>
       </c>
       <c r="F176" s="12">
@@ -7301,20 +7301,20 @@
       <c r="A182" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="B182" s="11" t="s">
+      <c r="B182" s="32" t="s">
         <v>461</v>
       </c>
       <c r="C182" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="D182" s="12">
-        <v>20</v>
-      </c>
-      <c r="E182" s="12">
-        <v>20</v>
-      </c>
-      <c r="F182" s="12">
-        <v>20</v>
+      <c r="D182" s="35">
+        <v>100</v>
+      </c>
+      <c r="E182" s="35">
+        <v>100</v>
+      </c>
+      <c r="F182" s="35">
+        <v>100</v>
       </c>
       <c r="G182" s="11" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
new output plots (district/origin), to search for error in origin distribution
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F4A08-4E30-4642-801B-0755DB2CF3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E959DDD-837B-4C1F-9066-D6E1C2644183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2031,7 +2031,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D170" sqref="D170"/>
+      <selection pane="bottomLeft" activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6988,14 +6988,14 @@
       <c r="C171" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="D171" s="12">
-        <v>10</v>
+      <c r="D171" s="35">
+        <v>80</v>
       </c>
       <c r="E171" s="35">
         <v>80</v>
       </c>
-      <c r="F171" s="12">
-        <v>10</v>
+      <c r="F171" s="35">
+        <v>80</v>
       </c>
       <c r="G171" s="11" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
back to 90:50, more origin checks
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF258CFA-C4B6-4A1F-83D2-ACF27281FD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008C5529-6D6B-45B5-88AA-EFBAA3A95395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2031,7 +2031,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A186" sqref="A186"/>
+      <selection pane="bottomLeft" activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7424,13 +7424,13 @@
         <v>469</v>
       </c>
       <c r="D186" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E186" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F186" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G186" s="27" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
after the prediction: new parameter (since smoothing with loess instead of gam)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271AF54D-E079-4D0B-9D1D-7D15110C0A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5C81DD-56F3-426D-9630-16D78663630E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="483">
   <si>
     <t>parameter</t>
   </si>
@@ -1461,6 +1461,12 @@
   </si>
   <si>
     <t>proportion of data points used in the loess regressions of fertility by age; groups: district, year, origin</t>
+  </si>
+  <si>
+    <t>bir_fer_span_pred</t>
+  </si>
+  <si>
+    <t>after the prediction: proportion of data points used in the loess regressions of fertility by age; groups: district, year, origin</t>
   </si>
 </sst>
 </file>
@@ -1603,7 +1609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1717,6 +1723,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2072,11 +2081,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I190"/>
+  <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3953,7 +3962,7 @@
       <c r="A65" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="41" t="s">
         <v>60</v>
       </c>
       <c r="C65" s="6" t="s">
@@ -3978,33 +3987,33 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>68</v>
+        <v>481</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D66" s="12">
-        <v>0</v>
-      </c>
-      <c r="E66" s="12">
-        <v>0</v>
-      </c>
-      <c r="F66" s="12">
-        <v>0</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>47</v>
+        <v>105</v>
+      </c>
+      <c r="D66" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E66" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="F66" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="H66" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I66" s="13" t="s">
-        <v>50</v>
+      <c r="I66" s="11" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4012,36 +4021,36 @@
         <v>20</v>
       </c>
       <c r="B67" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="12">
+        <v>0</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D67" s="12">
-        <v>20</v>
-      </c>
-      <c r="E67" s="12">
-        <v>20</v>
-      </c>
-      <c r="F67" s="12">
-        <v>20</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I67" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A68" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>105</v>
@@ -4059,39 +4068,39 @@
         <v>47</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="I68" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="12">
+        <v>20</v>
+      </c>
+      <c r="E69" s="12">
+        <v>20</v>
+      </c>
+      <c r="F69" s="12">
+        <v>20</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I69" s="13" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A69" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D69" s="12">
-        <v>13</v>
-      </c>
-      <c r="E69" s="12">
-        <v>13</v>
-      </c>
-      <c r="F69" s="12">
-        <v>13</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H69" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I69" s="13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4099,28 +4108,28 @@
         <v>20</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D70" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E70" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F70" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4128,19 +4137,19 @@
         <v>20</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D71" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E71" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F71" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>47</v>
@@ -4149,56 +4158,56 @@
         <v>59</v>
       </c>
       <c r="I71" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A72" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D72" s="12">
+        <v>100</v>
+      </c>
+      <c r="E72" s="12">
+        <v>100</v>
+      </c>
+      <c r="F72" s="12">
+        <v>100</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I72" s="13" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A72" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D72" s="16">
-        <v>30</v>
-      </c>
-      <c r="E72" s="14">
-        <v>30</v>
-      </c>
-      <c r="F72" s="14">
-        <v>30</v>
-      </c>
-      <c r="G72" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I72" s="15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D73" s="19">
-        <v>99</v>
-      </c>
-      <c r="E73" s="19">
-        <v>99</v>
-      </c>
-      <c r="F73" s="19">
-        <v>99</v>
+      <c r="B73" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" s="16">
+        <v>30</v>
+      </c>
+      <c r="E73" s="14">
+        <v>30</v>
+      </c>
+      <c r="F73" s="14">
+        <v>30</v>
       </c>
       <c r="G73" s="14" t="s">
         <v>99</v>
@@ -4207,27 +4216,27 @@
         <v>22</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B74" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>105</v>
+      <c r="B74" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="D74" s="19">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="E74" s="19">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F74" s="19">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="G74" s="14" t="s">
         <v>99</v>
@@ -4236,27 +4245,27 @@
         <v>22</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>105</v>
       </c>
       <c r="D75" s="19">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E75" s="19">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F75" s="19">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G75" s="14" t="s">
         <v>99</v>
@@ -4264,19 +4273,19 @@
       <c r="H75" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I75" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I75" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B76" s="17" t="s">
-        <v>114</v>
+      <c r="B76" s="38" t="s">
+        <v>106</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D76" s="19">
         <v>120</v>
@@ -4294,7 +4303,7 @@
         <v>22</v>
       </c>
       <c r="I76" s="20" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4302,28 +4311,28 @@
         <v>98</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D77" s="19">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="E77" s="19">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="F77" s="19">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I77" s="20" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -4331,19 +4340,19 @@
         <v>98</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>105</v>
       </c>
       <c r="D78" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E78" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F78" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G78" s="14" t="s">
         <v>91</v>
@@ -4352,76 +4361,76 @@
         <v>59</v>
       </c>
       <c r="I78" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B79" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" s="19">
+        <v>3</v>
+      </c>
+      <c r="E79" s="19">
+        <v>3</v>
+      </c>
+      <c r="F79" s="19">
+        <v>3</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I79" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C79" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D79" s="19">
+      <c r="C80" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D80" s="19">
         <v>0.8</v>
       </c>
-      <c r="E79" s="19">
+      <c r="E80" s="19">
         <v>0.8</v>
       </c>
-      <c r="F79" s="19">
+      <c r="F80" s="19">
         <v>0.8</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="G80" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="H79" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" s="20" t="s">
+      <c r="H80" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I80" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D80" s="12">
-        <v>20</v>
-      </c>
-      <c r="E80" s="12">
-        <v>20</v>
-      </c>
-      <c r="F80" s="12">
-        <v>20</v>
-      </c>
-      <c r="G80" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D81" s="12">
         <v>20</v>
@@ -4439,36 +4448,36 @@
         <v>22</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D82" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E82" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F82" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H82" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4476,28 +4485,28 @@
         <v>157</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="D83" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E83" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F83" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4505,39 +4514,39 @@
         <v>157</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="D84" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E84" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F84" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G84" s="11" t="s">
         <v>47</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D85" s="12">
         <v>20</v>
@@ -4555,36 +4564,36 @@
         <v>22</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D86" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E86" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F86" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H86" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4592,39 +4601,39 @@
         <v>157</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="D87" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E87" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F87" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B88" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>167</v>
+      <c r="B88" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="D88" s="12">
         <v>0</v>
@@ -4636,13 +4645,13 @@
         <v>0</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -4650,19 +4659,19 @@
         <v>157</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D89" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E89" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F89" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>99</v>
@@ -4671,36 +4680,36 @@
         <v>22</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B90" s="11" t="s">
-        <v>169</v>
+      <c r="B90" s="38" t="s">
+        <v>166</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="D90" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E90" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="F90" s="12">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4708,36 +4717,36 @@
         <v>157</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C91" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C91" s="13" t="s">
         <v>105</v>
       </c>
       <c r="D91" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E91" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F91" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>105</v>
@@ -4758,36 +4767,36 @@
         <v>22</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>157</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4795,68 +4804,68 @@
         <v>157</v>
       </c>
       <c r="B94" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D94" s="12">
+        <v>13</v>
+      </c>
+      <c r="E94" s="12">
+        <v>13</v>
+      </c>
+      <c r="F94" s="12">
+        <v>13</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D94" s="12">
-        <v>0</v>
-      </c>
-      <c r="E94" s="12">
-        <v>0</v>
-      </c>
-      <c r="F94" s="12">
-        <v>0</v>
-      </c>
-      <c r="G94" s="11" t="s">
+      <c r="C95" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D95" s="12">
+        <v>0</v>
+      </c>
+      <c r="E95" s="12">
+        <v>0</v>
+      </c>
+      <c r="F95" s="12">
+        <v>0</v>
+      </c>
+      <c r="G95" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H94" s="11" t="s">
+      <c r="H95" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="I95" s="13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="B95" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="D95" s="26">
-        <v>20</v>
-      </c>
-      <c r="E95" s="26">
-        <v>20</v>
-      </c>
-      <c r="F95" s="26">
-        <v>20</v>
-      </c>
-      <c r="G95" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H95" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I95" s="30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D96" s="26">
         <v>20</v>
@@ -4874,36 +4883,36 @@
         <v>22</v>
       </c>
       <c r="I96" s="30" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A97" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H97" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I97" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4911,28 +4920,28 @@
         <v>194</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>105</v>
+        <v>222</v>
       </c>
       <c r="D98" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E98" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F98" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H98" s="25" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>89</v>
+        <v>212</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4940,39 +4949,39 @@
         <v>194</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>223</v>
+        <v>105</v>
       </c>
       <c r="D99" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E99" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F99" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G99" s="25" t="s">
         <v>47</v>
       </c>
       <c r="H99" s="25" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D100" s="26">
         <v>20</v>
@@ -4990,36 +4999,36 @@
         <v>22</v>
       </c>
       <c r="I100" s="30" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A101" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="C101" s="31" t="s">
-        <v>225</v>
+        <v>200</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>224</v>
       </c>
       <c r="D101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H101" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5027,39 +5036,39 @@
         <v>194</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>105</v>
+        <v>201</v>
+      </c>
+      <c r="C102" s="31" t="s">
+        <v>225</v>
       </c>
       <c r="D102" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E102" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F102" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H102" s="25" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="B103" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="C103" s="30" t="s">
-        <v>226</v>
+      <c r="B103" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="D103" s="26">
         <v>0</v>
@@ -5071,13 +5080,13 @@
         <v>0</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="H103" s="25" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I103" s="30" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -5085,19 +5094,19 @@
         <v>194</v>
       </c>
       <c r="B104" s="38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G104" s="25" t="s">
         <v>99</v>
@@ -5106,36 +5115,36 @@
         <v>22</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="B105" s="25" t="s">
-        <v>205</v>
+      <c r="B105" s="38" t="s">
+        <v>204</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>105</v>
+        <v>227</v>
       </c>
       <c r="D105" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E105" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="F105" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="H105" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I105" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5143,36 +5152,36 @@
         <v>194</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="C106" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C106" s="30" t="s">
         <v>105</v>
       </c>
       <c r="D106" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E106" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F106" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H106" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A107" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>105</v>
@@ -5193,36 +5202,36 @@
         <v>22</v>
       </c>
       <c r="I107" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A108" s="25" t="s">
         <v>194</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>105</v>
       </c>
       <c r="D108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G108" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H108" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I108" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5230,86 +5239,86 @@
         <v>194</v>
       </c>
       <c r="B109" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D109" s="26">
+        <v>13</v>
+      </c>
+      <c r="E109" s="26">
+        <v>13</v>
+      </c>
+      <c r="F109" s="26">
+        <v>13</v>
+      </c>
+      <c r="G109" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H109" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I109" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A110" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="B110" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C109" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D109" s="26">
-        <v>0</v>
-      </c>
-      <c r="E109" s="26">
-        <v>0</v>
-      </c>
-      <c r="F109" s="26">
-        <v>0</v>
-      </c>
-      <c r="G109" s="25" t="s">
+      <c r="C110" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D110" s="26">
+        <v>0</v>
+      </c>
+      <c r="E110" s="26">
+        <v>0</v>
+      </c>
+      <c r="F110" s="26">
+        <v>0</v>
+      </c>
+      <c r="G110" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H109" s="25" t="s">
+      <c r="H110" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="I109" s="30" t="s">
+      <c r="I110" s="30" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D110" s="12">
-        <v>70</v>
-      </c>
-      <c r="E110" s="12">
-        <v>70</v>
-      </c>
-      <c r="F110" s="12">
-        <v>70</v>
-      </c>
-      <c r="G110" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H110" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I110" s="13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B111" s="11" t="s">
-        <v>254</v>
+      <c r="B111" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="D111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F111" s="6">
-        <v>0.2</v>
+        <v>233</v>
+      </c>
+      <c r="D111" s="12">
+        <v>70</v>
+      </c>
+      <c r="E111" s="12">
+        <v>70</v>
+      </c>
+      <c r="F111" s="12">
+        <v>70</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I111" s="11" t="s">
-        <v>240</v>
+        <v>22</v>
+      </c>
+      <c r="I111" s="13" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5317,7 +5326,7 @@
         <v>234</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>239</v>
@@ -5338,7 +5347,7 @@
         <v>64</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5346,19 +5355,19 @@
         <v>234</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>331</v>
+        <v>255</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>239</v>
       </c>
       <c r="D113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>91</v>
@@ -5367,7 +5376,7 @@
         <v>64</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>333</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5375,7 +5384,7 @@
         <v>234</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>239</v>
@@ -5396,7 +5405,7 @@
         <v>64</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5404,28 +5413,28 @@
         <v>234</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>244</v>
+        <v>91</v>
       </c>
       <c r="H115" s="11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5433,68 +5442,68 @@
         <v>234</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>256</v>
+        <v>335</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D116" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E116" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F116" s="6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>91</v>
+        <v>244</v>
       </c>
       <c r="H116" s="11" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
         <v>234</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="D117" s="12">
-        <v>20</v>
-      </c>
-      <c r="E117" s="12">
-        <v>20</v>
-      </c>
-      <c r="F117" s="12">
-        <v>20</v>
+        <v>239</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E117" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F117" s="6">
+        <v>0.3</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="H117" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I117" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="I117" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
         <v>234</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>105</v>
+        <v>250</v>
       </c>
       <c r="D118" s="12">
         <v>20</v>
@@ -5512,36 +5521,36 @@
         <v>22</v>
       </c>
       <c r="I118" s="13" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
         <v>234</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H119" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I119" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5549,28 +5558,28 @@
         <v>234</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D120" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E120" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F120" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G120" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I120" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5578,19 +5587,19 @@
         <v>234</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D121" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E121" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F121" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G121" s="11" t="s">
         <v>47</v>
@@ -5599,94 +5608,94 @@
         <v>59</v>
       </c>
       <c r="I121" s="13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>234</v>
       </c>
       <c r="B122" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D122" s="12">
+        <v>100</v>
+      </c>
+      <c r="E122" s="12">
+        <v>100</v>
+      </c>
+      <c r="F122" s="12">
+        <v>100</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H122" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I122" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B123" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="C123" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D123" s="6">
         <v>0.15</v>
       </c>
-      <c r="E122" s="6">
+      <c r="E123" s="6">
         <v>0.15</v>
       </c>
-      <c r="F122" s="6">
+      <c r="F123" s="6">
         <v>0.15</v>
       </c>
-      <c r="G122" s="11" t="s">
+      <c r="G123" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H122" s="11" t="s">
+      <c r="H123" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I122" s="11" t="s">
+      <c r="I123" s="11" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D123" s="29">
-        <v>70</v>
-      </c>
-      <c r="E123" s="29">
-        <v>70</v>
-      </c>
-      <c r="F123" s="29">
-        <v>70</v>
-      </c>
-      <c r="G123" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H123" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I123" s="28" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="B124" s="27" t="s">
-        <v>275</v>
+      <c r="B124" s="14" t="s">
+        <v>272</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="D124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F124" s="14">
-        <v>0.2</v>
+        <v>233</v>
+      </c>
+      <c r="D124" s="29">
+        <v>70</v>
+      </c>
+      <c r="E124" s="29">
+        <v>70</v>
+      </c>
+      <c r="F124" s="29">
+        <v>70</v>
       </c>
       <c r="G124" s="27" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="H124" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I124" s="27" t="s">
-        <v>274</v>
+        <v>22</v>
+      </c>
+      <c r="I124" s="28" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -5694,7 +5703,7 @@
         <v>263</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="C125" s="14" t="s">
         <v>239</v>
@@ -5715,7 +5724,7 @@
         <v>64</v>
       </c>
       <c r="I125" s="27" t="s">
-        <v>241</v>
+        <v>274</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -5723,19 +5732,19 @@
         <v>263</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>337</v>
+        <v>264</v>
       </c>
       <c r="C126" s="14" t="s">
         <v>239</v>
       </c>
       <c r="D126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G126" s="27" t="s">
         <v>91</v>
@@ -5744,7 +5753,7 @@
         <v>64</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>339</v>
+        <v>241</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -5752,7 +5761,7 @@
         <v>263</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C127" s="14" t="s">
         <v>239</v>
@@ -5773,7 +5782,7 @@
         <v>64</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -5781,28 +5790,28 @@
         <v>263</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>244</v>
+        <v>91</v>
       </c>
       <c r="H128" s="27" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5810,68 +5819,68 @@
         <v>263</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>265</v>
+        <v>340</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D129" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="E129" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F129" s="14">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G129" s="27" t="s">
-        <v>91</v>
+        <v>244</v>
       </c>
       <c r="H129" s="27" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
         <v>263</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="D130" s="29">
-        <v>20</v>
-      </c>
-      <c r="E130" s="29">
-        <v>20</v>
-      </c>
-      <c r="F130" s="29">
-        <v>20</v>
+        <v>239</v>
+      </c>
+      <c r="D130" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="E130" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F130" s="14">
+        <v>0.3</v>
       </c>
       <c r="G130" s="27" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="H130" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I130" s="28" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="I130" s="27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
         <v>263</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>105</v>
+        <v>250</v>
       </c>
       <c r="D131" s="29">
         <v>20</v>
@@ -5889,36 +5898,36 @@
         <v>22</v>
       </c>
       <c r="I131" s="28" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
         <v>263</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C132" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G132" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H132" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I132" s="28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5926,28 +5935,28 @@
         <v>263</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C133" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D133" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E133" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F133" s="29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G133" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H133" s="27" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I133" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5955,19 +5964,19 @@
         <v>263</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C134" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D134" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E134" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F134" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G134" s="27" t="s">
         <v>47</v>
@@ -5976,65 +5985,65 @@
         <v>59</v>
       </c>
       <c r="I134" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="27" t="s">
         <v>263</v>
       </c>
       <c r="B135" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D135" s="29">
+        <v>100</v>
+      </c>
+      <c r="E135" s="29">
+        <v>100</v>
+      </c>
+      <c r="F135" s="29">
+        <v>100</v>
+      </c>
+      <c r="G135" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H135" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I135" s="28" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A136" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="B136" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="C135" s="14" t="s">
+      <c r="C136" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="D135" s="14">
+      <c r="D136" s="14">
         <v>0.15</v>
       </c>
-      <c r="E135" s="14">
+      <c r="E136" s="14">
         <v>0.15</v>
       </c>
-      <c r="F135" s="14">
+      <c r="F136" s="14">
         <v>0.15</v>
       </c>
-      <c r="G135" s="27" t="s">
+      <c r="G136" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="H135" s="27" t="s">
+      <c r="H136" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="I135" s="27" t="s">
+      <c r="I136" s="27" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A136" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="B136" s="40" t="s">
-        <v>292</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="D136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="G136" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H136" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I136" s="11" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -6042,19 +6051,19 @@
         <v>289</v>
       </c>
       <c r="B137" s="40" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C137" s="6" t="s">
         <v>290</v>
       </c>
       <c r="D137" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E137" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F137" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G137" s="11" t="s">
         <v>91</v>
@@ -6063,36 +6072,36 @@
         <v>22</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="B138" s="11" t="s">
-        <v>294</v>
+      <c r="B138" s="40" t="s">
+        <v>293</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D138" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="E138" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="F138" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="H138" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -6100,28 +6109,28 @@
         <v>289</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>105</v>
+        <v>296</v>
       </c>
       <c r="D139" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E139" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F139" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>297</v>
+        <v>33</v>
       </c>
       <c r="H139" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -6129,28 +6138,28 @@
         <v>289</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>290</v>
+        <v>105</v>
       </c>
       <c r="D140" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E140" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F140" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>91</v>
+        <v>297</v>
       </c>
       <c r="H140" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -6158,7 +6167,7 @@
         <v>289</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C141" s="6" t="s">
         <v>290</v>
@@ -6179,7 +6188,7 @@
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6187,19 +6196,19 @@
         <v>289</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>290</v>
       </c>
       <c r="D142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G142" s="11" t="s">
         <v>91</v>
@@ -6208,7 +6217,7 @@
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6216,19 +6225,19 @@
         <v>289</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>290</v>
       </c>
       <c r="D143" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E143" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="F143" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G143" s="11" t="s">
         <v>91</v>
@@ -6237,7 +6246,7 @@
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6245,28 +6254,28 @@
         <v>289</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="D144" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E144" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="F144" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G144" s="11" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="H144" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6274,10 +6283,10 @@
         <v>289</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>105</v>
+        <v>310</v>
       </c>
       <c r="D145" s="6">
         <v>20</v>
@@ -6295,7 +6304,7 @@
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -6303,28 +6312,28 @@
         <v>289</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H146" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6332,28 +6341,28 @@
         <v>289</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D147" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E147" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F147" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G147" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H147" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -6361,28 +6370,28 @@
         <v>289</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>290</v>
+        <v>105</v>
       </c>
       <c r="D148" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E148" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F148" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G148" s="11" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="H148" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6390,19 +6399,19 @@
         <v>289</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>290</v>
       </c>
       <c r="D149" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E149" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F149" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G149" s="11" t="s">
         <v>91</v>
@@ -6411,7 +6420,7 @@
         <v>22</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -6419,19 +6428,19 @@
         <v>289</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>290</v>
       </c>
       <c r="D150" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E150" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="F150" s="6">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G150" s="11" t="s">
         <v>91</v>
@@ -6440,7 +6449,7 @@
         <v>22</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -6448,28 +6457,28 @@
         <v>289</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>105</v>
+        <v>290</v>
       </c>
       <c r="D151" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E151" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F151" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>326</v>
+        <v>91</v>
       </c>
       <c r="H151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -6477,28 +6486,28 @@
         <v>289</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C152" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D152" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E152" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F152" s="6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G152" s="11" t="s">
-        <v>91</v>
+        <v>326</v>
       </c>
       <c r="H152" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -6506,19 +6515,19 @@
         <v>289</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>290</v>
+        <v>105</v>
       </c>
       <c r="D153" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E153" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F153" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G153" s="11" t="s">
         <v>91</v>
@@ -6527,53 +6536,53 @@
         <v>22</v>
       </c>
       <c r="I153" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D154" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E154" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="F154" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G154" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H154" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I154" s="11" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="B154" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="C154" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="D154" s="29">
-        <v>25</v>
-      </c>
-      <c r="E154" s="29">
-        <v>25</v>
-      </c>
-      <c r="F154" s="29">
-        <v>25</v>
-      </c>
-      <c r="G154" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H154" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="I154" s="28" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="27" t="s">
         <v>341</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D155" s="29">
-        <v>-25</v>
+        <v>25</v>
       </c>
       <c r="E155" s="29">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F155" s="29">
         <v>25</v>
@@ -6582,30 +6591,30 @@
         <v>47</v>
       </c>
       <c r="H155" s="27" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="I155" s="28" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A156" s="27" t="s">
         <v>341</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D156" s="29">
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="E156" s="29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F156" s="29">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G156" s="27" t="s">
         <v>47</v>
@@ -6614,27 +6623,27 @@
         <v>49</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
         <v>341</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>105</v>
+        <v>345</v>
       </c>
       <c r="D157" s="29">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="E157" s="29">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F157" s="29">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="G157" s="27" t="s">
         <v>47</v>
@@ -6643,7 +6652,7 @@
         <v>49</v>
       </c>
       <c r="I157" s="28" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -6651,19 +6660,19 @@
         <v>341</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>346</v>
+        <v>105</v>
       </c>
       <c r="D158" s="29">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E158" s="29">
         <v>85</v>
       </c>
       <c r="F158" s="29">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G158" s="27" t="s">
         <v>47</v>
@@ -6672,7 +6681,7 @@
         <v>49</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -6680,28 +6689,28 @@
         <v>341</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D159" s="29">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F159" s="29">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G159" s="27" t="s">
-        <v>356</v>
+        <v>47</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="I159" s="28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6709,126 +6718,126 @@
         <v>341</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D160" s="29">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="E160" s="29">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="F160" s="29">
-        <v>2044</v>
+        <v>0</v>
       </c>
       <c r="G160" s="27" t="s">
-        <v>34</v>
+        <v>356</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I160" s="28" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="27" t="s">
         <v>341</v>
       </c>
       <c r="B161" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="C161" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="D161" s="29">
+        <v>2044</v>
+      </c>
+      <c r="E161" s="29">
+        <v>2044</v>
+      </c>
+      <c r="F161" s="29">
+        <v>2044</v>
+      </c>
+      <c r="G161" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H161" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I161" s="28" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A162" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="B162" s="27" t="s">
         <v>353</v>
       </c>
-      <c r="C161" s="14" t="s">
+      <c r="C162" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="D161" s="29">
+      <c r="D162" s="29">
         <v>-0.04</v>
       </c>
-      <c r="E161" s="29">
+      <c r="E162" s="29">
         <v>-0.04</v>
       </c>
-      <c r="F161" s="29">
+      <c r="F162" s="29">
         <v>-0.04</v>
       </c>
-      <c r="G161" s="27" t="s">
+      <c r="G162" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="H161" s="27" t="s">
+      <c r="H162" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="I161" s="28" t="s">
+      <c r="I162" s="28" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A162" s="11" t="s">
-        <v>374</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>375</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="D162" s="6">
-        <v>500</v>
-      </c>
-      <c r="E162" s="6">
-        <v>500</v>
-      </c>
-      <c r="F162" s="6">
-        <v>500</v>
-      </c>
-      <c r="G162" s="11" t="s">
-        <v>377</v>
-      </c>
-      <c r="H162" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I162" s="11" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
         <v>374</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="D163" s="12">
-        <v>20</v>
-      </c>
-      <c r="E163" s="12">
-        <v>20</v>
-      </c>
-      <c r="F163" s="12">
-        <v>20</v>
+        <v>376</v>
+      </c>
+      <c r="D163" s="6">
+        <v>500</v>
+      </c>
+      <c r="E163" s="6">
+        <v>500</v>
+      </c>
+      <c r="F163" s="6">
+        <v>500</v>
       </c>
       <c r="G163" s="11" t="s">
-        <v>47</v>
+        <v>377</v>
       </c>
       <c r="H163" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I163" s="13" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I163" s="11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
         <v>374</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D164" s="12">
         <v>20</v>
@@ -6846,36 +6855,36 @@
         <v>22</v>
       </c>
       <c r="I164" s="13" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
         <v>374</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G165" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H165" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I165" s="13" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -6883,97 +6892,97 @@
         <v>374</v>
       </c>
       <c r="B166" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="D166" s="12">
+        <v>7</v>
+      </c>
+      <c r="E166" s="12">
+        <v>7</v>
+      </c>
+      <c r="F166" s="12">
+        <v>7</v>
+      </c>
+      <c r="G166" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H166" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I166" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A167" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="B167" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="C166" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D166" s="12">
-        <v>0</v>
-      </c>
-      <c r="E166" s="12">
-        <v>0</v>
-      </c>
-      <c r="F166" s="12">
-        <v>0</v>
-      </c>
-      <c r="G166" s="11" t="s">
+      <c r="C167" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D167" s="12">
+        <v>0</v>
+      </c>
+      <c r="E167" s="12">
+        <v>0</v>
+      </c>
+      <c r="F167" s="12">
+        <v>0</v>
+      </c>
+      <c r="G167" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H166" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I166" s="13" t="s">
+      <c r="H167" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I167" s="13" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="167" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="B167" s="25" t="s">
-        <v>392</v>
-      </c>
-      <c r="C167" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="D167" s="10">
-        <v>500</v>
-      </c>
-      <c r="E167" s="10">
-        <v>500</v>
-      </c>
-      <c r="F167" s="10">
-        <v>500</v>
-      </c>
-      <c r="G167" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="H167" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I167" s="25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="25" t="s">
         <v>390</v>
       </c>
       <c r="B168" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="D168" s="26">
-        <v>20</v>
-      </c>
-      <c r="E168" s="26">
-        <v>20</v>
-      </c>
-      <c r="F168" s="26">
-        <v>20</v>
+        <v>391</v>
+      </c>
+      <c r="D168" s="10">
+        <v>500</v>
+      </c>
+      <c r="E168" s="10">
+        <v>500</v>
+      </c>
+      <c r="F168" s="10">
+        <v>500</v>
       </c>
       <c r="G168" s="25" t="s">
-        <v>47</v>
+        <v>377</v>
       </c>
       <c r="H168" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I168" s="30" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I168" s="25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
         <v>390</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D169" s="26">
         <v>20</v>
@@ -6991,36 +7000,36 @@
         <v>22</v>
       </c>
       <c r="I169" s="30" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A170" s="25" t="s">
         <v>390</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G170" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H170" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I170" s="30" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7028,57 +7037,57 @@
         <v>390</v>
       </c>
       <c r="B171" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="C171" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="D171" s="26">
+        <v>7</v>
+      </c>
+      <c r="E171" s="26">
+        <v>7</v>
+      </c>
+      <c r="F171" s="26">
+        <v>7</v>
+      </c>
+      <c r="G171" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="H171" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I171" s="30" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A172" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="B172" s="25" t="s">
         <v>409</v>
       </c>
-      <c r="C171" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D171" s="26">
-        <v>0</v>
-      </c>
-      <c r="E171" s="26">
-        <v>0</v>
-      </c>
-      <c r="F171" s="26">
-        <v>0</v>
-      </c>
-      <c r="G171" s="25" t="s">
+      <c r="C172" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D172" s="26">
+        <v>0</v>
+      </c>
+      <c r="E172" s="26">
+        <v>0</v>
+      </c>
+      <c r="F172" s="26">
+        <v>0</v>
+      </c>
+      <c r="G172" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H171" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I171" s="30" t="s">
+      <c r="H172" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I172" s="30" t="s">
         <v>410</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A172" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>414</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="D172" s="12">
-        <v>2</v>
-      </c>
-      <c r="E172" s="12">
-        <v>2</v>
-      </c>
-      <c r="F172" s="12">
-        <v>2</v>
-      </c>
-      <c r="G172" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H172" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I172" s="13" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -7086,19 +7095,19 @@
         <v>413</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D173" s="12">
-        <v>0.05</v>
+        <v>2</v>
       </c>
       <c r="E173" s="12">
-        <v>0.05</v>
+        <v>2</v>
       </c>
       <c r="F173" s="12">
-        <v>0.05</v>
+        <v>2</v>
       </c>
       <c r="G173" s="11" t="s">
         <v>117</v>
@@ -7107,36 +7116,36 @@
         <v>22</v>
       </c>
       <c r="I173" s="13" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
         <v>413</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="D174" s="39">
-        <v>80</v>
-      </c>
-      <c r="E174" s="39">
-        <v>80</v>
-      </c>
-      <c r="F174" s="39">
-        <v>80</v>
+        <v>418</v>
+      </c>
+      <c r="D174" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="E174" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="F174" s="12">
+        <v>0.05</v>
       </c>
       <c r="G174" s="11" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="H174" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I174" s="13" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
@@ -7144,19 +7153,19 @@
         <v>413</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="D175" s="12">
-        <v>0</v>
-      </c>
-      <c r="E175" s="12">
-        <v>0</v>
-      </c>
-      <c r="F175" s="12">
-        <v>0</v>
+        <v>420</v>
+      </c>
+      <c r="D175" s="39">
+        <v>80</v>
+      </c>
+      <c r="E175" s="39">
+        <v>80</v>
+      </c>
+      <c r="F175" s="39">
+        <v>80</v>
       </c>
       <c r="G175" s="11" t="s">
         <v>47</v>
@@ -7173,10 +7182,10 @@
         <v>413</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D176" s="12">
         <v>0</v>
@@ -7202,10 +7211,10 @@
         <v>413</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D177" s="12">
         <v>0</v>
@@ -7231,10 +7240,10 @@
         <v>413</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D178" s="12">
         <v>0</v>
@@ -7260,19 +7269,19 @@
         <v>413</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G179" s="11" t="s">
         <v>47</v>
@@ -7284,53 +7293,53 @@
         <v>432</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A180" s="27" t="s">
-        <v>441</v>
-      </c>
-      <c r="B180" s="27" t="s">
-        <v>442</v>
-      </c>
-      <c r="C180" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="D180" s="29">
-        <v>50</v>
-      </c>
-      <c r="E180" s="29">
-        <v>50</v>
-      </c>
-      <c r="F180" s="29">
-        <v>50</v>
-      </c>
-      <c r="G180" s="27" t="s">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A180" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="B180" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="D180" s="12">
+        <v>20</v>
+      </c>
+      <c r="E180" s="12">
+        <v>20</v>
+      </c>
+      <c r="F180" s="12">
+        <v>20</v>
+      </c>
+      <c r="G180" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H180" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I180" s="28" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="H180" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I180" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A181" s="27" t="s">
         <v>441</v>
       </c>
       <c r="B181" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D181" s="29">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E181" s="29">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F181" s="29">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G181" s="27" t="s">
         <v>47</v>
@@ -7339,36 +7348,36 @@
         <v>22</v>
       </c>
       <c r="I181" s="28" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A182" s="27" t="s">
         <v>441</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D182" s="29">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E182" s="29">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F182" s="29">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G182" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H182" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I182" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -7376,28 +7385,28 @@
         <v>441</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>105</v>
+        <v>449</v>
       </c>
       <c r="D183" s="29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E183" s="29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F183" s="29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G183" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H183" s="27" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="I183" s="28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -7405,19 +7414,19 @@
         <v>441</v>
       </c>
       <c r="B184" s="27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C184" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D184" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E184" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F184" s="29">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G184" s="27" t="s">
         <v>47</v>
@@ -7426,36 +7435,36 @@
         <v>59</v>
       </c>
       <c r="I184" s="28" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A185" s="27" t="s">
+        <v>441</v>
+      </c>
+      <c r="B185" s="27" t="s">
+        <v>446</v>
+      </c>
+      <c r="C185" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D185" s="29">
+        <v>100</v>
+      </c>
+      <c r="E185" s="29">
+        <v>100</v>
+      </c>
+      <c r="F185" s="29">
+        <v>100</v>
+      </c>
+      <c r="G185" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H185" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I185" s="28" t="s">
         <v>454</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A185" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="B185" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="C185" s="6" t="s">
-        <v>460</v>
-      </c>
-      <c r="D185" s="39">
-        <v>100</v>
-      </c>
-      <c r="E185" s="39">
-        <v>100</v>
-      </c>
-      <c r="F185" s="39">
-        <v>100</v>
-      </c>
-      <c r="G185" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H185" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I185" s="13" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -7463,57 +7472,57 @@
         <v>459</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D186" s="12">
-        <v>80</v>
-      </c>
-      <c r="E186" s="12">
-        <v>80</v>
-      </c>
-      <c r="F186" s="12">
-        <v>80</v>
+        <v>460</v>
+      </c>
+      <c r="D186" s="39">
+        <v>100</v>
+      </c>
+      <c r="E186" s="39">
+        <v>100</v>
+      </c>
+      <c r="F186" s="39">
+        <v>100</v>
       </c>
       <c r="G186" s="11" t="s">
         <v>47</v>
       </c>
       <c r="H186" s="11" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="I186" s="13" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
         <v>459</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>464</v>
+        <v>105</v>
       </c>
       <c r="D187" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E187" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F187" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G187" s="11" t="s">
         <v>47</v>
       </c>
       <c r="H187" s="11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="I187" s="13" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -7521,7 +7530,7 @@
         <v>459</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C188" s="6" t="s">
         <v>464</v>
@@ -7542,36 +7551,36 @@
         <v>22</v>
       </c>
       <c r="I188" s="13" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B189" s="11" t="s">
+        <v>465</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="D189" s="12">
+        <v>0</v>
+      </c>
+      <c r="E189" s="12">
+        <v>0</v>
+      </c>
+      <c r="F189" s="12">
+        <v>0</v>
+      </c>
+      <c r="G189" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H189" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I189" s="13" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A189" s="27" t="s">
-        <v>468</v>
-      </c>
-      <c r="B189" s="27" t="s">
-        <v>470</v>
-      </c>
-      <c r="C189" s="28" t="s">
-        <v>469</v>
-      </c>
-      <c r="D189" s="29">
-        <v>90</v>
-      </c>
-      <c r="E189" s="29">
-        <v>90</v>
-      </c>
-      <c r="F189" s="29">
-        <v>90</v>
-      </c>
-      <c r="G189" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H189" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I189" s="28" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -7579,19 +7588,19 @@
         <v>468</v>
       </c>
       <c r="B190" s="27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C190" s="28" t="s">
         <v>469</v>
       </c>
       <c r="D190" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E190" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F190" s="29">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G190" s="27" t="s">
         <v>47</v>
@@ -7600,6 +7609,35 @@
         <v>59</v>
       </c>
       <c r="I190" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A191" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="B191" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="C191" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="D191" s="29">
+        <v>50</v>
+      </c>
+      <c r="E191" s="29">
+        <v>50</v>
+      </c>
+      <c r="F191" s="29">
+        <v>50</v>
+      </c>
+      <c r="G191" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="H191" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I191" s="28" t="s">
         <v>475</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new parameter (smoothing with loess instead of gam)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5C81DD-56F3-426D-9630-16D78663630E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F835DF53-BBC1-407F-8C46-C9C59559A43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1609,7 +1609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1723,9 +1723,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2085,7 +2082,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3962,7 +3959,7 @@
       <c r="A65" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C65" s="6" t="s">

</xml_diff>

<commit_message>
new parameter (loess instead of gam)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F835DF53-BBC1-407F-8C46-C9C59559A43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8BA49F-1D67-46B3-8E36-831A51B6A3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2081,8 +2081,8 @@
   <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
remove redundant parameters (dea_age...)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8BA49F-1D67-46B3-8E36-831A51B6A3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7ADAC0-84A0-4730-BD98-FA89A6E00821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2081,8 +2081,8 @@
   <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new parameters, new documentation
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7ADAC0-84A0-4730-BD98-FA89A6E00821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">parameter!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
@@ -1472,7 +1474,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1728,7 +1730,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1832,23 +1834,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1884,23 +1869,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2076,13 +2044,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2095,7 +2063,7 @@
     <col min="6" max="6" width="6.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="21" customWidth="1"/>
     <col min="8" max="8" width="19" style="21" customWidth="1"/>
-    <col min="9" max="9" width="75.5703125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="89.7109375" style="24" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
@@ -2476,7 +2444,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
@@ -2505,7 +2473,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
@@ -2534,7 +2502,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>19</v>
       </c>
@@ -2563,7 +2531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>19</v>
       </c>
@@ -2592,7 +2560,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
@@ -2621,7 +2589,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>19</v>
       </c>
@@ -2650,7 +2618,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
@@ -2679,7 +2647,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
@@ -2708,7 +2676,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
@@ -2737,7 +2705,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>19</v>
       </c>
@@ -2766,7 +2734,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>19</v>
       </c>
@@ -2795,7 +2763,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>19</v>
       </c>
@@ -2824,7 +2792,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>19</v>
       </c>
@@ -2853,7 +2821,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>19</v>
       </c>
@@ -2882,7 +2850,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>19</v>
       </c>
@@ -2911,7 +2879,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>19</v>
       </c>
@@ -2940,7 +2908,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>19</v>
       </c>
@@ -2969,7 +2937,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
@@ -2998,7 +2966,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>19</v>
       </c>
@@ -3027,7 +2995,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
@@ -3056,7 +3024,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>19</v>
       </c>
@@ -3085,7 +3053,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>19</v>
       </c>
@@ -3114,7 +3082,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>19</v>
       </c>
@@ -3143,7 +3111,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>19</v>
       </c>
@@ -3172,7 +3140,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" s="9" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
@@ -3201,7 +3169,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>19</v>
       </c>
@@ -3230,7 +3198,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>19</v>
       </c>
@@ -3259,7 +3227,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" s="9" customFormat="1" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>19</v>
       </c>
@@ -3288,7 +3256,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>19</v>
       </c>
@@ -3317,7 +3285,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>19</v>
       </c>
@@ -3346,7 +3314,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
@@ -3375,7 +3343,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>19</v>
       </c>
@@ -7640,7 +7608,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="65" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
parameter change (last value of FSO data: 2020 instead of 2019)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -2050,8 +2050,8 @@
   <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2484,14 +2484,14 @@
       <c r="C15" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="10">
-        <v>2019</v>
-      </c>
-      <c r="E15" s="10">
-        <v>2019</v>
-      </c>
-      <c r="F15" s="10">
-        <v>2019</v>
+      <c r="D15" s="34">
+        <v>2020</v>
+      </c>
+      <c r="E15" s="34">
+        <v>2020</v>
+      </c>
+      <c r="F15" s="34">
+        <v>2020</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
base years for mortality rate ratio (Zurich vs. Switzerland): 2010 until 2020
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -307,12 +307,6 @@
     <t>tod.alt.alter.ende</t>
   </si>
   <si>
-    <t>base period (in the past) for death rate, begin</t>
-  </si>
-  <si>
-    <t>base period (in the past) for death rate, end</t>
-  </si>
-  <si>
     <t>no parameter in previous model</t>
   </si>
   <si>
@@ -1469,6 +1463,12 @@
   </si>
   <si>
     <t>Category in the FSO data: (smoothed) data of the past</t>
+  </si>
+  <si>
+    <t>base period (in the past) for death rate, end (data should be available for both Zurich and Switzerland)</t>
+  </si>
+  <si>
+    <t>base period (in the past) for death rate, begin (data should be available for both Zurich and Switzerland)</t>
   </si>
 </sst>
 </file>
@@ -2063,7 +2063,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2094,7 +2094,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -2106,7 +2106,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2172,7 +2172,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>50</v>
@@ -2201,7 +2201,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>51</v>
@@ -2349,7 +2349,7 @@
         <v>63</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D10" s="10">
         <v>2007</v>
@@ -2378,7 +2378,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D11" s="35">
         <v>2021</v>
@@ -2407,7 +2407,7 @@
         <v>65</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D12" s="10">
         <v>1993</v>
@@ -2436,7 +2436,7 @@
         <v>66</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D13" s="35">
         <v>2021</v>
@@ -2462,10 +2462,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="10">
         <v>1993</v>
@@ -2483,7 +2483,7 @@
         <v>22</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2491,10 +2491,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15" s="34">
         <v>2020</v>
@@ -2512,7 +2512,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2525,14 +2525,14 @@
       <c r="C16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="10">
-        <v>2014</v>
-      </c>
-      <c r="E16" s="10">
-        <v>2014</v>
-      </c>
-      <c r="F16" s="10">
-        <v>2014</v>
+      <c r="D16" s="41">
+        <v>2010</v>
+      </c>
+      <c r="E16" s="41">
+        <v>2010</v>
+      </c>
+      <c r="F16" s="41">
+        <v>2010</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>34</v>
@@ -2541,7 +2541,7 @@
         <v>22</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>96</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2570,7 +2570,7 @@
         <v>22</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>97</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2578,10 +2578,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D18" s="10">
         <v>2010</v>
@@ -2599,7 +2599,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2607,10 +2607,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D19" s="35">
         <v>2021</v>
@@ -2628,7 +2628,7 @@
         <v>22</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2636,10 +2636,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20" s="10">
         <v>2010</v>
@@ -2657,7 +2657,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2665,10 +2665,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="35">
         <v>2021</v>
@@ -2686,7 +2686,7 @@
         <v>22</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2694,10 +2694,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D22" s="10">
         <v>2010</v>
@@ -2715,7 +2715,7 @@
         <v>22</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2723,10 +2723,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D23" s="35">
         <v>2021</v>
@@ -2744,7 +2744,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2752,10 +2752,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24" s="10">
         <v>2010</v>
@@ -2773,7 +2773,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2781,10 +2781,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D25" s="35">
         <v>2021</v>
@@ -2802,7 +2802,7 @@
         <v>22</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2810,10 +2810,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D26" s="10">
         <v>2010</v>
@@ -2831,7 +2831,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2839,10 +2839,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D27" s="35">
         <v>2021</v>
@@ -2860,7 +2860,7 @@
         <v>22</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2868,10 +2868,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D28" s="10">
         <v>2010</v>
@@ -2889,7 +2889,7 @@
         <v>22</v>
       </c>
       <c r="I28" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2897,10 +2897,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D29" s="35">
         <v>2021</v>
@@ -2918,7 +2918,7 @@
         <v>22</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2926,10 +2926,10 @@
         <v>19</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D30" s="10">
         <v>2005</v>
@@ -2947,7 +2947,7 @@
         <v>22</v>
       </c>
       <c r="I30" s="31" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2955,10 +2955,10 @@
         <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D31" s="37">
         <v>2019</v>
@@ -2976,7 +2976,7 @@
         <v>22</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2984,10 +2984,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D32" s="10">
         <v>2005</v>
@@ -3005,7 +3005,7 @@
         <v>22</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3013,10 +3013,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D33" s="37">
         <v>2019</v>
@@ -3034,7 +3034,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3042,10 +3042,10 @@
         <v>19</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D34" s="10">
         <v>2011</v>
@@ -3063,7 +3063,7 @@
         <v>22</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3071,10 +3071,10 @@
         <v>19</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D35" s="35">
         <v>2021</v>
@@ -3092,7 +3092,7 @@
         <v>22</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3100,10 +3100,10 @@
         <v>19</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D36" s="10">
         <v>2011</v>
@@ -3121,7 +3121,7 @@
         <v>22</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3129,10 +3129,10 @@
         <v>19</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D37" s="35">
         <v>2021</v>
@@ -3150,7 +3150,7 @@
         <v>22</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3158,10 +3158,10 @@
         <v>19</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" s="10">
         <v>2015</v>
@@ -3179,7 +3179,7 @@
         <v>22</v>
       </c>
       <c r="I38" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3187,10 +3187,10 @@
         <v>19</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D39" s="10">
         <v>2011</v>
@@ -3208,7 +3208,7 @@
         <v>22</v>
       </c>
       <c r="I39" s="31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3216,10 +3216,10 @@
         <v>19</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40" s="35">
         <v>2021</v>
@@ -3237,7 +3237,7 @@
         <v>22</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3245,10 +3245,10 @@
         <v>19</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D41" s="10">
         <v>2015</v>
@@ -3266,7 +3266,7 @@
         <v>22</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3274,10 +3274,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>423</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>425</v>
       </c>
       <c r="D42" s="34">
         <v>2022</v>
@@ -3295,7 +3295,7 @@
         <v>22</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3303,10 +3303,10 @@
         <v>19</v>
       </c>
       <c r="B43" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>424</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>426</v>
       </c>
       <c r="D43" s="34">
         <v>2029</v>
@@ -3324,7 +3324,7 @@
         <v>22</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3332,10 +3332,10 @@
         <v>19</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D44" s="10">
         <v>2015</v>
@@ -3353,7 +3353,7 @@
         <v>22</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3361,10 +3361,10 @@
         <v>19</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D45" s="35">
         <v>2021</v>
@@ -3382,18 +3382,18 @@
         <v>22</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D46" s="12">
         <v>0</v>
@@ -3411,18 +3411,18 @@
         <v>22</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D47" s="12">
         <v>120</v>
@@ -3440,7 +3440,7 @@
         <v>22</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3451,7 +3451,7 @@
         <v>70</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" s="29">
         <v>4</v>
@@ -3463,13 +3463,13 @@
         <v>4</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H48" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I48" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3477,10 +3477,10 @@
         <v>61</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D49" s="29">
         <v>4</v>
@@ -3492,13 +3492,13 @@
         <v>4</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H49" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I49" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3506,10 +3506,10 @@
         <v>61</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D50" s="29">
         <v>4</v>
@@ -3521,13 +3521,13 @@
         <v>4</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H50" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3535,10 +3535,10 @@
         <v>61</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D51" s="26">
         <v>0</v>
@@ -3550,13 +3550,13 @@
         <v>0</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H51" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3564,10 +3564,10 @@
         <v>61</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D52" s="29">
         <v>4</v>
@@ -3579,13 +3579,13 @@
         <v>4</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H52" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3672,7 +3672,7 @@
         <v>22</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3701,7 +3701,7 @@
         <v>22</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -3730,7 +3730,7 @@
         <v>22</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3767,10 +3767,10 @@
         <v>20</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D59" s="6">
         <v>0.3</v>
@@ -3788,7 +3788,7 @@
         <v>22</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3886,7 +3886,7 @@
         <v>78</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D63" s="12">
         <v>0</v>
@@ -3898,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>22</v>
@@ -3915,7 +3915,7 @@
         <v>80</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>81</v>
@@ -3927,7 +3927,7 @@
         <v>81</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>22</v>
@@ -3944,7 +3944,7 @@
         <v>57</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D65" s="12">
         <v>30</v>
@@ -3956,7 +3956,7 @@
         <v>30</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H65" s="11" t="s">
         <v>56</v>
@@ -3970,10 +3970,10 @@
         <v>20</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D66" s="6">
         <v>0.15</v>
@@ -3991,7 +3991,7 @@
         <v>22</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4031,7 +4031,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D68" s="12">
         <v>20</v>
@@ -4060,7 +4060,7 @@
         <v>73</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D69" s="12">
         <v>20</v>
@@ -4089,7 +4089,7 @@
         <v>74</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D70" s="12">
         <v>13</v>
@@ -4118,7 +4118,7 @@
         <v>79</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D71" s="12">
         <v>0</v>
@@ -4136,7 +4136,7 @@
         <v>22</v>
       </c>
       <c r="I71" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4147,7 +4147,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D72" s="12">
         <v>100</v>
@@ -4165,7 +4165,7 @@
         <v>22</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4173,10 +4173,10 @@
         <v>93</v>
       </c>
       <c r="B73" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C73" s="14" t="s">
         <v>100</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>102</v>
       </c>
       <c r="D73" s="16">
         <v>30</v>
@@ -4194,7 +4194,7 @@
         <v>22</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4202,10 +4202,10 @@
         <v>93</v>
       </c>
       <c r="B74" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="D74" s="19">
         <v>99</v>
@@ -4223,7 +4223,7 @@
         <v>22</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -4231,7 +4231,7 @@
         <v>93</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>95</v>
@@ -4252,7 +4252,7 @@
         <v>22</v>
       </c>
       <c r="I75" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -4260,10 +4260,10 @@
         <v>93</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D76" s="19">
         <v>2</v>
@@ -4281,7 +4281,7 @@
         <v>56</v>
       </c>
       <c r="I76" s="20" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4289,10 +4289,10 @@
         <v>93</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D77" s="19">
         <v>3</v>
@@ -4310,7 +4310,7 @@
         <v>56</v>
       </c>
       <c r="I77" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4318,10 +4318,10 @@
         <v>93</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D78" s="19">
         <v>0.8</v>
@@ -4333,13 +4333,13 @@
         <v>0.8</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H78" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I78" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4347,10 +4347,10 @@
         <v>93</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D79" s="19">
         <v>0.2</v>
@@ -4368,18 +4368,18 @@
         <v>22</v>
       </c>
       <c r="I79" s="20" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D80" s="12">
         <v>20</v>
@@ -4397,18 +4397,18 @@
         <v>22</v>
       </c>
       <c r="I80" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D81" s="12">
         <v>20</v>
@@ -4426,18 +4426,18 @@
         <v>22</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B82" s="11" t="s">
-        <v>149</v>
-      </c>
       <c r="C82" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D82" s="12">
         <v>13</v>
@@ -4455,18 +4455,18 @@
         <v>22</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D83" s="12">
         <v>0</v>
@@ -4489,13 +4489,13 @@
     </row>
     <row r="84" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D84" s="12">
         <v>20</v>
@@ -4513,18 +4513,18 @@
         <v>22</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D85" s="12">
         <v>20</v>
@@ -4542,18 +4542,18 @@
         <v>22</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D86" s="12">
         <v>13</v>
@@ -4571,18 +4571,18 @@
         <v>22</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D87" s="12">
         <v>0</v>
@@ -4600,18 +4600,18 @@
         <v>56</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B88" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C88" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>157</v>
       </c>
       <c r="D88" s="12">
         <v>0</v>
@@ -4629,18 +4629,18 @@
         <v>22</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B89" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C89" s="13" t="s">
         <v>156</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="D89" s="12">
         <v>120</v>
@@ -4658,18 +4658,18 @@
         <v>22</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D90" s="12">
         <v>5</v>
@@ -4687,18 +4687,18 @@
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D91" s="12">
         <v>20</v>
@@ -4716,18 +4716,18 @@
         <v>22</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D92" s="12">
         <v>20</v>
@@ -4745,18 +4745,18 @@
         <v>22</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D93" s="12">
         <v>13</v>
@@ -4774,18 +4774,18 @@
         <v>22</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D94" s="12">
         <v>0</v>
@@ -4803,18 +4803,18 @@
         <v>56</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D95" s="26">
         <v>20</v>
@@ -4832,18 +4832,18 @@
         <v>22</v>
       </c>
       <c r="I95" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="B96" s="25" t="s">
-        <v>186</v>
-      </c>
       <c r="C96" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D96" s="26">
         <v>20</v>
@@ -4861,18 +4861,18 @@
         <v>22</v>
       </c>
       <c r="I96" s="30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D97" s="26">
         <v>13</v>
@@ -4890,18 +4890,18 @@
         <v>22</v>
       </c>
       <c r="I97" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D98" s="26">
         <v>0</v>
@@ -4924,13 +4924,13 @@
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D99" s="26">
         <v>20</v>
@@ -4948,18 +4948,18 @@
         <v>22</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D100" s="26">
         <v>20</v>
@@ -4977,18 +4977,18 @@
         <v>22</v>
       </c>
       <c r="I100" s="30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D101" s="26">
         <v>13</v>
@@ -5006,18 +5006,18 @@
         <v>22</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D102" s="26">
         <v>0</v>
@@ -5035,18 +5035,18 @@
         <v>56</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A103" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B103" s="38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C103" s="30" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D103" s="26">
         <v>0</v>
@@ -5064,18 +5064,18 @@
         <v>22</v>
       </c>
       <c r="I103" s="30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A104" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B104" s="38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D104" s="26">
         <v>120</v>
@@ -5093,18 +5093,18 @@
         <v>22</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A105" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D105" s="26">
         <v>5</v>
@@ -5122,18 +5122,18 @@
         <v>22</v>
       </c>
       <c r="I105" s="30" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D106" s="26">
         <v>20</v>
@@ -5151,18 +5151,18 @@
         <v>22</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A107" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D107" s="26">
         <v>20</v>
@@ -5180,18 +5180,18 @@
         <v>22</v>
       </c>
       <c r="I107" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D108" s="26">
         <v>13</v>
@@ -5209,18 +5209,18 @@
         <v>22</v>
       </c>
       <c r="I108" s="30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D109" s="26">
         <v>0</v>
@@ -5238,18 +5238,18 @@
         <v>56</v>
       </c>
       <c r="I109" s="30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D110" s="12">
         <v>70</v>
@@ -5267,18 +5267,18 @@
         <v>22</v>
       </c>
       <c r="I110" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D111" s="6">
         <v>0.2</v>
@@ -5296,18 +5296,18 @@
         <v>60</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D112" s="6">
         <v>0.2</v>
@@ -5325,18 +5325,18 @@
         <v>60</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D113" s="6">
         <v>0.12</v>
@@ -5354,18 +5354,18 @@
         <v>60</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D114" s="6">
         <v>0.12</v>
@@ -5383,18 +5383,18 @@
         <v>60</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D115" s="6">
         <v>0.4</v>
@@ -5406,24 +5406,24 @@
         <v>0.4</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H115" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D116" s="6">
         <v>0.3</v>
@@ -5441,18 +5441,18 @@
         <v>60</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D117" s="12">
         <v>20</v>
@@ -5470,18 +5470,18 @@
         <v>22</v>
       </c>
       <c r="I117" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D118" s="12">
         <v>20</v>
@@ -5499,18 +5499,18 @@
         <v>22</v>
       </c>
       <c r="I118" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D119" s="12">
         <v>13</v>
@@ -5528,18 +5528,18 @@
         <v>22</v>
       </c>
       <c r="I119" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D120" s="12">
         <v>0</v>
@@ -5557,18 +5557,18 @@
         <v>56</v>
       </c>
       <c r="I120" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D121" s="12">
         <v>100</v>
@@ -5586,18 +5586,18 @@
         <v>56</v>
       </c>
       <c r="I121" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D122" s="6">
         <v>0.15</v>
@@ -5615,18 +5615,18 @@
         <v>60</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D123" s="29">
         <v>70</v>
@@ -5644,18 +5644,18 @@
         <v>22</v>
       </c>
       <c r="I123" s="28" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D124" s="14">
         <v>0.2</v>
@@ -5673,18 +5673,18 @@
         <v>60</v>
       </c>
       <c r="I124" s="27" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D125" s="14">
         <v>0.2</v>
@@ -5702,18 +5702,18 @@
         <v>60</v>
       </c>
       <c r="I125" s="27" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D126" s="14">
         <v>0.12</v>
@@ -5731,18 +5731,18 @@
         <v>60</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D127" s="14">
         <v>0.12</v>
@@ -5760,18 +5760,18 @@
         <v>60</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D128" s="14">
         <v>0.4</v>
@@ -5783,24 +5783,24 @@
         <v>0.4</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H128" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="B129" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="B129" s="27" t="s">
-        <v>255</v>
-      </c>
       <c r="C129" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D129" s="14">
         <v>0.3</v>
@@ -5818,18 +5818,18 @@
         <v>60</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D130" s="29">
         <v>20</v>
@@ -5847,18 +5847,18 @@
         <v>22</v>
       </c>
       <c r="I130" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D131" s="29">
         <v>20</v>
@@ -5876,18 +5876,18 @@
         <v>22</v>
       </c>
       <c r="I131" s="28" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D132" s="29">
         <v>13</v>
@@ -5905,18 +5905,18 @@
         <v>22</v>
       </c>
       <c r="I132" s="28" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D133" s="29">
         <v>0</v>
@@ -5934,18 +5934,18 @@
         <v>56</v>
       </c>
       <c r="I133" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A134" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D134" s="29">
         <v>100</v>
@@ -5963,18 +5963,18 @@
         <v>56</v>
       </c>
       <c r="I134" s="28" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B135" s="27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D135" s="14">
         <v>0.15</v>
@@ -5992,18 +5992,18 @@
         <v>60</v>
       </c>
       <c r="I135" s="27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B136" s="40" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D136" s="6">
         <v>0.1</v>
@@ -6021,18 +6021,18 @@
         <v>22</v>
       </c>
       <c r="I136" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B137" s="40" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D137" s="6">
         <v>0.15</v>
@@ -6050,18 +6050,18 @@
         <v>22</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B138" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C138" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="D138" s="6">
         <v>0.5</v>
@@ -6079,47 +6079,47 @@
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B139" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D139" s="6">
+        <v>0</v>
+      </c>
+      <c r="E139" s="6">
+        <v>0</v>
+      </c>
+      <c r="F139" s="6">
+        <v>0</v>
+      </c>
+      <c r="G139" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="C139" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D139" s="6">
-        <v>0</v>
-      </c>
-      <c r="E139" s="6">
-        <v>0</v>
-      </c>
-      <c r="F139" s="6">
-        <v>0</v>
-      </c>
-      <c r="G139" s="11" t="s">
-        <v>287</v>
-      </c>
       <c r="H139" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D140" s="6">
         <v>0.1</v>
@@ -6137,18 +6137,18 @@
         <v>22</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D141" s="6">
         <v>0.1</v>
@@ -6166,18 +6166,18 @@
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D142" s="6">
         <v>0.15</v>
@@ -6195,18 +6195,18 @@
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D143" s="6">
         <v>0.1</v>
@@ -6224,18 +6224,18 @@
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D144" s="6">
         <v>20</v>
@@ -6253,18 +6253,18 @@
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D145" s="6">
         <v>20</v>
@@ -6282,18 +6282,18 @@
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D146" s="6">
         <v>13</v>
@@ -6311,18 +6311,18 @@
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D147" s="6">
         <v>0</v>
@@ -6340,18 +6340,18 @@
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D148" s="6">
         <v>0.1</v>
@@ -6369,18 +6369,18 @@
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D149" s="6">
         <v>0.15</v>
@@ -6398,18 +6398,18 @@
         <v>22</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D150" s="6">
         <v>0.1</v>
@@ -6427,18 +6427,18 @@
         <v>22</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D151" s="6">
         <v>0.5</v>
@@ -6450,24 +6450,24 @@
         <v>0.5</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D152" s="6">
         <v>0</v>
@@ -6485,18 +6485,18 @@
         <v>22</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D153" s="6">
         <v>0.1</v>
@@ -6514,18 +6514,18 @@
         <v>22</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="B154" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="B154" s="27" t="s">
-        <v>333</v>
-      </c>
       <c r="C154" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D154" s="29">
         <v>25</v>
@@ -6543,18 +6543,18 @@
         <v>60</v>
       </c>
       <c r="I154" s="28" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A155" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D155" s="29">
         <v>-25</v>
@@ -6572,18 +6572,18 @@
         <v>46</v>
       </c>
       <c r="I155" s="28" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D156" s="29">
         <v>0</v>
@@ -6601,18 +6601,18 @@
         <v>46</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D157" s="29">
         <v>85</v>
@@ -6630,18 +6630,18 @@
         <v>46</v>
       </c>
       <c r="I157" s="28" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D158" s="29">
         <v>75</v>
@@ -6659,18 +6659,18 @@
         <v>46</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D159" s="29">
         <v>0</v>
@@ -6682,24 +6682,24 @@
         <v>0</v>
       </c>
       <c r="G159" s="27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H159" s="27" t="s">
         <v>60</v>
       </c>
       <c r="I159" s="28" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D160" s="29">
         <v>2044</v>
@@ -6717,18 +6717,18 @@
         <v>22</v>
       </c>
       <c r="I160" s="28" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A161" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B161" s="27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D161" s="29">
         <v>-0.04</v>
@@ -6740,24 +6740,24 @@
         <v>-0.04</v>
       </c>
       <c r="G161" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H161" s="27" t="s">
         <v>46</v>
       </c>
       <c r="I161" s="28" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>363</v>
+      </c>
+      <c r="C162" s="6" t="s">
         <v>364</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>366</v>
       </c>
       <c r="D162" s="6">
         <v>500</v>
@@ -6769,24 +6769,24 @@
         <v>500</v>
       </c>
       <c r="G162" s="11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H162" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I162" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D163" s="12">
         <v>20</v>
@@ -6804,18 +6804,18 @@
         <v>22</v>
       </c>
       <c r="I163" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D164" s="12">
         <v>20</v>
@@ -6833,18 +6833,18 @@
         <v>22</v>
       </c>
       <c r="I164" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D165" s="12">
         <v>7</v>
@@ -6862,18 +6862,18 @@
         <v>22</v>
       </c>
       <c r="I165" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D166" s="12">
         <v>0</v>
@@ -6891,18 +6891,18 @@
         <v>22</v>
       </c>
       <c r="I166" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="B167" s="25" t="s">
         <v>380</v>
       </c>
-      <c r="B167" s="25" t="s">
-        <v>382</v>
-      </c>
       <c r="C167" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D167" s="10">
         <v>500</v>
@@ -6914,24 +6914,24 @@
         <v>500</v>
       </c>
       <c r="G167" s="25" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H167" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I167" s="25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A168" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B168" s="25" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D168" s="26">
         <v>20</v>
@@ -6949,18 +6949,18 @@
         <v>22</v>
       </c>
       <c r="I168" s="30" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="169" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D169" s="26">
         <v>20</v>
@@ -6978,18 +6978,18 @@
         <v>22</v>
       </c>
       <c r="I169" s="30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="170" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D170" s="26">
         <v>7</v>
@@ -7007,18 +7007,18 @@
         <v>22</v>
       </c>
       <c r="I170" s="30" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A171" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D171" s="26">
         <v>0</v>
@@ -7036,18 +7036,18 @@
         <v>22</v>
       </c>
       <c r="I171" s="30" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A172" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="B172" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C172" s="6" t="s">
         <v>403</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>405</v>
       </c>
       <c r="D172" s="12">
         <v>2</v>
@@ -7059,24 +7059,24 @@
         <v>2</v>
       </c>
       <c r="G172" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H172" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I172" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D173" s="12">
         <v>0.05</v>
@@ -7088,24 +7088,24 @@
         <v>0.05</v>
       </c>
       <c r="G173" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H173" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I173" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D174" s="39">
         <v>80</v>
@@ -7123,18 +7123,18 @@
         <v>22</v>
       </c>
       <c r="I174" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D175" s="12">
         <v>0</v>
@@ -7152,18 +7152,18 @@
         <v>22</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D176" s="12">
         <v>0</v>
@@ -7181,18 +7181,18 @@
         <v>22</v>
       </c>
       <c r="I176" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D177" s="12">
         <v>0</v>
@@ -7210,18 +7210,18 @@
         <v>22</v>
       </c>
       <c r="I177" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D178" s="12">
         <v>0</v>
@@ -7239,18 +7239,18 @@
         <v>22</v>
       </c>
       <c r="I178" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D179" s="12">
         <v>20</v>
@@ -7268,18 +7268,18 @@
         <v>22</v>
       </c>
       <c r="I179" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A180" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B180" s="27" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D180" s="29">
         <v>50</v>
@@ -7297,18 +7297,18 @@
         <v>22</v>
       </c>
       <c r="I180" s="28" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A181" s="27" t="s">
+        <v>429</v>
+      </c>
+      <c r="B181" s="27" t="s">
         <v>431</v>
       </c>
-      <c r="B181" s="27" t="s">
-        <v>433</v>
-      </c>
       <c r="C181" s="14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D181" s="29">
         <v>20</v>
@@ -7326,18 +7326,18 @@
         <v>22</v>
       </c>
       <c r="I181" s="28" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D182" s="29">
         <v>7</v>
@@ -7355,18 +7355,18 @@
         <v>22</v>
       </c>
       <c r="I182" s="28" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A183" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D183" s="29">
         <v>0</v>
@@ -7384,18 +7384,18 @@
         <v>56</v>
       </c>
       <c r="I183" s="28" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A184" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B184" s="27" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D184" s="29">
         <v>100</v>
@@ -7413,18 +7413,18 @@
         <v>56</v>
       </c>
       <c r="I184" s="28" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="B185" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="B185" s="11" t="s">
-        <v>451</v>
-      </c>
       <c r="C185" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D185" s="39">
         <v>100</v>
@@ -7442,18 +7442,18 @@
         <v>22</v>
       </c>
       <c r="I185" s="13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D186" s="12">
         <v>80</v>
@@ -7471,18 +7471,18 @@
         <v>60</v>
       </c>
       <c r="I186" s="13" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D187" s="12">
         <v>0</v>
@@ -7500,18 +7500,18 @@
         <v>22</v>
       </c>
       <c r="I187" s="13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D188" s="12">
         <v>0</v>
@@ -7529,18 +7529,18 @@
         <v>22</v>
       </c>
       <c r="I188" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A189" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="B189" s="27" t="s">
         <v>458</v>
       </c>
-      <c r="B189" s="27" t="s">
-        <v>460</v>
-      </c>
       <c r="C189" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D189" s="29">
         <v>90</v>
@@ -7558,18 +7558,18 @@
         <v>56</v>
       </c>
       <c r="I189" s="28" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A190" s="27" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B190" s="27" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C190" s="28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D190" s="29">
         <v>50</v>
@@ -7587,7 +7587,7 @@
         <v>56</v>
       </c>
       <c r="I190" s="28" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
review parameters birth only typos changed
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -193,9 +193,6 @@
     <t>bir_plot_lim</t>
   </si>
   <si>
-    <t>the fertility rates of the past are compared with the precitions; the y-axis is limited (since the fertility rate of the past can be very large due to low population)</t>
-  </si>
-  <si>
     <t>birth per woman and year in %</t>
   </si>
   <si>
@@ -1455,20 +1452,23 @@
     <t>after the prediction: proportion of data points used in the loess regressions of fertility by age; groups: district, year, origin</t>
   </si>
   <si>
-    <t xml:space="preserve">age distribution of women (population): if there are less woman than this threshold in the tails (cumulative measure), then the rate based on origin (but not district) is used.
+    <t>age distribution of women (population): if there are less woman than this threshold in the tails (cumulative measure), then the overall rate is used (e.g not the rate based on origin and district).</t>
+  </si>
+  <si>
+    <t>origin change (mother-baby): lower threshold for the rate (here: the rate should not be negative), NA if there is no lower threshold</t>
+  </si>
+  <si>
+    <t>origin change (mother-baby): upper threshold for the rate (here: not more than 100 %), NA if there is no lower threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age distribution of women (population): if there are less women than this threshold in the tails (cumulative measure), then the rate based on origin (but not district) is used.
 </t>
   </si>
   <si>
-    <t>age distribution of women (population): if there are less woman than this threshold in the tails (cumulative measure), then the overall rate is used (e.g not the rate based on origin and district).</t>
-  </si>
-  <si>
-    <t>age distribution of women (population): if there are less woman than this threshold in the tails (cumulative measure), then a constant rate is used (e.g not the rate based on origin and district). The constant rate is set by the parameter bir_thres_value.</t>
-  </si>
-  <si>
-    <t>origin change (mother-baby): lower threshold for the rate (here: the rate should not be negative), NA if there is no lower threshold</t>
-  </si>
-  <si>
-    <t>origin change (mother-baby): upper threshold for the rate (here: not more than 100 %), NA if there is no lower threshold</t>
+    <t>age distribution of women (population): if there are less women than this threshold in the tails (cumulative measure), then a constant rate is used (e.g not the rate based on origin and district). The constant rate is set by the parameter bir_thres_value.</t>
+  </si>
+  <si>
+    <t>the fertility rates of the past are compared with the predictions; the y-axis is limited (since the fertility rate of the past can be very large due to low population)</t>
   </si>
 </sst>
 </file>
@@ -2050,8 +2050,8 @@
   <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2082,7 +2082,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -2094,7 +2094,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2160,7 +2160,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>50</v>
@@ -2189,7 +2189,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>51</v>
@@ -2294,10 +2294,10 @@
         <v>34</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2323,10 +2323,10 @@
         <v>34</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2334,10 +2334,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="10">
         <v>2007</v>
@@ -2355,7 +2355,7 @@
         <v>22</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2363,10 +2363,10 @@
         <v>19</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="35">
         <v>2021</v>
@@ -2384,7 +2384,7 @@
         <v>22</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2392,10 +2392,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" s="10">
         <v>1993</v>
@@ -2413,7 +2413,7 @@
         <v>22</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2421,10 +2421,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="35">
         <v>2021</v>
@@ -2442,7 +2442,7 @@
         <v>22</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2450,10 +2450,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="10">
         <v>1993</v>
@@ -2471,7 +2471,7 @@
         <v>22</v>
       </c>
       <c r="I14" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2479,10 +2479,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="10">
         <v>2019</v>
@@ -2500,7 +2500,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2508,10 +2508,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="D16" s="10">
         <v>2014</v>
@@ -2529,7 +2529,7 @@
         <v>22</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2537,10 +2537,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="D17" s="35">
         <v>2021</v>
@@ -2558,7 +2558,7 @@
         <v>22</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2566,10 +2566,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="10">
         <v>2010</v>
@@ -2587,7 +2587,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2595,10 +2595,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="35">
         <v>2021</v>
@@ -2616,7 +2616,7 @@
         <v>22</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2624,10 +2624,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="10">
         <v>2010</v>
@@ -2645,7 +2645,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2653,10 +2653,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="35">
         <v>2021</v>
@@ -2674,7 +2674,7 @@
         <v>22</v>
       </c>
       <c r="I21" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2682,10 +2682,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="10">
         <v>2010</v>
@@ -2703,7 +2703,7 @@
         <v>22</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2711,10 +2711,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="35">
         <v>2021</v>
@@ -2732,7 +2732,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2740,10 +2740,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" s="10">
         <v>2010</v>
@@ -2761,7 +2761,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2769,10 +2769,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="35">
         <v>2021</v>
@@ -2790,7 +2790,7 @@
         <v>22</v>
       </c>
       <c r="I25" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2798,10 +2798,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="10">
         <v>2010</v>
@@ -2819,7 +2819,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2827,10 +2827,10 @@
         <v>19</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="35">
         <v>2021</v>
@@ -2848,7 +2848,7 @@
         <v>22</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2856,10 +2856,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="10">
         <v>2010</v>
@@ -2877,7 +2877,7 @@
         <v>22</v>
       </c>
       <c r="I28" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2885,10 +2885,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" s="35">
         <v>2021</v>
@@ -2906,7 +2906,7 @@
         <v>22</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2914,10 +2914,10 @@
         <v>19</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="10">
         <v>2005</v>
@@ -2935,7 +2935,7 @@
         <v>22</v>
       </c>
       <c r="I30" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2943,10 +2943,10 @@
         <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="37">
         <v>2019</v>
@@ -2964,7 +2964,7 @@
         <v>22</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2972,10 +2972,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="10">
         <v>2005</v>
@@ -2993,7 +2993,7 @@
         <v>22</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3001,10 +3001,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="37">
         <v>2019</v>
@@ -3022,7 +3022,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3030,10 +3030,10 @@
         <v>19</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" s="10">
         <v>2011</v>
@@ -3051,7 +3051,7 @@
         <v>22</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3059,10 +3059,10 @@
         <v>19</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="35">
         <v>2021</v>
@@ -3080,7 +3080,7 @@
         <v>22</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3088,10 +3088,10 @@
         <v>19</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="10">
         <v>2011</v>
@@ -3109,7 +3109,7 @@
         <v>22</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3117,10 +3117,10 @@
         <v>19</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D37" s="35">
         <v>2021</v>
@@ -3138,7 +3138,7 @@
         <v>22</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3146,10 +3146,10 @@
         <v>19</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="10">
         <v>2015</v>
@@ -3167,7 +3167,7 @@
         <v>22</v>
       </c>
       <c r="I38" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3175,10 +3175,10 @@
         <v>19</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="10">
         <v>2011</v>
@@ -3196,7 +3196,7 @@
         <v>22</v>
       </c>
       <c r="I39" s="31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3204,10 +3204,10 @@
         <v>19</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="35">
         <v>2021</v>
@@ -3225,7 +3225,7 @@
         <v>22</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3233,10 +3233,10 @@
         <v>19</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D41" s="10">
         <v>2015</v>
@@ -3254,7 +3254,7 @@
         <v>22</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3262,10 +3262,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D42" s="34">
         <v>2022</v>
@@ -3283,7 +3283,7 @@
         <v>22</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3291,10 +3291,10 @@
         <v>19</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D43" s="34">
         <v>2029</v>
@@ -3312,7 +3312,7 @@
         <v>22</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3320,10 +3320,10 @@
         <v>19</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" s="10">
         <v>2015</v>
@@ -3341,7 +3341,7 @@
         <v>22</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3349,10 +3349,10 @@
         <v>19</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D45" s="35">
         <v>2021</v>
@@ -3370,18 +3370,18 @@
         <v>22</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B46" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="C46" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D46" s="12">
         <v>0</v>
@@ -3393,24 +3393,24 @@
         <v>0</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D47" s="12">
         <v>120</v>
@@ -3422,24 +3422,24 @@
         <v>120</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48" s="29">
         <v>4</v>
@@ -3451,24 +3451,24 @@
         <v>4</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H48" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I48" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" s="29">
         <v>4</v>
@@ -3480,24 +3480,24 @@
         <v>4</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H49" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I49" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D50" s="29">
         <v>4</v>
@@ -3509,24 +3509,24 @@
         <v>4</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H50" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D51" s="26">
         <v>0</v>
@@ -3538,24 +3538,24 @@
         <v>0</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H51" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" s="29">
         <v>4</v>
@@ -3567,13 +3567,13 @@
         <v>4</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H52" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3660,7 +3660,7 @@
         <v>22</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3689,7 +3689,7 @@
         <v>22</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -3718,7 +3718,7 @@
         <v>22</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3741,7 +3741,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>22</v>
@@ -3755,10 +3755,10 @@
         <v>20</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" s="6">
         <v>0.3</v>
@@ -3770,13 +3770,13 @@
         <v>0.3</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H59" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3871,10 +3871,10 @@
         <v>20</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D63" s="12">
         <v>0</v>
@@ -3886,13 +3886,13 @@
         <v>0</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I63" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -3900,28 +3900,28 @@
         <v>20</v>
       </c>
       <c r="B64" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>81</v>
-      </c>
       <c r="E64" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I64" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3932,7 +3932,7 @@
         <v>57</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D65" s="12">
         <v>30</v>
@@ -3944,13 +3944,13 @@
         <v>30</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H65" s="11" t="s">
         <v>56</v>
       </c>
       <c r="I65" s="13" t="s">
-        <v>58</v>
+        <v>482</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3958,10 +3958,10 @@
         <v>20</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D66" s="6">
         <v>0.15</v>
@@ -3973,13 +3973,13 @@
         <v>0.15</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H66" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3987,10 +3987,10 @@
         <v>20</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D67" s="12">
         <v>0</v>
@@ -4008,7 +4008,7 @@
         <v>22</v>
       </c>
       <c r="I67" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4016,10 +4016,10 @@
         <v>20</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D68" s="12">
         <v>20</v>
@@ -4037,7 +4037,7 @@
         <v>46</v>
       </c>
       <c r="I68" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -4045,10 +4045,10 @@
         <v>20</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D69" s="12">
         <v>20</v>
@@ -4066,7 +4066,7 @@
         <v>22</v>
       </c>
       <c r="I69" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4074,10 +4074,10 @@
         <v>20</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D70" s="12">
         <v>13</v>
@@ -4095,7 +4095,7 @@
         <v>22</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4103,10 +4103,10 @@
         <v>20</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D71" s="12">
         <v>0</v>
@@ -4124,7 +4124,7 @@
         <v>22</v>
       </c>
       <c r="I71" s="13" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4132,10 +4132,10 @@
         <v>20</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D72" s="12">
         <v>100</v>
@@ -4153,18 +4153,18 @@
         <v>22</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D73" s="16">
         <v>30</v>
@@ -4176,82 +4176,82 @@
         <v>30</v>
       </c>
       <c r="G73" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I73" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="H73" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I73" s="15" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="19">
+        <v>99</v>
+      </c>
+      <c r="E74" s="19">
+        <v>99</v>
+      </c>
+      <c r="F74" s="19">
+        <v>99</v>
+      </c>
+      <c r="G74" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B74" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D74" s="19">
-        <v>99</v>
-      </c>
-      <c r="E74" s="19">
-        <v>99</v>
-      </c>
-      <c r="F74" s="19">
-        <v>99</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>94</v>
-      </c>
       <c r="H74" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="19">
+        <v>0</v>
+      </c>
+      <c r="E75" s="19">
+        <v>0</v>
+      </c>
+      <c r="F75" s="19">
+        <v>0</v>
+      </c>
+      <c r="G75" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B75" s="38" t="s">
+      <c r="H75" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I75" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D75" s="19">
-        <v>0</v>
-      </c>
-      <c r="E75" s="19">
-        <v>0</v>
-      </c>
-      <c r="F75" s="19">
-        <v>0</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H75" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I75" s="15" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D76" s="19">
         <v>120</v>
@@ -4263,24 +4263,24 @@
         <v>120</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H76" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I76" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D77" s="19">
         <v>120</v>
@@ -4292,24 +4292,24 @@
         <v>120</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>22</v>
       </c>
       <c r="I77" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D78" s="19">
         <v>2</v>
@@ -4321,24 +4321,24 @@
         <v>2</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H78" s="14" t="s">
         <v>56</v>
       </c>
       <c r="I78" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D79" s="19">
         <v>3</v>
@@ -4350,24 +4350,24 @@
         <v>3</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H79" s="14" t="s">
         <v>56</v>
       </c>
       <c r="I79" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D80" s="19">
         <v>0.8</v>
@@ -4379,24 +4379,24 @@
         <v>0.8</v>
       </c>
       <c r="G80" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I80" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="H80" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I80" s="20" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D81" s="12">
         <v>20</v>
@@ -4414,18 +4414,18 @@
         <v>22</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="11" t="s">
-        <v>153</v>
-      </c>
       <c r="C82" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D82" s="12">
         <v>20</v>
@@ -4443,18 +4443,18 @@
         <v>22</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D83" s="12">
         <v>13</v>
@@ -4472,18 +4472,18 @@
         <v>22</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D84" s="12">
         <v>0</v>
@@ -4501,18 +4501,18 @@
         <v>56</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D85" s="12">
         <v>20</v>
@@ -4530,18 +4530,18 @@
         <v>22</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D86" s="12">
         <v>20</v>
@@ -4559,18 +4559,18 @@
         <v>22</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D87" s="12">
         <v>13</v>
@@ -4588,18 +4588,18 @@
         <v>22</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D88" s="12">
         <v>0</v>
@@ -4617,18 +4617,18 @@
         <v>56</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D89" s="12">
         <v>0</v>
@@ -4640,24 +4640,24 @@
         <v>0</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B90" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D90" s="12">
         <v>120</v>
@@ -4669,24 +4669,24 @@
         <v>120</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D91" s="12">
         <v>5</v>
@@ -4704,18 +4704,18 @@
         <v>22</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D92" s="12">
         <v>20</v>
@@ -4733,18 +4733,18 @@
         <v>22</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D93" s="12">
         <v>20</v>
@@ -4762,18 +4762,18 @@
         <v>22</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D94" s="12">
         <v>13</v>
@@ -4791,18 +4791,18 @@
         <v>22</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D95" s="12">
         <v>0</v>
@@ -4820,18 +4820,18 @@
         <v>56</v>
       </c>
       <c r="I95" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="25" t="s">
-        <v>190</v>
-      </c>
       <c r="C96" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D96" s="26">
         <v>20</v>
@@ -4849,18 +4849,18 @@
         <v>22</v>
       </c>
       <c r="I96" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D97" s="26">
         <v>20</v>
@@ -4878,18 +4878,18 @@
         <v>22</v>
       </c>
       <c r="I97" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D98" s="26">
         <v>13</v>
@@ -4907,18 +4907,18 @@
         <v>22</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D99" s="26">
         <v>0</v>
@@ -4936,18 +4936,18 @@
         <v>56</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D100" s="26">
         <v>20</v>
@@ -4965,18 +4965,18 @@
         <v>22</v>
       </c>
       <c r="I100" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A101" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D101" s="26">
         <v>20</v>
@@ -4994,18 +4994,18 @@
         <v>22</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D102" s="26">
         <v>13</v>
@@ -5023,18 +5023,18 @@
         <v>22</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D103" s="26">
         <v>0</v>
@@ -5052,18 +5052,18 @@
         <v>56</v>
       </c>
       <c r="I103" s="30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A104" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B104" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D104" s="26">
         <v>0</v>
@@ -5075,24 +5075,24 @@
         <v>0</v>
       </c>
       <c r="G104" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H104" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B105" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D105" s="26">
         <v>120</v>
@@ -5104,24 +5104,24 @@
         <v>120</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H105" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I105" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C106" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D106" s="26">
         <v>5</v>
@@ -5139,18 +5139,18 @@
         <v>22</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A107" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D107" s="26">
         <v>20</v>
@@ -5168,18 +5168,18 @@
         <v>22</v>
       </c>
       <c r="I107" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A108" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D108" s="26">
         <v>20</v>
@@ -5197,18 +5197,18 @@
         <v>22</v>
       </c>
       <c r="I108" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A109" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D109" s="26">
         <v>13</v>
@@ -5226,18 +5226,18 @@
         <v>22</v>
       </c>
       <c r="I109" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A110" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D110" s="26">
         <v>0</v>
@@ -5255,18 +5255,18 @@
         <v>56</v>
       </c>
       <c r="I110" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D111" s="12">
         <v>70</v>
@@ -5284,18 +5284,18 @@
         <v>22</v>
       </c>
       <c r="I111" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D112" s="6">
         <v>0.2</v>
@@ -5307,24 +5307,24 @@
         <v>0.2</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D113" s="6">
         <v>0.2</v>
@@ -5336,24 +5336,24 @@
         <v>0.2</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H113" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D114" s="6">
         <v>0.12</v>
@@ -5365,24 +5365,24 @@
         <v>0.12</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D115" s="6">
         <v>0.12</v>
@@ -5394,24 +5394,24 @@
         <v>0.12</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H115" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D116" s="6">
         <v>0.4</v>
@@ -5423,24 +5423,24 @@
         <v>0.4</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H116" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D117" s="6">
         <v>0.3</v>
@@ -5452,24 +5452,24 @@
         <v>0.3</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H117" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I117" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D118" s="12">
         <v>20</v>
@@ -5487,18 +5487,18 @@
         <v>22</v>
       </c>
       <c r="I118" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D119" s="12">
         <v>20</v>
@@ -5516,18 +5516,18 @@
         <v>22</v>
       </c>
       <c r="I119" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D120" s="12">
         <v>13</v>
@@ -5545,18 +5545,18 @@
         <v>22</v>
       </c>
       <c r="I120" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D121" s="12">
         <v>0</v>
@@ -5574,18 +5574,18 @@
         <v>56</v>
       </c>
       <c r="I121" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D122" s="12">
         <v>100</v>
@@ -5603,18 +5603,18 @@
         <v>56</v>
       </c>
       <c r="I122" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D123" s="6">
         <v>0.15</v>
@@ -5626,24 +5626,24 @@
         <v>0.15</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H123" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D124" s="29">
         <v>70</v>
@@ -5661,18 +5661,18 @@
         <v>22</v>
       </c>
       <c r="I124" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D125" s="14">
         <v>0.2</v>
@@ -5684,24 +5684,24 @@
         <v>0.2</v>
       </c>
       <c r="G125" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H125" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I125" s="27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="B126" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="B126" s="27" t="s">
-        <v>259</v>
-      </c>
       <c r="C126" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D126" s="14">
         <v>0.2</v>
@@ -5713,24 +5713,24 @@
         <v>0.2</v>
       </c>
       <c r="G126" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H126" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D127" s="14">
         <v>0.12</v>
@@ -5742,24 +5742,24 @@
         <v>0.12</v>
       </c>
       <c r="G127" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H127" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D128" s="14">
         <v>0.12</v>
@@ -5771,24 +5771,24 @@
         <v>0.12</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H128" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D129" s="14">
         <v>0.4</v>
@@ -5800,24 +5800,24 @@
         <v>0.4</v>
       </c>
       <c r="G129" s="27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H129" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D130" s="14">
         <v>0.3</v>
@@ -5829,24 +5829,24 @@
         <v>0.3</v>
       </c>
       <c r="G130" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H130" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I130" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D131" s="29">
         <v>20</v>
@@ -5864,18 +5864,18 @@
         <v>22</v>
       </c>
       <c r="I131" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D132" s="29">
         <v>20</v>
@@ -5893,18 +5893,18 @@
         <v>22</v>
       </c>
       <c r="I132" s="28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A133" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D133" s="29">
         <v>13</v>
@@ -5922,18 +5922,18 @@
         <v>22</v>
       </c>
       <c r="I133" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A134" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D134" s="29">
         <v>0</v>
@@ -5951,18 +5951,18 @@
         <v>56</v>
       </c>
       <c r="I134" s="28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B135" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C135" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D135" s="29">
         <v>100</v>
@@ -5980,18 +5980,18 @@
         <v>56</v>
       </c>
       <c r="I135" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B136" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D136" s="14">
         <v>0.15</v>
@@ -6003,24 +6003,24 @@
         <v>0.15</v>
       </c>
       <c r="G136" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H136" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I136" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B137" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="C137" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B137" s="40" t="s">
-        <v>287</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D137" s="6">
         <v>0.1</v>
@@ -6032,24 +6032,24 @@
         <v>0.1</v>
       </c>
       <c r="G137" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H137" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B138" s="40" t="s">
+        <v>287</v>
+      </c>
+      <c r="C138" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B138" s="40" t="s">
-        <v>288</v>
-      </c>
-      <c r="C138" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D138" s="6">
         <v>0.15</v>
@@ -6061,24 +6061,24 @@
         <v>0.15</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H138" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D139" s="6">
         <v>0.5</v>
@@ -6096,18 +6096,18 @@
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D140" s="6">
         <v>0</v>
@@ -6119,24 +6119,24 @@
         <v>0</v>
       </c>
       <c r="G140" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="H140" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I140" s="11" t="s">
         <v>292</v>
-      </c>
-      <c r="H140" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I140" s="11" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B141" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="C141" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B141" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="C141" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D141" s="6">
         <v>0.1</v>
@@ -6148,24 +6148,24 @@
         <v>0.1</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H141" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B142" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C142" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B142" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D142" s="6">
         <v>0.1</v>
@@ -6177,24 +6177,24 @@
         <v>0.1</v>
       </c>
       <c r="G142" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H142" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="C143" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B143" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="C143" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D143" s="6">
         <v>0.15</v>
@@ -6206,24 +6206,24 @@
         <v>0.15</v>
       </c>
       <c r="G143" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H143" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C144" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B144" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="C144" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D144" s="6">
         <v>0.1</v>
@@ -6235,24 +6235,24 @@
         <v>0.1</v>
       </c>
       <c r="G144" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H144" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B145" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="C145" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="C145" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="D145" s="6">
         <v>20</v>
@@ -6270,18 +6270,18 @@
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D146" s="6">
         <v>20</v>
@@ -6299,18 +6299,18 @@
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D147" s="6">
         <v>13</v>
@@ -6328,18 +6328,18 @@
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D148" s="6">
         <v>0</v>
@@ -6357,18 +6357,18 @@
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C149" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B149" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C149" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D149" s="6">
         <v>0.1</v>
@@ -6380,24 +6380,24 @@
         <v>0.1</v>
       </c>
       <c r="G149" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H149" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="C150" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B150" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="C150" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D150" s="6">
         <v>0.15</v>
@@ -6409,24 +6409,24 @@
         <v>0.15</v>
       </c>
       <c r="G150" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H150" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B151" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="C151" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B151" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D151" s="6">
         <v>0.1</v>
@@ -6438,24 +6438,24 @@
         <v>0.1</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D152" s="6">
         <v>0.5</v>
@@ -6467,24 +6467,24 @@
         <v>0.5</v>
       </c>
       <c r="G152" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H152" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I152" s="11" t="s">
         <v>321</v>
-      </c>
-      <c r="H152" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I152" s="11" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D153" s="6">
         <v>0</v>
@@ -6496,24 +6496,24 @@
         <v>0</v>
       </c>
       <c r="G153" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H153" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="C154" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B154" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="C154" s="6" t="s">
-        <v>285</v>
       </c>
       <c r="D154" s="6">
         <v>0.1</v>
@@ -6525,24 +6525,24 @@
         <v>0.1</v>
       </c>
       <c r="G154" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H154" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I154" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="B155" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="C155" s="14" t="s">
         <v>336</v>
-      </c>
-      <c r="B155" s="27" t="s">
-        <v>338</v>
-      </c>
-      <c r="C155" s="14" t="s">
-        <v>337</v>
       </c>
       <c r="D155" s="29">
         <v>25</v>
@@ -6557,21 +6557,21 @@
         <v>44</v>
       </c>
       <c r="H155" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I155" s="28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A156" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D156" s="29">
         <v>-25</v>
@@ -6589,18 +6589,18 @@
         <v>46</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D157" s="29">
         <v>0</v>
@@ -6618,18 +6618,18 @@
         <v>46</v>
       </c>
       <c r="I157" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D158" s="29">
         <v>85</v>
@@ -6647,18 +6647,18 @@
         <v>46</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D159" s="29">
         <v>75</v>
@@ -6676,47 +6676,47 @@
         <v>46</v>
       </c>
       <c r="I159" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B160" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="C160" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D160" s="29">
+        <v>0</v>
+      </c>
+      <c r="E160" s="29">
+        <v>0</v>
+      </c>
+      <c r="F160" s="29">
+        <v>0</v>
+      </c>
+      <c r="G160" s="27" t="s">
         <v>350</v>
       </c>
-      <c r="C160" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="D160" s="29">
-        <v>0</v>
-      </c>
-      <c r="E160" s="29">
-        <v>0</v>
-      </c>
-      <c r="F160" s="29">
-        <v>0</v>
-      </c>
-      <c r="G160" s="27" t="s">
-        <v>351</v>
-      </c>
       <c r="H160" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I160" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B161" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D161" s="29">
         <v>2044</v>
@@ -6734,18 +6734,18 @@
         <v>22</v>
       </c>
       <c r="I161" s="28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A162" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D162" s="29">
         <v>-0.04</v>
@@ -6757,24 +6757,24 @@
         <v>-0.04</v>
       </c>
       <c r="G162" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H162" s="27" t="s">
         <v>46</v>
       </c>
       <c r="I162" s="28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="B163" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="B163" s="11" t="s">
+      <c r="C163" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>371</v>
       </c>
       <c r="D163" s="6">
         <v>500</v>
@@ -6786,24 +6786,24 @@
         <v>500</v>
       </c>
       <c r="G163" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="H163" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I163" s="11" t="s">
         <v>372</v>
-      </c>
-      <c r="H163" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I163" s="11" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D164" s="12">
         <v>20</v>
@@ -6821,18 +6821,18 @@
         <v>22</v>
       </c>
       <c r="I164" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D165" s="12">
         <v>20</v>
@@ -6850,18 +6850,18 @@
         <v>22</v>
       </c>
       <c r="I165" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D166" s="12">
         <v>7</v>
@@ -6879,18 +6879,18 @@
         <v>22</v>
       </c>
       <c r="I166" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A167" s="11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D167" s="12">
         <v>0</v>
@@ -6908,18 +6908,18 @@
         <v>22</v>
       </c>
       <c r="I167" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="B168" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="C168" s="10" t="s">
         <v>385</v>
-      </c>
-      <c r="B168" s="25" t="s">
-        <v>387</v>
-      </c>
-      <c r="C168" s="10" t="s">
-        <v>386</v>
       </c>
       <c r="D168" s="10">
         <v>500</v>
@@ -6931,24 +6931,24 @@
         <v>500</v>
       </c>
       <c r="G168" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="H168" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I168" s="25" t="s">
         <v>372</v>
-      </c>
-      <c r="H168" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I168" s="25" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="169" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D169" s="26">
         <v>20</v>
@@ -6966,18 +6966,18 @@
         <v>22</v>
       </c>
       <c r="I169" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="170" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A170" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D170" s="26">
         <v>20</v>
@@ -6995,18 +6995,18 @@
         <v>22</v>
       </c>
       <c r="I170" s="30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D171" s="26">
         <v>7</v>
@@ -7024,18 +7024,18 @@
         <v>22</v>
       </c>
       <c r="I171" s="30" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A172" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B172" s="25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C172" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D172" s="26">
         <v>0</v>
@@ -7053,18 +7053,18 @@
         <v>22</v>
       </c>
       <c r="I172" s="30" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="B173" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="B173" s="11" t="s">
+      <c r="C173" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>410</v>
       </c>
       <c r="D173" s="12">
         <v>2</v>
@@ -7076,24 +7076,24 @@
         <v>2</v>
       </c>
       <c r="G173" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H173" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I173" s="13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B174" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="C174" s="6" t="s">
         <v>412</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>413</v>
       </c>
       <c r="D174" s="12">
         <v>0.05</v>
@@ -7105,24 +7105,24 @@
         <v>0.05</v>
       </c>
       <c r="G174" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H174" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I174" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D175" s="39">
         <v>80</v>
@@ -7140,18 +7140,18 @@
         <v>22</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D176" s="12">
         <v>0</v>
@@ -7169,18 +7169,18 @@
         <v>22</v>
       </c>
       <c r="I176" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D177" s="12">
         <v>0</v>
@@ -7198,18 +7198,18 @@
         <v>22</v>
       </c>
       <c r="I177" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D178" s="12">
         <v>0</v>
@@ -7227,18 +7227,18 @@
         <v>22</v>
       </c>
       <c r="I178" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D179" s="12">
         <v>0</v>
@@ -7256,18 +7256,18 @@
         <v>22</v>
       </c>
       <c r="I179" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D180" s="12">
         <v>20</v>
@@ -7285,18 +7285,18 @@
         <v>22</v>
       </c>
       <c r="I180" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A181" s="27" t="s">
+        <v>435</v>
+      </c>
+      <c r="B181" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="B181" s="27" t="s">
-        <v>437</v>
-      </c>
       <c r="C181" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D181" s="29">
         <v>50</v>
@@ -7314,18 +7314,18 @@
         <v>22</v>
       </c>
       <c r="I181" s="28" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A182" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D182" s="29">
         <v>20</v>
@@ -7343,18 +7343,18 @@
         <v>22</v>
       </c>
       <c r="I182" s="28" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D183" s="29">
         <v>7</v>
@@ -7372,18 +7372,18 @@
         <v>22</v>
       </c>
       <c r="I183" s="28" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A184" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B184" s="27" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D184" s="29">
         <v>0</v>
@@ -7401,18 +7401,18 @@
         <v>56</v>
       </c>
       <c r="I184" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A185" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B185" s="27" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D185" s="29">
         <v>100</v>
@@ -7430,18 +7430,18 @@
         <v>56</v>
       </c>
       <c r="I185" s="28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
+        <v>453</v>
+      </c>
+      <c r="B186" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="C186" s="6" t="s">
         <v>454</v>
-      </c>
-      <c r="B186" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="C186" s="6" t="s">
-        <v>455</v>
       </c>
       <c r="D186" s="39">
         <v>100</v>
@@ -7459,18 +7459,18 @@
         <v>22</v>
       </c>
       <c r="I186" s="13" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D187" s="12">
         <v>80</v>
@@ -7485,21 +7485,21 @@
         <v>44</v>
       </c>
       <c r="H187" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I187" s="13" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B188" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="C188" s="6" t="s">
         <v>458</v>
-      </c>
-      <c r="C188" s="6" t="s">
-        <v>459</v>
       </c>
       <c r="D188" s="12">
         <v>0</v>
@@ -7517,18 +7517,18 @@
         <v>22</v>
       </c>
       <c r="I188" s="13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B189" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D189" s="12">
         <v>0</v>
@@ -7546,18 +7546,18 @@
         <v>22</v>
       </c>
       <c r="I189" s="13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A190" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B190" s="27" t="s">
+        <v>464</v>
+      </c>
+      <c r="C190" s="28" t="s">
         <v>463</v>
-      </c>
-      <c r="B190" s="27" t="s">
-        <v>465</v>
-      </c>
-      <c r="C190" s="28" t="s">
-        <v>464</v>
       </c>
       <c r="D190" s="29">
         <v>90</v>
@@ -7575,18 +7575,18 @@
         <v>56</v>
       </c>
       <c r="I190" s="28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A191" s="27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B191" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="C191" s="28" t="s">
         <v>463</v>
-      </c>
-      <c r="B191" s="27" t="s">
-        <v>466</v>
-      </c>
-      <c r="C191" s="28" t="s">
-        <v>464</v>
       </c>
       <c r="D191" s="29">
         <v>50</v>
@@ -7604,7 +7604,7 @@
         <v>56</v>
       </c>
       <c r="I191" s="28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style, scen (instead of szen), clean up
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16FEB4A-6BE2-4CC3-A815-D0248A0AB169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE0E0F-6CDB-49CB-AE2F-AFC614BF2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1527,7 +1527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1561,6 +1561,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1606,7 +1618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1711,6 +1723,32 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2581,351 +2619,351 @@
         <v>477</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="32">
+      <c r="C18" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="39">
         <v>2010</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="39">
         <v>2010</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="39">
         <v>2010</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="31" t="s">
+      <c r="H18" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="40" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="32">
+      <c r="C19" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="39">
         <v>2021</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="39">
         <v>2021</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="39">
         <v>2021</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="31" t="s">
+      <c r="H19" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="40" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="32">
+      <c r="C20" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="39">
         <v>2010</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="39">
         <v>2010</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="39">
         <v>2010</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="31" t="s">
+      <c r="H20" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="40" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="32">
+      <c r="C21" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="39">
         <v>2021</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="39">
         <v>2021</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="39">
         <v>2021</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="31" t="s">
+      <c r="H21" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="40" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="32">
+      <c r="C22" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="39">
         <v>2010</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="39">
         <v>2010</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="39">
         <v>2010</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="31" t="s">
+      <c r="H22" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="32">
+      <c r="C23" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="39">
         <v>2021</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="39">
         <v>2021</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="39">
         <v>2021</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="31" t="s">
+      <c r="H23" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="40" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="32">
+      <c r="C24" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="43">
         <v>2010</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="43">
         <v>2010</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="43">
         <v>2010</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="31" t="s">
+      <c r="H24" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="44" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="32">
+      <c r="C25" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="43">
         <v>2021</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="43">
         <v>2021</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="43">
         <v>2021</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="31" t="s">
+      <c r="H25" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="44" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="32">
+      <c r="C26" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="43">
         <v>2010</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="43">
         <v>2010</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="43">
         <v>2010</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="31" t="s">
+      <c r="H26" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="44" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="32">
+      <c r="C27" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="43">
         <v>2021</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="43">
         <v>2021</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="43">
         <v>2021</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="31" t="s">
+      <c r="H27" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="44" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="32">
+      <c r="C28" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="43">
         <v>2010</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="43">
         <v>2010</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="43">
         <v>2010</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="31" t="s">
+      <c r="H28" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="44" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="32">
+      <c r="C29" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="43">
         <v>2021</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="43">
         <v>2021</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="43">
         <v>2021</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H29" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="31" t="s">
+      <c r="H29" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="44" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4380,7 +4418,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B80" s="11" t="s">
@@ -4409,7 +4447,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B81" s="11" t="s">
@@ -4438,7 +4476,7 @@
       </c>
     </row>
     <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B82" s="11" t="s">
@@ -4467,7 +4505,7 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B83" s="11" t="s">
@@ -4496,7 +4534,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B84" s="11" t="s">
@@ -4525,7 +4563,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B85" s="11" t="s">
@@ -4554,7 +4592,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B86" s="11" t="s">
@@ -4583,7 +4621,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B87" s="11" t="s">
@@ -4612,7 +4650,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B88" s="35" t="s">
@@ -4641,7 +4679,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B89" s="35" t="s">
@@ -4670,7 +4708,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B90" s="11" t="s">
@@ -4699,7 +4737,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B91" s="11" t="s">
@@ -4728,7 +4766,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B92" s="11" t="s">
@@ -4757,7 +4795,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B93" s="11" t="s">
@@ -4786,7 +4824,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="11" t="s">
+      <c r="A94" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B94" s="11" t="s">
@@ -4815,7 +4853,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="25" t="s">
+      <c r="A95" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B95" s="25" t="s">
@@ -4844,7 +4882,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B96" s="25" t="s">
@@ -4873,7 +4911,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B97" s="25" t="s">
@@ -4902,7 +4940,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="25" t="s">
+      <c r="A98" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B98" s="25" t="s">
@@ -4931,7 +4969,7 @@
       </c>
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A99" s="25" t="s">
+      <c r="A99" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B99" s="25" t="s">
@@ -4960,7 +4998,7 @@
       </c>
     </row>
     <row r="100" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A100" s="25" t="s">
+      <c r="A100" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B100" s="25" t="s">
@@ -4989,7 +5027,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A101" s="25" t="s">
+      <c r="A101" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B101" s="25" t="s">
@@ -5018,7 +5056,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A102" s="25" t="s">
+      <c r="A102" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B102" s="25" t="s">
@@ -5047,7 +5085,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A103" s="25" t="s">
+      <c r="A103" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B103" s="35" t="s">
@@ -5076,7 +5114,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A104" s="25" t="s">
+      <c r="A104" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B104" s="35" t="s">
@@ -5105,7 +5143,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A105" s="25" t="s">
+      <c r="A105" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B105" s="25" t="s">
@@ -5134,7 +5172,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A106" s="25" t="s">
+      <c r="A106" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B106" s="25" t="s">
@@ -5163,7 +5201,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A107" s="25" t="s">
+      <c r="A107" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B107" s="25" t="s">
@@ -5192,7 +5230,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A108" s="25" t="s">
+      <c r="A108" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B108" s="25" t="s">
@@ -5221,7 +5259,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A109" s="25" t="s">
+      <c r="A109" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B109" s="25" t="s">

</xml_diff>

<commit_message>
gam to LOESS, gather to pivot_to_long, style, cleanup
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFE0E0F-6CDB-49CB-AE2F-AFC614BF2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931EDB4D-6AC7-4DEB-8320-35AC8107F7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="486">
   <si>
     <t>parameter</t>
   </si>
@@ -1470,6 +1470,15 @@
   </si>
   <si>
     <t>the fertility rates of the past are compared with the predictions; the y-axis is limited (since the fertility rate of the past can be very large due to low population)</t>
+  </si>
+  <si>
+    <t>ims_span</t>
+  </si>
+  <si>
+    <t>proportion of data points used in the loess regressions of proportion by age; groups: district, year, sex, origin</t>
+  </si>
+  <si>
+    <t>ems_span</t>
   </si>
 </sst>
 </file>
@@ -2105,11 +2114,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I190"/>
+  <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4712,28 +4721,28 @@
         <v>144</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>156</v>
+        <v>483</v>
       </c>
       <c r="C90" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D90" s="12">
-        <v>5</v>
+        <v>0.08</v>
       </c>
       <c r="E90" s="12">
-        <v>5</v>
+        <v>0.08</v>
       </c>
       <c r="F90" s="12">
-        <v>5</v>
+        <v>0.08</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>157</v>
+        <v>484</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4741,36 +4750,36 @@
         <v>144</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C91" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D91" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E91" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F91" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>95</v>
@@ -4791,36 +4800,36 @@
         <v>22</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A93" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4828,57 +4837,57 @@
         <v>144</v>
       </c>
       <c r="B94" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D94" s="12">
+        <v>13</v>
+      </c>
+      <c r="E94" s="12">
+        <v>13</v>
+      </c>
+      <c r="F94" s="12">
+        <v>13</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A95" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D94" s="12">
-        <v>0</v>
-      </c>
-      <c r="E94" s="12">
-        <v>0</v>
-      </c>
-      <c r="F94" s="12">
-        <v>0</v>
-      </c>
-      <c r="G94" s="11" t="s">
+      <c r="C95" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D95" s="12">
+        <v>0</v>
+      </c>
+      <c r="E95" s="12">
+        <v>0</v>
+      </c>
+      <c r="F95" s="12">
+        <v>0</v>
+      </c>
+      <c r="G95" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H94" s="11" t="s">
+      <c r="H95" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="I95" s="13" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="47" t="s">
-        <v>181</v>
-      </c>
-      <c r="B95" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D95" s="26">
-        <v>20</v>
-      </c>
-      <c r="E95" s="26">
-        <v>20</v>
-      </c>
-      <c r="F95" s="26">
-        <v>20</v>
-      </c>
-      <c r="G95" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H95" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I95" s="30" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4886,10 +4895,10 @@
         <v>181</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D96" s="26">
         <v>20</v>
@@ -4907,7 +4916,7 @@
         <v>22</v>
       </c>
       <c r="I96" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4915,97 +4924,97 @@
         <v>181</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H97" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I97" s="30" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>95</v>
+        <v>209</v>
       </c>
       <c r="D98" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E98" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F98" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H98" s="25" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>210</v>
+        <v>95</v>
       </c>
       <c r="D99" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E99" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F99" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G99" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H99" s="25" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D100" s="26">
         <v>20</v>
@@ -5023,36 +5032,36 @@
         <v>22</v>
       </c>
       <c r="I100" s="30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A101" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C101" s="31" t="s">
-        <v>212</v>
+        <v>187</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="D101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H101" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5060,39 +5069,39 @@
         <v>181</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>95</v>
+        <v>188</v>
+      </c>
+      <c r="C102" s="31" t="s">
+        <v>212</v>
       </c>
       <c r="D102" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E102" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F102" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H102" s="25" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="B103" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="C103" s="30" t="s">
-        <v>213</v>
+      <c r="B103" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="D103" s="26">
         <v>0</v>
@@ -5104,13 +5113,13 @@
         <v>0</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="H103" s="25" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I103" s="30" t="s">
-        <v>200</v>
+        <v>142</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -5118,19 +5127,19 @@
         <v>181</v>
       </c>
       <c r="B104" s="35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C104" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G104" s="25" t="s">
         <v>93</v>
@@ -5139,94 +5148,94 @@
         <v>22</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="B105" s="25" t="s">
-        <v>192</v>
+      <c r="B105" s="35" t="s">
+        <v>191</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="D105" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E105" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="F105" s="26">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="H105" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I105" s="30" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C106" s="30" t="s">
         <v>95</v>
       </c>
       <c r="D106" s="26">
-        <v>20</v>
+        <v>0.08</v>
       </c>
       <c r="E106" s="26">
-        <v>20</v>
+        <v>0.08</v>
       </c>
       <c r="F106" s="26">
-        <v>20</v>
+        <v>0.08</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H106" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A107" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="C107" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C107" s="30" t="s">
         <v>95</v>
       </c>
       <c r="D107" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E107" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F107" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H107" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I107" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5234,144 +5243,144 @@
         <v>181</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G108" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H108" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I108" s="30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A109" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D109" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E109" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F109" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G109" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H109" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I109" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A110" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D110" s="26">
+        <v>13</v>
+      </c>
+      <c r="E110" s="26">
+        <v>13</v>
+      </c>
+      <c r="F110" s="26">
+        <v>13</v>
+      </c>
+      <c r="G110" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H110" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I110" s="30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A111" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D111" s="26">
+        <v>0</v>
+      </c>
+      <c r="E111" s="26">
+        <v>0</v>
+      </c>
+      <c r="F111" s="26">
+        <v>0</v>
+      </c>
+      <c r="G111" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H111" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I109" s="30" t="s">
+      <c r="I111" s="30" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D110" s="12">
-        <v>70</v>
-      </c>
-      <c r="E110" s="12">
-        <v>70</v>
-      </c>
-      <c r="F110" s="12">
-        <v>70</v>
-      </c>
-      <c r="G110" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H110" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I110" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="G111" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H111" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I111" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B112" s="11" t="s">
-        <v>242</v>
+      <c r="B112" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E112" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F112" s="6">
-        <v>0.2</v>
+        <v>220</v>
+      </c>
+      <c r="D112" s="12">
+        <v>70</v>
+      </c>
+      <c r="E112" s="12">
+        <v>70</v>
+      </c>
+      <c r="F112" s="12">
+        <v>70</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I112" s="11" t="s">
-        <v>228</v>
+        <v>22</v>
+      </c>
+      <c r="I112" s="13" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5379,19 +5388,19 @@
         <v>221</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>318</v>
+        <v>241</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>85</v>
@@ -5400,7 +5409,7 @@
         <v>59</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5408,19 +5417,19 @@
         <v>221</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D114" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E114" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F114" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>85</v>
@@ -5429,7 +5438,7 @@
         <v>59</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5437,28 +5446,28 @@
         <v>221</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="H115" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5466,19 +5475,19 @@
         <v>221</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>243</v>
+        <v>319</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D116" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E116" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="F116" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>85</v>
@@ -5487,65 +5496,65 @@
         <v>59</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>244</v>
+        <v>322</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D117" s="12">
-        <v>20</v>
-      </c>
-      <c r="E117" s="12">
-        <v>20</v>
-      </c>
-      <c r="F117" s="12">
-        <v>20</v>
+        <v>230</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="E117" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F117" s="6">
+        <v>0.4</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="H117" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I117" s="13" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I117" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D118" s="12">
-        <v>20</v>
-      </c>
-      <c r="E118" s="12">
-        <v>20</v>
-      </c>
-      <c r="F118" s="12">
-        <v>20</v>
+        <v>226</v>
+      </c>
+      <c r="D118" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E118" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F118" s="6">
+        <v>0.3</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I118" s="13" t="s">
-        <v>234</v>
+        <v>59</v>
+      </c>
+      <c r="I118" s="11" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5553,57 +5562,57 @@
         <v>221</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>95</v>
+        <v>237</v>
       </c>
       <c r="D119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H119" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I119" s="13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D120" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E120" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F120" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G120" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I120" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5611,144 +5620,144 @@
         <v>221</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D121" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="E121" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F121" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G121" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H121" s="11" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I121" s="13" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B122" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D122" s="12">
+        <v>0</v>
+      </c>
+      <c r="E122" s="12">
+        <v>0</v>
+      </c>
+      <c r="F122" s="12">
+        <v>0</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H122" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I122" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D123" s="12">
+        <v>100</v>
+      </c>
+      <c r="E123" s="12">
+        <v>100</v>
+      </c>
+      <c r="F123" s="12">
+        <v>100</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H123" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I123" s="13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B124" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="C124" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D124" s="6">
         <v>0.15</v>
       </c>
-      <c r="E122" s="6">
+      <c r="E124" s="6">
         <v>0.15</v>
       </c>
-      <c r="F122" s="6">
+      <c r="F124" s="6">
         <v>0.15</v>
       </c>
-      <c r="G122" s="11" t="s">
+      <c r="G124" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H122" s="11" t="s">
+      <c r="H124" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I122" s="11" t="s">
+      <c r="I124" s="11" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="D123" s="29">
-        <v>70</v>
-      </c>
-      <c r="E123" s="29">
-        <v>70</v>
-      </c>
-      <c r="F123" s="29">
-        <v>70</v>
-      </c>
-      <c r="G123" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H123" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I123" s="28" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="B124" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="G124" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H124" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I124" s="27" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="B125" s="27" t="s">
-        <v>251</v>
+      <c r="B125" s="14" t="s">
+        <v>259</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D125" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E125" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F125" s="14">
-        <v>0.2</v>
+        <v>220</v>
+      </c>
+      <c r="D125" s="29">
+        <v>70</v>
+      </c>
+      <c r="E125" s="29">
+        <v>70</v>
+      </c>
+      <c r="F125" s="29">
+        <v>70</v>
       </c>
       <c r="G125" s="27" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H125" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I125" s="27" t="s">
-        <v>228</v>
+        <v>22</v>
+      </c>
+      <c r="I125" s="28" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -5756,19 +5765,19 @@
         <v>250</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>324</v>
+        <v>262</v>
       </c>
       <c r="C126" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G126" s="27" t="s">
         <v>85</v>
@@ -5777,7 +5786,7 @@
         <v>59</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>326</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -5785,19 +5794,19 @@
         <v>250</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>325</v>
+        <v>251</v>
       </c>
       <c r="C127" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D127" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E127" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F127" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G127" s="27" t="s">
         <v>85</v>
@@ -5806,7 +5815,7 @@
         <v>59</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -5814,28 +5823,28 @@
         <v>250</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="H128" s="27" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5843,19 +5852,19 @@
         <v>250</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>252</v>
+        <v>325</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D129" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E129" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="F129" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="G129" s="27" t="s">
         <v>85</v>
@@ -5864,65 +5873,65 @@
         <v>59</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>253</v>
+        <v>327</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D130" s="29">
-        <v>20</v>
-      </c>
-      <c r="E130" s="29">
-        <v>20</v>
-      </c>
-      <c r="F130" s="29">
-        <v>20</v>
+        <v>229</v>
+      </c>
+      <c r="D130" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="E130" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F130" s="14">
+        <v>0.4</v>
       </c>
       <c r="G130" s="27" t="s">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="H130" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I130" s="28" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I130" s="27" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D131" s="29">
-        <v>20</v>
-      </c>
-      <c r="E131" s="29">
-        <v>20</v>
-      </c>
-      <c r="F131" s="29">
-        <v>20</v>
+        <v>226</v>
+      </c>
+      <c r="D131" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="E131" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F131" s="14">
+        <v>0.3</v>
       </c>
       <c r="G131" s="27" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H131" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I131" s="28" t="s">
-        <v>264</v>
+        <v>59</v>
+      </c>
+      <c r="I131" s="27" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5930,57 +5939,57 @@
         <v>250</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>95</v>
+        <v>237</v>
       </c>
       <c r="D132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G132" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H132" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I132" s="28" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A133" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C133" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D133" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E133" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F133" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G133" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H133" s="27" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I133" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5988,173 +5997,173 @@
         <v>250</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C134" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D134" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="E134" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F134" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G134" s="27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H134" s="27" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I134" s="28" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B135" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D135" s="29">
+        <v>0</v>
+      </c>
+      <c r="E135" s="29">
+        <v>0</v>
+      </c>
+      <c r="F135" s="29">
+        <v>0</v>
+      </c>
+      <c r="G135" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H135" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I135" s="28" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A136" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D136" s="29">
+        <v>100</v>
+      </c>
+      <c r="E136" s="29">
+        <v>100</v>
+      </c>
+      <c r="F136" s="29">
+        <v>100</v>
+      </c>
+      <c r="G136" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H136" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I136" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="B137" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="C135" s="14" t="s">
+      <c r="C137" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="D135" s="14">
+      <c r="D137" s="14">
         <v>0.15</v>
       </c>
-      <c r="E135" s="14">
+      <c r="E137" s="14">
         <v>0.15</v>
       </c>
-      <c r="F135" s="14">
+      <c r="F137" s="14">
         <v>0.15</v>
       </c>
-      <c r="G135" s="27" t="s">
+      <c r="G137" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="H135" s="27" t="s">
+      <c r="H137" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I135" s="27" t="s">
+      <c r="I137" s="27" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A136" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B136" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="G136" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H136" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I136" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A137" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B137" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D137" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="E137" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="F137" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="G137" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H137" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I137" s="11" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B138" s="11" t="s">
-        <v>281</v>
+      <c r="B138" s="37" t="s">
+        <v>279</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D138" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E138" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F138" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="H138" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B139" s="11" t="s">
-        <v>282</v>
+      <c r="B139" s="37" t="s">
+        <v>280</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D139" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E139" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F139" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>284</v>
+        <v>85</v>
       </c>
       <c r="H139" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -6162,28 +6171,28 @@
         <v>276</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D140" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E140" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F140" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="H140" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -6191,28 +6200,28 @@
         <v>276</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D141" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E141" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F141" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>85</v>
+        <v>284</v>
       </c>
       <c r="H141" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6220,19 +6229,19 @@
         <v>276</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>277</v>
       </c>
       <c r="D142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G142" s="11" t="s">
         <v>85</v>
@@ -6241,7 +6250,7 @@
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6249,7 +6258,7 @@
         <v>276</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>277</v>
@@ -6270,7 +6279,7 @@
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6278,28 +6287,28 @@
         <v>276</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="D144" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="E144" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="F144" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="G144" s="11" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H144" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6307,28 +6316,28 @@
         <v>276</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D145" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E145" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="F145" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G145" s="11" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H145" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -6336,28 +6345,28 @@
         <v>276</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>95</v>
+        <v>297</v>
       </c>
       <c r="D146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H146" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6365,19 +6374,19 @@
         <v>276</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D147" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E147" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F147" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G147" s="11" t="s">
         <v>44</v>
@@ -6386,7 +6395,7 @@
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -6394,28 +6403,28 @@
         <v>276</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D148" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="E148" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="F148" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="G148" s="11" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H148" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6423,28 +6432,28 @@
         <v>276</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D149" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E149" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F149" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G149" s="11" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="H149" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -6452,7 +6461,7 @@
         <v>276</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>277</v>
@@ -6473,7 +6482,7 @@
         <v>22</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -6481,28 +6490,28 @@
         <v>276</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D151" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="E151" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="F151" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>313</v>
+        <v>85</v>
       </c>
       <c r="H151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -6510,19 +6519,19 @@
         <v>276</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D152" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E152" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F152" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G152" s="11" t="s">
         <v>85</v>
@@ -6531,7 +6540,7 @@
         <v>22</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -6539,86 +6548,86 @@
         <v>276</v>
       </c>
       <c r="B153" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D153" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E153" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F153" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G153" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="H153" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I153" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D154" s="6">
+        <v>0</v>
+      </c>
+      <c r="E154" s="6">
+        <v>0</v>
+      </c>
+      <c r="F154" s="6">
+        <v>0</v>
+      </c>
+      <c r="G154" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H154" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I154" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B155" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="C153" s="6" t="s">
+      <c r="C155" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="D153" s="6">
+      <c r="D155" s="6">
         <v>0.1</v>
       </c>
-      <c r="E153" s="6">
+      <c r="E155" s="6">
         <v>0.1</v>
       </c>
-      <c r="F153" s="6">
+      <c r="F155" s="6">
         <v>0.1</v>
       </c>
-      <c r="G153" s="11" t="s">
+      <c r="G155" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H153" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I153" s="11" t="s">
+      <c r="H155" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I155" s="11" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="27" t="s">
-        <v>328</v>
-      </c>
-      <c r="B154" s="27" t="s">
-        <v>330</v>
-      </c>
-      <c r="C154" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="D154" s="29">
-        <v>25</v>
-      </c>
-      <c r="E154" s="29">
-        <v>25</v>
-      </c>
-      <c r="F154" s="29">
-        <v>25</v>
-      </c>
-      <c r="G154" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H154" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I154" s="28" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A155" s="27" t="s">
-        <v>328</v>
-      </c>
-      <c r="B155" s="27" t="s">
-        <v>335</v>
-      </c>
-      <c r="C155" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="D155" s="29">
-        <v>-25</v>
-      </c>
-      <c r="E155" s="29">
-        <v>0</v>
-      </c>
-      <c r="F155" s="29">
-        <v>25</v>
-      </c>
-      <c r="G155" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H155" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I155" s="28" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -6626,48 +6635,48 @@
         <v>328</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D156" s="29">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E156" s="29">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F156" s="29">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G156" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H156" s="27" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
         <v>328</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>95</v>
+        <v>331</v>
       </c>
       <c r="D157" s="29">
-        <v>85</v>
+        <v>-25</v>
       </c>
       <c r="E157" s="29">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="F157" s="29">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G157" s="27" t="s">
         <v>44</v>
@@ -6676,7 +6685,7 @@
         <v>46</v>
       </c>
       <c r="I157" s="28" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -6684,19 +6693,19 @@
         <v>328</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D158" s="29">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E158" s="29">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F158" s="29">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G158" s="27" t="s">
         <v>44</v>
@@ -6705,7 +6714,7 @@
         <v>46</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -6713,28 +6722,28 @@
         <v>328</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>334</v>
+        <v>95</v>
       </c>
       <c r="D159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G159" s="27" t="s">
-        <v>343</v>
+        <v>44</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="I159" s="28" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6742,173 +6751,173 @@
         <v>328</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D160" s="29">
-        <v>2044</v>
+        <v>75</v>
       </c>
       <c r="E160" s="29">
-        <v>2044</v>
+        <v>85</v>
       </c>
       <c r="F160" s="29">
-        <v>2044</v>
+        <v>90</v>
       </c>
       <c r="G160" s="27" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I160" s="28" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="27" t="s">
         <v>328</v>
       </c>
       <c r="B161" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C161" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="D161" s="29">
+        <v>0</v>
+      </c>
+      <c r="E161" s="29">
+        <v>0</v>
+      </c>
+      <c r="F161" s="29">
+        <v>0</v>
+      </c>
+      <c r="G161" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="H161" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I161" s="28" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="B162" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="C162" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="D162" s="29">
+        <v>2044</v>
+      </c>
+      <c r="E162" s="29">
+        <v>2044</v>
+      </c>
+      <c r="F162" s="29">
+        <v>2044</v>
+      </c>
+      <c r="G162" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H162" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I162" s="28" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A163" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="B163" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="C161" s="14" t="s">
+      <c r="C163" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="D161" s="29">
+      <c r="D163" s="29">
         <v>-0.04</v>
       </c>
-      <c r="E161" s="29">
+      <c r="E163" s="29">
         <v>-0.04</v>
       </c>
-      <c r="F161" s="29">
+      <c r="F163" s="29">
         <v>-0.04</v>
       </c>
-      <c r="G161" s="27" t="s">
+      <c r="G163" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="H161" s="27" t="s">
+      <c r="H163" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I161" s="28" t="s">
+      <c r="I163" s="28" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A162" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="D162" s="6">
-        <v>500</v>
-      </c>
-      <c r="E162" s="6">
-        <v>500</v>
-      </c>
-      <c r="F162" s="6">
-        <v>500</v>
-      </c>
-      <c r="G162" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="H162" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I162" s="11" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A163" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="B163" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="D163" s="12">
-        <v>20</v>
-      </c>
-      <c r="E163" s="12">
-        <v>20</v>
-      </c>
-      <c r="F163" s="12">
-        <v>20</v>
-      </c>
-      <c r="G163" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H163" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I163" s="13" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
         <v>361</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D164" s="12">
-        <v>20</v>
-      </c>
-      <c r="E164" s="12">
-        <v>20</v>
-      </c>
-      <c r="F164" s="12">
-        <v>20</v>
+        <v>363</v>
+      </c>
+      <c r="D164" s="6">
+        <v>500</v>
+      </c>
+      <c r="E164" s="6">
+        <v>500</v>
+      </c>
+      <c r="F164" s="6">
+        <v>500</v>
       </c>
       <c r="G164" s="11" t="s">
-        <v>44</v>
+        <v>364</v>
       </c>
       <c r="H164" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I164" s="13" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I164" s="11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
         <v>361</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G165" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H165" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I165" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -6916,19 +6925,19 @@
         <v>361</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>95</v>
+        <v>370</v>
       </c>
       <c r="D166" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E166" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F166" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G166" s="11" t="s">
         <v>44</v>
@@ -6937,143 +6946,143 @@
         <v>22</v>
       </c>
       <c r="I166" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D167" s="12">
+        <v>7</v>
+      </c>
+      <c r="E167" s="12">
+        <v>7</v>
+      </c>
+      <c r="F167" s="12">
+        <v>7</v>
+      </c>
+      <c r="G167" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H167" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I167" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A168" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D168" s="12">
+        <v>0</v>
+      </c>
+      <c r="E168" s="12">
+        <v>0</v>
+      </c>
+      <c r="F168" s="12">
+        <v>0</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H168" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I168" s="13" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="167" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="B167" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="C167" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="D167" s="10">
-        <v>500</v>
-      </c>
-      <c r="E167" s="10">
-        <v>500</v>
-      </c>
-      <c r="F167" s="10">
-        <v>500</v>
-      </c>
-      <c r="G167" s="25" t="s">
-        <v>364</v>
-      </c>
-      <c r="H167" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I167" s="25" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A168" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="B168" s="25" t="s">
-        <v>380</v>
-      </c>
-      <c r="C168" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="D168" s="26">
-        <v>20</v>
-      </c>
-      <c r="E168" s="26">
-        <v>20</v>
-      </c>
-      <c r="F168" s="26">
-        <v>20</v>
-      </c>
-      <c r="G168" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H168" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I168" s="30" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
         <v>377</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="D169" s="26">
-        <v>20</v>
-      </c>
-      <c r="E169" s="26">
-        <v>20</v>
-      </c>
-      <c r="F169" s="26">
-        <v>20</v>
+        <v>378</v>
+      </c>
+      <c r="D169" s="10">
+        <v>500</v>
+      </c>
+      <c r="E169" s="10">
+        <v>500</v>
+      </c>
+      <c r="F169" s="10">
+        <v>500</v>
       </c>
       <c r="G169" s="25" t="s">
-        <v>44</v>
+        <v>364</v>
       </c>
       <c r="H169" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I169" s="30" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I169" s="25" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A170" s="25" t="s">
         <v>377</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G170" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H170" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I170" s="30" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A171" s="25" t="s">
         <v>377</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>95</v>
+        <v>386</v>
       </c>
       <c r="D171" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E171" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F171" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G171" s="25" t="s">
         <v>44</v>
@@ -7082,123 +7091,123 @@
         <v>22</v>
       </c>
       <c r="I171" s="30" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="B172" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="C172" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D172" s="26">
+        <v>7</v>
+      </c>
+      <c r="E172" s="26">
+        <v>7</v>
+      </c>
+      <c r="F172" s="26">
+        <v>7</v>
+      </c>
+      <c r="G172" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H172" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I172" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A173" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="B173" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="C173" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D173" s="26">
+        <v>0</v>
+      </c>
+      <c r="E173" s="26">
+        <v>0</v>
+      </c>
+      <c r="F173" s="26">
+        <v>0</v>
+      </c>
+      <c r="G173" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H173" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I173" s="30" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A172" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="D172" s="12">
-        <v>2</v>
-      </c>
-      <c r="E172" s="12">
-        <v>2</v>
-      </c>
-      <c r="F172" s="12">
-        <v>2</v>
-      </c>
-      <c r="G172" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H172" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I172" s="13" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A173" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B173" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="D173" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="E173" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="F173" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="G173" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H173" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I173" s="13" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
         <v>400</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="D174" s="36">
-        <v>80</v>
-      </c>
-      <c r="E174" s="36">
-        <v>80</v>
-      </c>
-      <c r="F174" s="36">
-        <v>80</v>
+        <v>402</v>
+      </c>
+      <c r="D174" s="12">
+        <v>2</v>
+      </c>
+      <c r="E174" s="12">
+        <v>2</v>
+      </c>
+      <c r="F174" s="12">
+        <v>2</v>
       </c>
       <c r="G174" s="11" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="H174" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I174" s="13" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
         <v>400</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="D175" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E175" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F175" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G175" s="11" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="H175" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -7206,19 +7215,19 @@
         <v>400</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="D176" s="12">
-        <v>0</v>
-      </c>
-      <c r="E176" s="12">
-        <v>0</v>
-      </c>
-      <c r="F176" s="12">
-        <v>0</v>
+        <v>407</v>
+      </c>
+      <c r="D176" s="36">
+        <v>80</v>
+      </c>
+      <c r="E176" s="36">
+        <v>80</v>
+      </c>
+      <c r="F176" s="36">
+        <v>80</v>
       </c>
       <c r="G176" s="11" t="s">
         <v>44</v>
@@ -7235,10 +7244,10 @@
         <v>400</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D177" s="12">
         <v>0</v>
@@ -7264,10 +7273,10 @@
         <v>400</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D178" s="12">
         <v>0</v>
@@ -7293,19 +7302,19 @@
         <v>400</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G179" s="11" t="s">
         <v>44</v>
@@ -7317,91 +7326,91 @@
         <v>419</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A180" s="27" t="s">
-        <v>428</v>
-      </c>
-      <c r="B180" s="27" t="s">
-        <v>429</v>
-      </c>
-      <c r="C180" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="D180" s="29">
-        <v>50</v>
-      </c>
-      <c r="E180" s="29">
-        <v>50</v>
-      </c>
-      <c r="F180" s="29">
-        <v>50</v>
-      </c>
-      <c r="G180" s="27" t="s">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A180" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B180" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="D180" s="12">
+        <v>0</v>
+      </c>
+      <c r="E180" s="12">
+        <v>0</v>
+      </c>
+      <c r="F180" s="12">
+        <v>0</v>
+      </c>
+      <c r="G180" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H180" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I180" s="28" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A181" s="27" t="s">
-        <v>428</v>
-      </c>
-      <c r="B181" s="27" t="s">
-        <v>430</v>
-      </c>
-      <c r="C181" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="D181" s="29">
-        <v>20</v>
-      </c>
-      <c r="E181" s="29">
-        <v>20</v>
-      </c>
-      <c r="F181" s="29">
-        <v>20</v>
-      </c>
-      <c r="G181" s="27" t="s">
+      <c r="H180" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I180" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A181" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B181" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D181" s="12">
+        <v>20</v>
+      </c>
+      <c r="E181" s="12">
+        <v>20</v>
+      </c>
+      <c r="F181" s="12">
+        <v>20</v>
+      </c>
+      <c r="G181" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H181" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I181" s="28" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H181" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I181" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A182" s="27" t="s">
         <v>428</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D182" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E182" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F182" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="G182" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H182" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I182" s="28" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -7409,135 +7418,135 @@
         <v>428</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>95</v>
+        <v>435</v>
       </c>
       <c r="D183" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E183" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F183" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G183" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H183" s="27" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I183" s="28" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="27" t="s">
         <v>428</v>
       </c>
       <c r="B184" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="C184" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="D184" s="29">
+        <v>7</v>
+      </c>
+      <c r="E184" s="29">
+        <v>7</v>
+      </c>
+      <c r="F184" s="29">
+        <v>7</v>
+      </c>
+      <c r="G184" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H184" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I184" s="28" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A185" s="27" t="s">
+        <v>428</v>
+      </c>
+      <c r="B185" s="27" t="s">
+        <v>432</v>
+      </c>
+      <c r="C185" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D185" s="29">
+        <v>0</v>
+      </c>
+      <c r="E185" s="29">
+        <v>0</v>
+      </c>
+      <c r="F185" s="29">
+        <v>0</v>
+      </c>
+      <c r="G185" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H185" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I185" s="28" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A186" s="27" t="s">
+        <v>428</v>
+      </c>
+      <c r="B186" s="27" t="s">
         <v>433</v>
       </c>
-      <c r="C184" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D184" s="29">
+      <c r="C186" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D186" s="29">
         <v>100</v>
       </c>
-      <c r="E184" s="29">
+      <c r="E186" s="29">
         <v>100</v>
       </c>
-      <c r="F184" s="29">
+      <c r="F186" s="29">
         <v>100</v>
       </c>
-      <c r="G184" s="27" t="s">
+      <c r="G186" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H184" s="27" t="s">
+      <c r="H186" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I184" s="28" t="s">
+      <c r="I186" s="28" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A185" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="B185" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="C185" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D185" s="36">
-        <v>100</v>
-      </c>
-      <c r="E185" s="36">
-        <v>100</v>
-      </c>
-      <c r="F185" s="36">
-        <v>100</v>
-      </c>
-      <c r="G185" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H185" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I185" s="13" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A186" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="B186" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="C186" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D186" s="12">
-        <v>80</v>
-      </c>
-      <c r="E186" s="12">
-        <v>80</v>
-      </c>
-      <c r="F186" s="12">
-        <v>80</v>
-      </c>
-      <c r="G186" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H186" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I186" s="13" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
         <v>446</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="D187" s="12">
-        <v>0</v>
-      </c>
-      <c r="E187" s="12">
-        <v>0</v>
-      </c>
-      <c r="F187" s="12">
-        <v>0</v>
+        <v>447</v>
+      </c>
+      <c r="D187" s="36">
+        <v>100</v>
+      </c>
+      <c r="E187" s="36">
+        <v>100</v>
+      </c>
+      <c r="F187" s="36">
+        <v>100</v>
       </c>
       <c r="G187" s="11" t="s">
         <v>44</v>
@@ -7546,93 +7555,151 @@
         <v>22</v>
       </c>
       <c r="I187" s="13" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
         <v>446</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>451</v>
+        <v>95</v>
       </c>
       <c r="D188" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E188" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F188" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G188" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H188" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I188" s="13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B189" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D189" s="12">
+        <v>0</v>
+      </c>
+      <c r="E189" s="12">
+        <v>0</v>
+      </c>
+      <c r="F189" s="12">
+        <v>0</v>
+      </c>
+      <c r="G189" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H189" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I189" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A190" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B190" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D190" s="12">
+        <v>0</v>
+      </c>
+      <c r="E190" s="12">
+        <v>0</v>
+      </c>
+      <c r="F190" s="12">
+        <v>0</v>
+      </c>
+      <c r="G190" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H190" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I190" s="13" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A189" s="27" t="s">
+    <row r="191" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A191" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="B189" s="27" t="s">
+      <c r="B191" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="C189" s="28" t="s">
+      <c r="C191" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="D189" s="29">
+      <c r="D191" s="29">
         <v>90</v>
       </c>
-      <c r="E189" s="29">
+      <c r="E191" s="29">
         <v>90</v>
       </c>
-      <c r="F189" s="29">
+      <c r="F191" s="29">
         <v>90</v>
       </c>
-      <c r="G189" s="27" t="s">
+      <c r="G191" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H189" s="27" t="s">
+      <c r="H191" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I189" s="28" t="s">
+      <c r="I191" s="28" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A190" s="27" t="s">
+    <row r="192" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A192" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="B190" s="27" t="s">
+      <c r="B192" s="27" t="s">
         <v>458</v>
       </c>
-      <c r="C190" s="28" t="s">
+      <c r="C192" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="D190" s="29">
+      <c r="D192" s="29">
         <v>50</v>
       </c>
-      <c r="E190" s="29">
+      <c r="E192" s="29">
         <v>50</v>
       </c>
-      <c r="F190" s="29">
+      <c r="F192" s="29">
         <v>50</v>
       </c>
-      <c r="G190" s="27" t="s">
+      <c r="G192" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H190" s="27" t="s">
+      <c r="H192" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I190" s="28" t="s">
+      <c r="I192" s="28" t="s">
         <v>462</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replace moving average (for migration* over years) by a LOESS model
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60098D02-7091-4408-92C2-5970DBDC3E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79BBAFD-D7CD-45B3-89CC-06D73EB283E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="475">
   <si>
     <t>parameter</t>
   </si>
@@ -477,12 +477,6 @@
     <t>ims_so_lower_thres</t>
   </si>
   <si>
-    <t>ims_age_window_years</t>
-  </si>
-  <si>
-    <t>immigration*, age distribution: moving average window over years (to calculate mean immigrations* per district, age, sex, origin over the given window of years)</t>
-  </si>
-  <si>
     <t>ims_age_thres_percent</t>
   </si>
   <si>
@@ -1436,13 +1430,22 @@
     <t>the fertility rates of the past are compared with the predictions; the y-axis is limited (since the fertility rate of the past can be very large due to low population)</t>
   </si>
   <si>
-    <t>ims_span</t>
-  </si>
-  <si>
     <t>proportion of data points used in the loess regressions of proportion by age; groups: district, year, sex, origin</t>
   </si>
   <si>
     <t>ems_span</t>
+  </si>
+  <si>
+    <t>ims_span_y</t>
+  </si>
+  <si>
+    <t>ims_span_a</t>
+  </si>
+  <si>
+    <t>proportion of data points used in the loess regressions of proportion by year; groups: district, age, sex, origin (immigrations* by district, year, age, sex, origin)</t>
+  </si>
+  <si>
+    <t>proportion of data points used in the loess regressions of proportion by age; groups: district, year, sex, origin (age proportion by district, year, sex, origin)</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1503,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1549,6 +1552,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1591,7 +1600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1721,6 +1730,16 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1730,9 +1749,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FF9999FF"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FFFFCCFF"/>
@@ -2078,8 +2097,8 @@
   <dimension ref="A1:I188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2110,7 +2129,7 @@
         <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>10</v>
@@ -2122,7 +2141,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2188,7 +2207,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>50</v>
@@ -2217,7 +2236,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>51</v>
@@ -2557,7 +2576,7 @@
         <v>22</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2586,7 +2605,7 @@
         <v>22</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" x14ac:dyDescent="0.2">
@@ -2768,7 +2787,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>95</v>
@@ -2789,7 +2808,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -2797,7 +2816,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C25" s="41" t="s">
         <v>95</v>
@@ -2818,7 +2837,7 @@
         <v>22</v>
       </c>
       <c r="I25" s="43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -2826,7 +2845,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C26" s="41" t="s">
         <v>95</v>
@@ -2847,7 +2866,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="43" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -2855,7 +2874,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C27" s="41" t="s">
         <v>95</v>
@@ -2876,7 +2895,7 @@
         <v>22</v>
       </c>
       <c r="I27" s="43" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -2884,7 +2903,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C28" s="41" t="s">
         <v>95</v>
@@ -2905,7 +2924,7 @@
         <v>22</v>
       </c>
       <c r="I28" s="43" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -2913,7 +2932,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>95</v>
@@ -2934,7 +2953,7 @@
         <v>22</v>
       </c>
       <c r="I29" s="43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2942,7 +2961,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>95</v>
@@ -2963,7 +2982,7 @@
         <v>22</v>
       </c>
       <c r="I30" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -2971,7 +2990,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>95</v>
@@ -2992,7 +3011,7 @@
         <v>22</v>
       </c>
       <c r="I31" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3000,7 +3019,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>95</v>
@@ -3021,7 +3040,7 @@
         <v>22</v>
       </c>
       <c r="I32" s="31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3029,7 +3048,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>95</v>
@@ -3050,7 +3069,7 @@
         <v>22</v>
       </c>
       <c r="I33" s="31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3058,7 +3077,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>95</v>
@@ -3079,7 +3098,7 @@
         <v>22</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3087,7 +3106,7 @@
         <v>19</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>95</v>
@@ -3108,7 +3127,7 @@
         <v>22</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3116,7 +3135,7 @@
         <v>19</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>95</v>
@@ -3137,7 +3156,7 @@
         <v>22</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3145,7 +3164,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>95</v>
@@ -3166,7 +3185,7 @@
         <v>22</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3174,7 +3193,7 @@
         <v>19</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>95</v>
@@ -3195,7 +3214,7 @@
         <v>22</v>
       </c>
       <c r="I38" s="31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3203,7 +3222,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>95</v>
@@ -3224,7 +3243,7 @@
         <v>22</v>
       </c>
       <c r="I39" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3232,7 +3251,7 @@
         <v>19</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>95</v>
@@ -3253,7 +3272,7 @@
         <v>22</v>
       </c>
       <c r="I40" s="31" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3261,7 +3280,7 @@
         <v>19</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>95</v>
@@ -3282,7 +3301,7 @@
         <v>22</v>
       </c>
       <c r="I41" s="31" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3290,10 +3309,10 @@
         <v>19</v>
       </c>
       <c r="B42" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>408</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>410</v>
       </c>
       <c r="D42" s="32">
         <v>2022</v>
@@ -3311,7 +3330,7 @@
         <v>22</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3319,10 +3338,10 @@
         <v>19</v>
       </c>
       <c r="B43" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>409</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>411</v>
       </c>
       <c r="D43" s="32">
         <v>2029</v>
@@ -3340,7 +3359,7 @@
         <v>22</v>
       </c>
       <c r="I43" s="31" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3348,7 +3367,7 @@
         <v>19</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>95</v>
@@ -3369,7 +3388,7 @@
         <v>22</v>
       </c>
       <c r="I44" s="31" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3377,7 +3396,7 @@
         <v>19</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>95</v>
@@ -3398,15 +3417,15 @@
         <v>22</v>
       </c>
       <c r="I45" s="31" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>95</v>
@@ -3432,10 +3451,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>95</v>
@@ -3522,7 +3541,7 @@
         <v>60</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>95</v>
@@ -3537,13 +3556,13 @@
         <v>4</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H50" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I50" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3551,7 +3570,7 @@
         <v>60</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>95</v>
@@ -3566,13 +3585,13 @@
         <v>0</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H51" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3580,7 +3599,7 @@
         <v>60</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>95</v>
@@ -3595,13 +3614,13 @@
         <v>4</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H52" s="27" t="s">
         <v>56</v>
       </c>
       <c r="I52" s="28" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3688,7 +3707,7 @@
         <v>22</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3717,7 +3736,7 @@
         <v>22</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -3746,7 +3765,7 @@
         <v>22</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3783,7 +3802,7 @@
         <v>20</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>95</v>
@@ -3804,7 +3823,7 @@
         <v>22</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -3914,7 +3933,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>22</v>
@@ -3943,7 +3962,7 @@
         <v>80</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>22</v>
@@ -3972,13 +3991,13 @@
         <v>30</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H65" s="11" t="s">
         <v>56</v>
       </c>
       <c r="I65" s="13" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3986,7 +4005,7 @@
         <v>20</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>95</v>
@@ -4007,7 +4026,7 @@
         <v>22</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4152,7 +4171,7 @@
         <v>22</v>
       </c>
       <c r="I71" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4181,7 +4200,7 @@
         <v>22</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4210,7 +4229,7 @@
         <v>22</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4239,7 +4258,7 @@
         <v>22</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -4297,7 +4316,7 @@
         <v>56</v>
       </c>
       <c r="I76" s="20" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4363,7 +4382,7 @@
         <v>92</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>95</v>
@@ -4384,7 +4403,7 @@
         <v>22</v>
       </c>
       <c r="I79" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4558,7 +4577,7 @@
         <v>22</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -4630,13 +4649,13 @@
         <v>95</v>
       </c>
       <c r="D88" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="E88" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F88" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G88" s="11" t="s">
         <v>85</v>
@@ -4645,7 +4664,7 @@
         <v>22</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4653,28 +4672,28 @@
         <v>144</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>152</v>
+        <v>472</v>
       </c>
       <c r="C89" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D89" s="12">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="E89" s="12">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="F89" s="12">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>153</v>
+        <v>474</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4682,7 +4701,7 @@
         <v>144</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>95</v>
@@ -4703,7 +4722,7 @@
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -4711,7 +4730,7 @@
         <v>144</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>95</v>
@@ -4732,7 +4751,7 @@
         <v>22</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4740,7 +4759,7 @@
         <v>144</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>95</v>
@@ -4761,7 +4780,7 @@
         <v>22</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4769,7 +4788,7 @@
         <v>144</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>95</v>
@@ -4790,18 +4809,18 @@
         <v>56</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D94" s="26">
         <v>20</v>
@@ -4819,18 +4838,18 @@
         <v>22</v>
       </c>
       <c r="I94" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="B95" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="B95" s="25" t="s">
-        <v>177</v>
-      </c>
       <c r="C95" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D95" s="26">
         <v>20</v>
@@ -4848,18 +4867,18 @@
         <v>22</v>
       </c>
       <c r="I95" s="30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D96" s="26">
         <v>13</v>
@@ -4877,15 +4896,15 @@
         <v>22</v>
       </c>
       <c r="I96" s="30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>95</v>
@@ -4911,13 +4930,13 @@
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D98" s="26">
         <v>20</v>
@@ -4940,13 +4959,13 @@
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A99" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D99" s="26">
         <v>20</v>
@@ -4964,18 +4983,18 @@
         <v>22</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D100" s="26">
         <v>13</v>
@@ -4998,10 +5017,10 @@
     </row>
     <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>95</v>
@@ -5027,10 +5046,10 @@
     </row>
     <row r="102" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C102" s="30" t="s">
         <v>95</v>
@@ -5051,44 +5070,44 @@
         <v>22</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="B103" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C103" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D103" s="26">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="50" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A103" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="B103" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D103" s="49">
         <v>5</v>
       </c>
-      <c r="E103" s="26">
+      <c r="E103" s="49">
         <v>5</v>
       </c>
-      <c r="F103" s="26">
+      <c r="F103" s="49">
         <v>5</v>
       </c>
-      <c r="G103" s="25" t="s">
+      <c r="G103" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H103" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I103" s="30" t="s">
-        <v>192</v>
+      <c r="H103" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I103" s="48" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>95</v>
@@ -5109,15 +5128,15 @@
         <v>22</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>95</v>
@@ -5138,15 +5157,15 @@
         <v>22</v>
       </c>
       <c r="I105" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>95</v>
@@ -5167,15 +5186,15 @@
         <v>22</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A107" s="46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>95</v>
@@ -5196,18 +5215,18 @@
         <v>56</v>
       </c>
       <c r="I107" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D108" s="12">
         <v>70</v>
@@ -5225,18 +5244,18 @@
         <v>22</v>
       </c>
       <c r="I108" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D109" s="6">
         <v>0.2</v>
@@ -5254,18 +5273,18 @@
         <v>59</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D110" s="6">
         <v>0.2</v>
@@ -5283,18 +5302,18 @@
         <v>59</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D111" s="6">
         <v>0.12</v>
@@ -5312,18 +5331,18 @@
         <v>59</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D112" s="6">
         <v>0.12</v>
@@ -5341,18 +5360,18 @@
         <v>59</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D113" s="6">
         <v>0.4</v>
@@ -5364,24 +5383,24 @@
         <v>0.4</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H113" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D114" s="6">
         <v>0.3</v>
@@ -5399,18 +5418,18 @@
         <v>59</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D115" s="12">
         <v>20</v>
@@ -5428,15 +5447,15 @@
         <v>22</v>
       </c>
       <c r="I115" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>95</v>
@@ -5457,15 +5476,15 @@
         <v>22</v>
       </c>
       <c r="I116" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>95</v>
@@ -5486,15 +5505,15 @@
         <v>22</v>
       </c>
       <c r="I117" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>95</v>
@@ -5515,15 +5534,15 @@
         <v>56</v>
       </c>
       <c r="I118" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>95</v>
@@ -5544,18 +5563,18 @@
         <v>56</v>
       </c>
       <c r="I119" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D120" s="6">
         <v>0.15</v>
@@ -5573,18 +5592,18 @@
         <v>59</v>
       </c>
       <c r="I120" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D121" s="29">
         <v>70</v>
@@ -5602,18 +5621,18 @@
         <v>22</v>
       </c>
       <c r="I121" s="28" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D122" s="14">
         <v>0.2</v>
@@ -5631,18 +5650,18 @@
         <v>59</v>
       </c>
       <c r="I122" s="27" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B123" s="27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D123" s="14">
         <v>0.2</v>
@@ -5660,18 +5679,18 @@
         <v>59</v>
       </c>
       <c r="I123" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D124" s="14">
         <v>0.12</v>
@@ -5689,18 +5708,18 @@
         <v>59</v>
       </c>
       <c r="I124" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D125" s="14">
         <v>0.12</v>
@@ -5718,18 +5737,18 @@
         <v>59</v>
       </c>
       <c r="I125" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D126" s="14">
         <v>0.4</v>
@@ -5741,24 +5760,24 @@
         <v>0.4</v>
       </c>
       <c r="G126" s="27" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H126" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B127" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="B127" s="27" t="s">
-        <v>240</v>
-      </c>
       <c r="C127" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D127" s="14">
         <v>0.3</v>
@@ -5776,18 +5795,18 @@
         <v>59</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A128" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D128" s="29">
         <v>20</v>
@@ -5805,15 +5824,15 @@
         <v>22</v>
       </c>
       <c r="I128" s="28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A129" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>95</v>
@@ -5834,15 +5853,15 @@
         <v>22</v>
       </c>
       <c r="I129" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C130" s="14" t="s">
         <v>95</v>
@@ -5863,15 +5882,15 @@
         <v>22</v>
       </c>
       <c r="I130" s="28" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C131" s="14" t="s">
         <v>95</v>
@@ -5892,15 +5911,15 @@
         <v>56</v>
       </c>
       <c r="I131" s="28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A132" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C132" s="14" t="s">
         <v>95</v>
@@ -5921,18 +5940,18 @@
         <v>56</v>
       </c>
       <c r="I132" s="28" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C133" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D133" s="14">
         <v>0.15</v>
@@ -5950,18 +5969,18 @@
         <v>59</v>
       </c>
       <c r="I133" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B134" s="36" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D134" s="6">
         <v>0.1</v>
@@ -5979,18 +5998,18 @@
         <v>22</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B135" s="36" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D135" s="6">
         <v>0.15</v>
@@ -6008,18 +6027,18 @@
         <v>22</v>
       </c>
       <c r="I135" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B136" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C136" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="D136" s="6">
         <v>0.5</v>
@@ -6037,47 +6056,47 @@
         <v>22</v>
       </c>
       <c r="I136" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B137" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D137" s="6">
+        <v>0</v>
+      </c>
+      <c r="E137" s="6">
+        <v>0</v>
+      </c>
+      <c r="F137" s="6">
+        <v>0</v>
+      </c>
+      <c r="G137" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="C137" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D137" s="6">
-        <v>0</v>
-      </c>
-      <c r="E137" s="6">
-        <v>0</v>
-      </c>
-      <c r="F137" s="6">
-        <v>0</v>
-      </c>
-      <c r="G137" s="11" t="s">
-        <v>272</v>
-      </c>
       <c r="H137" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D138" s="6">
         <v>0.1</v>
@@ -6095,18 +6114,18 @@
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D139" s="6">
         <v>0.1</v>
@@ -6124,18 +6143,18 @@
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D140" s="6">
         <v>0.15</v>
@@ -6153,18 +6172,18 @@
         <v>22</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D141" s="6">
         <v>0.1</v>
@@ -6182,18 +6201,18 @@
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D142" s="6">
         <v>20</v>
@@ -6211,15 +6230,15 @@
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>95</v>
@@ -6240,15 +6259,15 @@
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>95</v>
@@ -6269,15 +6288,15 @@
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C145" s="6" t="s">
         <v>95</v>
@@ -6298,18 +6317,18 @@
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D146" s="6">
         <v>0.1</v>
@@ -6327,18 +6346,18 @@
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D147" s="6">
         <v>0.15</v>
@@ -6356,18 +6375,18 @@
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D148" s="6">
         <v>0.1</v>
@@ -6385,15 +6404,15 @@
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>95</v>
@@ -6408,21 +6427,21 @@
         <v>0.5</v>
       </c>
       <c r="G149" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H149" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>95</v>
@@ -6443,18 +6462,18 @@
         <v>22</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D151" s="6">
         <v>0.1</v>
@@ -6472,18 +6491,18 @@
         <v>22</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="B152" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="B152" s="27" t="s">
-        <v>318</v>
-      </c>
       <c r="C152" s="14" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D152" s="29">
         <v>25</v>
@@ -6501,18 +6520,18 @@
         <v>59</v>
       </c>
       <c r="I152" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A153" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B153" s="27" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D153" s="29">
         <v>-25</v>
@@ -6530,18 +6549,18 @@
         <v>46</v>
       </c>
       <c r="I153" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B154" s="27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D154" s="29">
         <v>0</v>
@@ -6559,15 +6578,15 @@
         <v>46</v>
       </c>
       <c r="I154" s="28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C155" s="14" t="s">
         <v>95</v>
@@ -6588,18 +6607,18 @@
         <v>46</v>
       </c>
       <c r="I155" s="28" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D156" s="29">
         <v>75</v>
@@ -6617,18 +6636,18 @@
         <v>46</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D157" s="29">
         <v>0</v>
@@ -6640,24 +6659,24 @@
         <v>0</v>
       </c>
       <c r="G157" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H157" s="27" t="s">
         <v>59</v>
       </c>
       <c r="I157" s="28" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D158" s="29">
         <v>2044</v>
@@ -6675,18 +6694,18 @@
         <v>22</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A159" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D159" s="29">
         <v>-0.04</v>
@@ -6704,18 +6723,18 @@
         <v>46</v>
       </c>
       <c r="I159" s="28" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="B160" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="C160" s="6" t="s">
         <v>349</v>
-      </c>
-      <c r="B160" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="D160" s="6">
         <v>500</v>
@@ -6727,24 +6746,24 @@
         <v>500</v>
       </c>
       <c r="G160" s="11" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H160" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I160" s="11" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D161" s="12">
         <v>20</v>
@@ -6762,18 +6781,18 @@
         <v>22</v>
       </c>
       <c r="I161" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D162" s="12">
         <v>20</v>
@@ -6791,18 +6810,18 @@
         <v>22</v>
       </c>
       <c r="I162" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D163" s="12">
         <v>7</v>
@@ -6820,15 +6839,15 @@
         <v>22</v>
       </c>
       <c r="I163" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C164" s="6" t="s">
         <v>95</v>
@@ -6849,18 +6868,18 @@
         <v>22</v>
       </c>
       <c r="I164" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="165" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="B165" s="25" t="s">
         <v>365</v>
       </c>
-      <c r="B165" s="25" t="s">
-        <v>367</v>
-      </c>
       <c r="C165" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D165" s="10">
         <v>500</v>
@@ -6872,24 +6891,24 @@
         <v>500</v>
       </c>
       <c r="G165" s="25" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H165" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I165" s="25" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="166" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A166" s="25" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B166" s="25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D166" s="26">
         <v>20</v>
@@ -6907,18 +6926,18 @@
         <v>22</v>
       </c>
       <c r="I166" s="30" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A167" s="25" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B167" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D167" s="26">
         <v>20</v>
@@ -6936,18 +6955,18 @@
         <v>22</v>
       </c>
       <c r="I167" s="30" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="25" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B168" s="25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C168" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D168" s="26">
         <v>7</v>
@@ -6965,15 +6984,15 @@
         <v>22</v>
       </c>
       <c r="I168" s="30" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="169" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C169" s="10" t="s">
         <v>95</v>
@@ -6994,18 +7013,18 @@
         <v>22</v>
       </c>
       <c r="I169" s="30" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="B170" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="C170" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="B170" s="11" t="s">
-        <v>389</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>390</v>
       </c>
       <c r="D170" s="12">
         <v>2</v>
@@ -7023,18 +7042,18 @@
         <v>22</v>
       </c>
       <c r="I170" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A171" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D171" s="12">
         <v>0.05</v>
@@ -7052,18 +7071,18 @@
         <v>22</v>
       </c>
       <c r="I171" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D172" s="35">
         <v>80</v>
@@ -7081,18 +7100,18 @@
         <v>22</v>
       </c>
       <c r="I172" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D173" s="12">
         <v>0</v>
@@ -7110,18 +7129,18 @@
         <v>22</v>
       </c>
       <c r="I173" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D174" s="12">
         <v>0</v>
@@ -7139,18 +7158,18 @@
         <v>22</v>
       </c>
       <c r="I174" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D175" s="12">
         <v>0</v>
@@ -7168,18 +7187,18 @@
         <v>22</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D176" s="12">
         <v>0</v>
@@ -7197,18 +7216,18 @@
         <v>22</v>
       </c>
       <c r="I176" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D177" s="12">
         <v>20</v>
@@ -7226,18 +7245,18 @@
         <v>22</v>
       </c>
       <c r="I177" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A178" s="27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B178" s="27" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D178" s="29">
         <v>50</v>
@@ -7255,18 +7274,18 @@
         <v>22</v>
       </c>
       <c r="I178" s="28" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A179" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="B179" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="B179" s="27" t="s">
-        <v>418</v>
-      </c>
       <c r="C179" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D179" s="29">
         <v>20</v>
@@ -7284,18 +7303,18 @@
         <v>22</v>
       </c>
       <c r="I179" s="28" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B180" s="27" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D180" s="29">
         <v>7</v>
@@ -7313,15 +7332,15 @@
         <v>22</v>
       </c>
       <c r="I180" s="28" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A181" s="27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B181" s="27" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C181" s="14" t="s">
         <v>95</v>
@@ -7342,15 +7361,15 @@
         <v>56</v>
       </c>
       <c r="I181" s="28" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A182" s="27" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C182" s="14" t="s">
         <v>95</v>
@@ -7371,18 +7390,18 @@
         <v>56</v>
       </c>
       <c r="I182" s="28" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="B183" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="B183" s="11" t="s">
-        <v>436</v>
-      </c>
       <c r="C183" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D183" s="35">
         <v>100</v>
@@ -7400,15 +7419,15 @@
         <v>22</v>
       </c>
       <c r="I183" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A184" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C184" s="6" t="s">
         <v>95</v>
@@ -7429,18 +7448,18 @@
         <v>59</v>
       </c>
       <c r="I184" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D185" s="12">
         <v>0</v>
@@ -7458,18 +7477,18 @@
         <v>22</v>
       </c>
       <c r="I185" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D186" s="12">
         <v>0</v>
@@ -7487,18 +7506,18 @@
         <v>22</v>
       </c>
       <c r="I186" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A187" s="27" t="s">
+        <v>441</v>
+      </c>
+      <c r="B187" s="27" t="s">
         <v>443</v>
       </c>
-      <c r="B187" s="27" t="s">
-        <v>445</v>
-      </c>
       <c r="C187" s="28" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D187" s="29">
         <v>90</v>
@@ -7516,18 +7535,18 @@
         <v>56</v>
       </c>
       <c r="I187" s="28" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A188" s="27" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B188" s="27" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C188" s="28" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D188" s="29">
         <v>50</v>
@@ -7545,7 +7564,7 @@
         <v>56</v>
       </c>
       <c r="I188" s="28" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes after review (new parameters)
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16FEB4A-6BE2-4CC3-A815-D0248A0AB169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="489">
   <si>
     <t>parameter</t>
   </si>
@@ -1470,12 +1469,30 @@
   </si>
   <si>
     <t>the fertility rates of the past are compared with the predictions; the y-axis is limited (since the fertility rate of the past can be very large due to low population)</t>
+  </si>
+  <si>
+    <t>dea_radix</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>dea_age_at</t>
+  </si>
+  <si>
+    <t>life expectancy at certain age (usually at birth)</t>
+  </si>
+  <si>
+    <t>radix for life expectancy calcuation (no effect on result)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1716,7 +1733,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1821,23 +1838,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1873,23 +1873,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2065,12 +2048,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I190"/>
+  <dimension ref="A1:I192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2079,9 +2062,9 @@
     <col min="1" max="1" width="27.5703125" style="21" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="21" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="21" customWidth="1"/>
     <col min="8" max="8" width="19" style="21" customWidth="1"/>
     <col min="9" max="9" width="89.7109375" style="24" customWidth="1"/>
@@ -4239,28 +4222,28 @@
         <v>92</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>94</v>
+        <v>483</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>95</v>
       </c>
       <c r="D75" s="19">
-        <v>120</v>
+        <v>100000</v>
       </c>
       <c r="E75" s="19">
-        <v>120</v>
+        <v>100000</v>
       </c>
       <c r="F75" s="19">
-        <v>120</v>
+        <v>100000</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>93</v>
+        <v>484</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I75" s="20" t="s">
-        <v>103</v>
+        <v>485</v>
+      </c>
+      <c r="I75" s="15" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -4268,28 +4251,28 @@
         <v>92</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C76" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C76" s="18" t="s">
         <v>95</v>
       </c>
       <c r="D76" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E76" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F76" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I76" s="20" t="s">
-        <v>476</v>
+        <v>485</v>
+      </c>
+      <c r="I76" s="15" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4297,144 +4280,144 @@
         <v>92</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77" s="19">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="E77" s="19">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="F77" s="19">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I77" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D78" s="19">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="E78" s="19">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="F78" s="19">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I78" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>472</v>
+        <v>112</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D79" s="19">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="E79" s="19">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="F79" s="19">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="G79" s="14" t="s">
         <v>85</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I79" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A80" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D80" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="E80" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="F80" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I80" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A81" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="E81" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="F81" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I81" s="20" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D80" s="12">
-        <v>20</v>
-      </c>
-      <c r="E80" s="12">
-        <v>20</v>
-      </c>
-      <c r="F80" s="12">
-        <v>20</v>
-      </c>
-      <c r="G80" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D81" s="12">
-        <v>20</v>
-      </c>
-      <c r="E81" s="12">
-        <v>20</v>
-      </c>
-      <c r="F81" s="12">
-        <v>20</v>
-      </c>
-      <c r="G81" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H81" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I81" s="13" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4442,57 +4425,57 @@
         <v>144</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D82" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E82" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F82" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H82" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="D83" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E83" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F83" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G83" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4500,260 +4483,260 @@
         <v>144</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D84" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E84" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F84" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H84" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="D85" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E85" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F85" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D86" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E86" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F86" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H86" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="D87" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E87" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F87" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G87" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B88" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>154</v>
+      <c r="B88" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="D88" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E88" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F88" s="12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="H88" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B89" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>155</v>
+      <c r="B89" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="D89" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E89" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F89" s="12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B90" s="11" t="s">
-        <v>156</v>
+      <c r="B90" s="35" t="s">
+        <v>152</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="D90" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E90" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F90" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B91" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>95</v>
+      <c r="B91" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="D91" s="12">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="E91" s="12">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F91" s="12">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C92" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C92" s="13" t="s">
         <v>95</v>
       </c>
       <c r="D92" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E92" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F92" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H92" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4761,115 +4744,115 @@
         <v>144</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F93" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D94" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E94" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F94" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G94" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H94" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I94" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D95" s="12">
+        <v>13</v>
+      </c>
+      <c r="E95" s="12">
+        <v>13</v>
+      </c>
+      <c r="F95" s="12">
+        <v>13</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H95" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I95" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D96" s="12">
+        <v>0</v>
+      </c>
+      <c r="E96" s="12">
+        <v>0</v>
+      </c>
+      <c r="F96" s="12">
+        <v>0</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H96" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I94" s="13" t="s">
+      <c r="I96" s="13" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A95" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="B95" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D95" s="26">
-        <v>20</v>
-      </c>
-      <c r="E95" s="26">
-        <v>20</v>
-      </c>
-      <c r="F95" s="26">
-        <v>20</v>
-      </c>
-      <c r="G95" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H95" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I95" s="30" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="B96" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D96" s="26">
-        <v>20</v>
-      </c>
-      <c r="E96" s="26">
-        <v>20</v>
-      </c>
-      <c r="F96" s="26">
-        <v>20</v>
-      </c>
-      <c r="G96" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H96" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I96" s="30" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4877,57 +4860,57 @@
         <v>181</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F97" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H97" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I97" s="30" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="25" t="s">
         <v>181</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
       <c r="D98" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E98" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F98" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G98" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H98" s="25" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4935,57 +4918,57 @@
         <v>181</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D99" s="26">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E99" s="26">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F99" s="26">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G99" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H99" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
         <v>181</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>211</v>
+        <v>95</v>
       </c>
       <c r="D100" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E100" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F100" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G100" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H100" s="25" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I100" s="30" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4993,202 +4976,202 @@
         <v>181</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="C101" s="31" t="s">
-        <v>212</v>
+        <v>186</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>210</v>
       </c>
       <c r="D101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F101" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H101" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A102" s="25" t="s">
         <v>181</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>95</v>
+        <v>211</v>
       </c>
       <c r="D102" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E102" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F102" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G102" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H102" s="25" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B103" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="C103" s="30" t="s">
-        <v>213</v>
+      <c r="B103" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C103" s="31" t="s">
+        <v>212</v>
       </c>
       <c r="D103" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E103" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F103" s="26">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="H103" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I103" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A104" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B104" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="C104" s="30" t="s">
-        <v>214</v>
+      <c r="B104" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="D104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="E104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F104" s="26">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G104" s="25" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="H104" s="25" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B105" s="25" t="s">
-        <v>192</v>
+      <c r="B105" s="35" t="s">
+        <v>190</v>
       </c>
       <c r="C105" s="30" t="s">
-        <v>95</v>
+        <v>213</v>
       </c>
       <c r="D105" s="26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E105" s="26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F105" s="26">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="H105" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I105" s="30" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A106" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="B106" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>95</v>
+      <c r="B106" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="C106" s="30" t="s">
+        <v>214</v>
       </c>
       <c r="D106" s="26">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="E106" s="26">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="F106" s="26">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="H106" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I106" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A107" s="25" t="s">
         <v>181</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="C107" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C107" s="30" t="s">
         <v>95</v>
       </c>
       <c r="D107" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E107" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F107" s="26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H107" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I107" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5196,144 +5179,144 @@
         <v>181</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F108" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G108" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H108" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I108" s="30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A109" s="25" t="s">
         <v>181</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>95</v>
       </c>
       <c r="D109" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E109" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F109" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G109" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H109" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I109" s="30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A110" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D110" s="26">
+        <v>13</v>
+      </c>
+      <c r="E110" s="26">
+        <v>13</v>
+      </c>
+      <c r="F110" s="26">
+        <v>13</v>
+      </c>
+      <c r="G110" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H110" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I110" s="30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A111" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D111" s="26">
+        <v>0</v>
+      </c>
+      <c r="E111" s="26">
+        <v>0</v>
+      </c>
+      <c r="F111" s="26">
+        <v>0</v>
+      </c>
+      <c r="G111" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H111" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I109" s="30" t="s">
+      <c r="I111" s="30" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A110" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D110" s="12">
-        <v>70</v>
-      </c>
-      <c r="E110" s="12">
-        <v>70</v>
-      </c>
-      <c r="F110" s="12">
-        <v>70</v>
-      </c>
-      <c r="G110" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H110" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I110" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="C111" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F111" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="G111" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H111" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I111" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B112" s="11" t="s">
-        <v>242</v>
+      <c r="B112" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E112" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F112" s="6">
-        <v>0.2</v>
+        <v>220</v>
+      </c>
+      <c r="D112" s="12">
+        <v>70</v>
+      </c>
+      <c r="E112" s="12">
+        <v>70</v>
+      </c>
+      <c r="F112" s="12">
+        <v>70</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I112" s="11" t="s">
-        <v>228</v>
+        <v>22</v>
+      </c>
+      <c r="I112" s="13" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5341,19 +5324,19 @@
         <v>221</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>318</v>
+        <v>241</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F113" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>85</v>
@@ -5362,7 +5345,7 @@
         <v>59</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5370,19 +5353,19 @@
         <v>221</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D114" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E114" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F114" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>85</v>
@@ -5391,7 +5374,7 @@
         <v>59</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5399,28 +5382,28 @@
         <v>221</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F115" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="H115" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5428,19 +5411,19 @@
         <v>221</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>243</v>
+        <v>319</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>226</v>
       </c>
       <c r="D116" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E116" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="F116" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>85</v>
@@ -5449,65 +5432,65 @@
         <v>59</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>244</v>
+        <v>322</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D117" s="12">
-        <v>20</v>
-      </c>
-      <c r="E117" s="12">
-        <v>20</v>
-      </c>
-      <c r="F117" s="12">
-        <v>20</v>
+        <v>230</v>
+      </c>
+      <c r="D117" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="E117" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F117" s="6">
+        <v>0.4</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="H117" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I117" s="13" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I117" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D118" s="12">
-        <v>20</v>
-      </c>
-      <c r="E118" s="12">
-        <v>20</v>
-      </c>
-      <c r="F118" s="12">
-        <v>20</v>
+        <v>226</v>
+      </c>
+      <c r="D118" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E118" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F118" s="6">
+        <v>0.3</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I118" s="13" t="s">
-        <v>234</v>
+        <v>59</v>
+      </c>
+      <c r="I118" s="11" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5515,57 +5498,57 @@
         <v>221</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>95</v>
+        <v>237</v>
       </c>
       <c r="D119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F119" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H119" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I119" s="13" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D120" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E120" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F120" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G120" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I120" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5573,144 +5556,144 @@
         <v>221</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D121" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="E121" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F121" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G121" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H121" s="11" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I121" s="13" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B122" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D122" s="12">
+        <v>0</v>
+      </c>
+      <c r="E122" s="12">
+        <v>0</v>
+      </c>
+      <c r="F122" s="12">
+        <v>0</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H122" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I122" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D123" s="12">
+        <v>100</v>
+      </c>
+      <c r="E123" s="12">
+        <v>100</v>
+      </c>
+      <c r="F123" s="12">
+        <v>100</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H123" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I123" s="13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B124" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="C124" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D124" s="6">
         <v>0.15</v>
       </c>
-      <c r="E122" s="6">
+      <c r="E124" s="6">
         <v>0.15</v>
       </c>
-      <c r="F122" s="6">
+      <c r="F124" s="6">
         <v>0.15</v>
       </c>
-      <c r="G122" s="11" t="s">
+      <c r="G124" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H122" s="11" t="s">
+      <c r="H124" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I122" s="11" t="s">
+      <c r="I124" s="11" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A123" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="D123" s="29">
-        <v>70</v>
-      </c>
-      <c r="E123" s="29">
-        <v>70</v>
-      </c>
-      <c r="F123" s="29">
-        <v>70</v>
-      </c>
-      <c r="G123" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H123" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I123" s="28" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A124" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="B124" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="C124" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F124" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="G124" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H124" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I124" s="27" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="B125" s="27" t="s">
-        <v>251</v>
+      <c r="B125" s="14" t="s">
+        <v>259</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D125" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E125" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F125" s="14">
-        <v>0.2</v>
+        <v>220</v>
+      </c>
+      <c r="D125" s="29">
+        <v>70</v>
+      </c>
+      <c r="E125" s="29">
+        <v>70</v>
+      </c>
+      <c r="F125" s="29">
+        <v>70</v>
       </c>
       <c r="G125" s="27" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H125" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I125" s="27" t="s">
-        <v>228</v>
+        <v>22</v>
+      </c>
+      <c r="I125" s="28" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
@@ -5718,19 +5701,19 @@
         <v>250</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>324</v>
+        <v>262</v>
       </c>
       <c r="C126" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F126" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G126" s="27" t="s">
         <v>85</v>
@@ -5739,7 +5722,7 @@
         <v>59</v>
       </c>
       <c r="I126" s="27" t="s">
-        <v>326</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -5747,19 +5730,19 @@
         <v>250</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>325</v>
+        <v>251</v>
       </c>
       <c r="C127" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D127" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E127" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F127" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G127" s="27" t="s">
         <v>85</v>
@@ -5768,7 +5751,7 @@
         <v>59</v>
       </c>
       <c r="I127" s="27" t="s">
-        <v>321</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
@@ -5776,28 +5759,28 @@
         <v>250</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F128" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>231</v>
+        <v>85</v>
       </c>
       <c r="H128" s="27" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I128" s="27" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5805,19 +5788,19 @@
         <v>250</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>252</v>
+        <v>325</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D129" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E129" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="F129" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="G129" s="27" t="s">
         <v>85</v>
@@ -5826,65 +5809,65 @@
         <v>59</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>253</v>
+        <v>327</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D130" s="29">
-        <v>20</v>
-      </c>
-      <c r="E130" s="29">
-        <v>20</v>
-      </c>
-      <c r="F130" s="29">
-        <v>20</v>
+        <v>229</v>
+      </c>
+      <c r="D130" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="E130" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F130" s="14">
+        <v>0.4</v>
       </c>
       <c r="G130" s="27" t="s">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="H130" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I130" s="28" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I130" s="27" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D131" s="29">
-        <v>20</v>
-      </c>
-      <c r="E131" s="29">
-        <v>20</v>
-      </c>
-      <c r="F131" s="29">
-        <v>20</v>
+        <v>226</v>
+      </c>
+      <c r="D131" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="E131" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F131" s="14">
+        <v>0.3</v>
       </c>
       <c r="G131" s="27" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H131" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I131" s="28" t="s">
-        <v>264</v>
+        <v>59</v>
+      </c>
+      <c r="I131" s="27" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5892,57 +5875,57 @@
         <v>250</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C132" s="14" t="s">
-        <v>95</v>
+        <v>237</v>
       </c>
       <c r="D132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F132" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G132" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H132" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I132" s="28" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A133" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C133" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D133" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E133" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F133" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G133" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H133" s="27" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I133" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5950,173 +5933,173 @@
         <v>250</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C134" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D134" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="E134" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F134" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G134" s="27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H134" s="27" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I134" s="28" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A135" s="27" t="s">
         <v>250</v>
       </c>
       <c r="B135" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D135" s="29">
+        <v>0</v>
+      </c>
+      <c r="E135" s="29">
+        <v>0</v>
+      </c>
+      <c r="F135" s="29">
+        <v>0</v>
+      </c>
+      <c r="G135" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H135" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I135" s="28" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A136" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D136" s="29">
+        <v>100</v>
+      </c>
+      <c r="E136" s="29">
+        <v>100</v>
+      </c>
+      <c r="F136" s="29">
+        <v>100</v>
+      </c>
+      <c r="G136" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H136" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I136" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A137" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="B137" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="C135" s="14" t="s">
+      <c r="C137" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="D135" s="14">
+      <c r="D137" s="14">
         <v>0.15</v>
       </c>
-      <c r="E135" s="14">
+      <c r="E137" s="14">
         <v>0.15</v>
       </c>
-      <c r="F135" s="14">
+      <c r="F137" s="14">
         <v>0.15</v>
       </c>
-      <c r="G135" s="27" t="s">
+      <c r="G137" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="H135" s="27" t="s">
+      <c r="H137" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I135" s="27" t="s">
+      <c r="I137" s="27" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A136" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B136" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="C136" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F136" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="G136" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H136" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I136" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A137" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="B137" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="C137" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D137" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="E137" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="F137" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="G137" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H137" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I137" s="11" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B138" s="11" t="s">
-        <v>281</v>
+      <c r="B138" s="37" t="s">
+        <v>279</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D138" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E138" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F138" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="H138" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B139" s="11" t="s">
-        <v>282</v>
+      <c r="B139" s="37" t="s">
+        <v>280</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D139" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E139" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F139" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>284</v>
+        <v>85</v>
       </c>
       <c r="H139" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -6124,28 +6107,28 @@
         <v>276</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="D140" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E140" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F140" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="H140" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -6153,28 +6136,28 @@
         <v>276</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D141" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E141" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F141" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>85</v>
+        <v>284</v>
       </c>
       <c r="H141" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6182,19 +6165,19 @@
         <v>276</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C142" s="6" t="s">
         <v>277</v>
       </c>
       <c r="D142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F142" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G142" s="11" t="s">
         <v>85</v>
@@ -6203,7 +6186,7 @@
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6211,7 +6194,7 @@
         <v>276</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>277</v>
@@ -6232,7 +6215,7 @@
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6240,28 +6223,28 @@
         <v>276</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="D144" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="E144" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="F144" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="G144" s="11" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H144" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6269,28 +6252,28 @@
         <v>276</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D145" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E145" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="F145" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G145" s="11" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="H145" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -6298,28 +6281,28 @@
         <v>276</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>95</v>
+        <v>297</v>
       </c>
       <c r="D146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F146" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H146" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6327,19 +6310,19 @@
         <v>276</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C147" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D147" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E147" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F147" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G147" s="11" t="s">
         <v>44</v>
@@ -6348,7 +6331,7 @@
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -6356,28 +6339,28 @@
         <v>276</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D148" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="E148" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="F148" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="G148" s="11" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="H148" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6385,28 +6368,28 @@
         <v>276</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="D149" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E149" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F149" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G149" s="11" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="H149" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.2">
@@ -6414,7 +6397,7 @@
         <v>276</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>277</v>
@@ -6435,7 +6418,7 @@
         <v>22</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.2">
@@ -6443,28 +6426,28 @@
         <v>276</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D151" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="E151" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="F151" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>313</v>
+        <v>85</v>
       </c>
       <c r="H151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -6472,19 +6455,19 @@
         <v>276</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>95</v>
+        <v>277</v>
       </c>
       <c r="D152" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E152" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F152" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G152" s="11" t="s">
         <v>85</v>
@@ -6493,7 +6476,7 @@
         <v>22</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -6501,86 +6484,86 @@
         <v>276</v>
       </c>
       <c r="B153" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D153" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E153" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F153" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G153" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="H153" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I153" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A154" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D154" s="6">
+        <v>0</v>
+      </c>
+      <c r="E154" s="6">
+        <v>0</v>
+      </c>
+      <c r="F154" s="6">
+        <v>0</v>
+      </c>
+      <c r="G154" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H154" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I154" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A155" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B155" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="C153" s="6" t="s">
+      <c r="C155" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="D153" s="6">
+      <c r="D155" s="6">
         <v>0.1</v>
       </c>
-      <c r="E153" s="6">
+      <c r="E155" s="6">
         <v>0.1</v>
       </c>
-      <c r="F153" s="6">
+      <c r="F155" s="6">
         <v>0.1</v>
       </c>
-      <c r="G153" s="11" t="s">
+      <c r="G155" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H153" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I153" s="11" t="s">
+      <c r="H155" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I155" s="11" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A154" s="27" t="s">
-        <v>328</v>
-      </c>
-      <c r="B154" s="27" t="s">
-        <v>330</v>
-      </c>
-      <c r="C154" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="D154" s="29">
-        <v>25</v>
-      </c>
-      <c r="E154" s="29">
-        <v>25</v>
-      </c>
-      <c r="F154" s="29">
-        <v>25</v>
-      </c>
-      <c r="G154" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H154" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I154" s="28" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A155" s="27" t="s">
-        <v>328</v>
-      </c>
-      <c r="B155" s="27" t="s">
-        <v>335</v>
-      </c>
-      <c r="C155" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="D155" s="29">
-        <v>-25</v>
-      </c>
-      <c r="E155" s="29">
-        <v>0</v>
-      </c>
-      <c r="F155" s="29">
-        <v>25</v>
-      </c>
-      <c r="G155" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H155" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I155" s="28" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -6588,48 +6571,48 @@
         <v>328</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D156" s="29">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E156" s="29">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F156" s="29">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G156" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H156" s="27" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
         <v>328</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>95</v>
+        <v>331</v>
       </c>
       <c r="D157" s="29">
-        <v>85</v>
+        <v>-25</v>
       </c>
       <c r="E157" s="29">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="F157" s="29">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G157" s="27" t="s">
         <v>44</v>
@@ -6638,7 +6621,7 @@
         <v>46</v>
       </c>
       <c r="I157" s="28" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.2">
@@ -6646,19 +6629,19 @@
         <v>328</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D158" s="29">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E158" s="29">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F158" s="29">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G158" s="27" t="s">
         <v>44</v>
@@ -6667,7 +6650,7 @@
         <v>46</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -6675,28 +6658,28 @@
         <v>328</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>334</v>
+        <v>95</v>
       </c>
       <c r="D159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F159" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G159" s="27" t="s">
-        <v>343</v>
+        <v>44</v>
       </c>
       <c r="H159" s="27" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="I159" s="28" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6704,173 +6687,173 @@
         <v>328</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D160" s="29">
-        <v>2044</v>
+        <v>75</v>
       </c>
       <c r="E160" s="29">
-        <v>2044</v>
+        <v>85</v>
       </c>
       <c r="F160" s="29">
-        <v>2044</v>
+        <v>90</v>
       </c>
       <c r="G160" s="27" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H160" s="27" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I160" s="28" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="27" t="s">
         <v>328</v>
       </c>
       <c r="B161" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C161" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="D161" s="29">
+        <v>0</v>
+      </c>
+      <c r="E161" s="29">
+        <v>0</v>
+      </c>
+      <c r="F161" s="29">
+        <v>0</v>
+      </c>
+      <c r="G161" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="H161" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="I161" s="28" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A162" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="B162" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="C162" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="D162" s="29">
+        <v>2044</v>
+      </c>
+      <c r="E162" s="29">
+        <v>2044</v>
+      </c>
+      <c r="F162" s="29">
+        <v>2044</v>
+      </c>
+      <c r="G162" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H162" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I162" s="28" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A163" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="B163" s="27" t="s">
         <v>340</v>
       </c>
-      <c r="C161" s="14" t="s">
+      <c r="C163" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="D161" s="29">
+      <c r="D163" s="29">
         <v>-0.04</v>
       </c>
-      <c r="E161" s="29">
+      <c r="E163" s="29">
         <v>-0.04</v>
       </c>
-      <c r="F161" s="29">
+      <c r="F163" s="29">
         <v>-0.04</v>
       </c>
-      <c r="G161" s="27" t="s">
+      <c r="G163" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="H161" s="27" t="s">
+      <c r="H163" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I161" s="28" t="s">
+      <c r="I163" s="28" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A162" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="D162" s="6">
-        <v>500</v>
-      </c>
-      <c r="E162" s="6">
-        <v>500</v>
-      </c>
-      <c r="F162" s="6">
-        <v>500</v>
-      </c>
-      <c r="G162" s="11" t="s">
-        <v>364</v>
-      </c>
-      <c r="H162" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I162" s="11" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A163" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="B163" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="D163" s="12">
-        <v>20</v>
-      </c>
-      <c r="E163" s="12">
-        <v>20</v>
-      </c>
-      <c r="F163" s="12">
-        <v>20</v>
-      </c>
-      <c r="G163" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H163" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I163" s="13" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
         <v>361</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D164" s="12">
-        <v>20</v>
-      </c>
-      <c r="E164" s="12">
-        <v>20</v>
-      </c>
-      <c r="F164" s="12">
-        <v>20</v>
+        <v>363</v>
+      </c>
+      <c r="D164" s="6">
+        <v>500</v>
+      </c>
+      <c r="E164" s="6">
+        <v>500</v>
+      </c>
+      <c r="F164" s="6">
+        <v>500</v>
       </c>
       <c r="G164" s="11" t="s">
-        <v>44</v>
+        <v>364</v>
       </c>
       <c r="H164" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I164" s="13" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I164" s="11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
         <v>361</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F165" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G165" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H165" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I165" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -6878,19 +6861,19 @@
         <v>361</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>95</v>
+        <v>370</v>
       </c>
       <c r="D166" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E166" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F166" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G166" s="11" t="s">
         <v>44</v>
@@ -6899,143 +6882,143 @@
         <v>22</v>
       </c>
       <c r="I166" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A167" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D167" s="12">
+        <v>7</v>
+      </c>
+      <c r="E167" s="12">
+        <v>7</v>
+      </c>
+      <c r="F167" s="12">
+        <v>7</v>
+      </c>
+      <c r="G167" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H167" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I167" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A168" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D168" s="12">
+        <v>0</v>
+      </c>
+      <c r="E168" s="12">
+        <v>0</v>
+      </c>
+      <c r="F168" s="12">
+        <v>0</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H168" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I168" s="13" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="167" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="B167" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="C167" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="D167" s="10">
-        <v>500</v>
-      </c>
-      <c r="E167" s="10">
-        <v>500</v>
-      </c>
-      <c r="F167" s="10">
-        <v>500</v>
-      </c>
-      <c r="G167" s="25" t="s">
-        <v>364</v>
-      </c>
-      <c r="H167" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I167" s="25" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A168" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="B168" s="25" t="s">
-        <v>380</v>
-      </c>
-      <c r="C168" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="D168" s="26">
-        <v>20</v>
-      </c>
-      <c r="E168" s="26">
-        <v>20</v>
-      </c>
-      <c r="F168" s="26">
-        <v>20</v>
-      </c>
-      <c r="G168" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H168" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I168" s="30" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="25" t="s">
         <v>377</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C169" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="D169" s="26">
-        <v>20</v>
-      </c>
-      <c r="E169" s="26">
-        <v>20</v>
-      </c>
-      <c r="F169" s="26">
-        <v>20</v>
+        <v>378</v>
+      </c>
+      <c r="D169" s="10">
+        <v>500</v>
+      </c>
+      <c r="E169" s="10">
+        <v>500</v>
+      </c>
+      <c r="F169" s="10">
+        <v>500</v>
       </c>
       <c r="G169" s="25" t="s">
-        <v>44</v>
+        <v>364</v>
       </c>
       <c r="H169" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I169" s="30" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I169" s="25" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A170" s="25" t="s">
         <v>377</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C170" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F170" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G170" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H170" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I170" s="30" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A171" s="25" t="s">
         <v>377</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="C171" s="10" t="s">
-        <v>95</v>
+        <v>386</v>
       </c>
       <c r="D171" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E171" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F171" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G171" s="25" t="s">
         <v>44</v>
@@ -7044,123 +7027,123 @@
         <v>22</v>
       </c>
       <c r="I171" s="30" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="B172" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="C172" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D172" s="26">
+        <v>7</v>
+      </c>
+      <c r="E172" s="26">
+        <v>7</v>
+      </c>
+      <c r="F172" s="26">
+        <v>7</v>
+      </c>
+      <c r="G172" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H172" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I172" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A173" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="B173" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="C173" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D173" s="26">
+        <v>0</v>
+      </c>
+      <c r="E173" s="26">
+        <v>0</v>
+      </c>
+      <c r="F173" s="26">
+        <v>0</v>
+      </c>
+      <c r="G173" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H173" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I173" s="30" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A172" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="D172" s="12">
-        <v>2</v>
-      </c>
-      <c r="E172" s="12">
-        <v>2</v>
-      </c>
-      <c r="F172" s="12">
-        <v>2</v>
-      </c>
-      <c r="G172" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H172" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I172" s="13" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A173" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="B173" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="D173" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="E173" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="F173" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="G173" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H173" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I173" s="13" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
         <v>400</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="D174" s="36">
-        <v>80</v>
-      </c>
-      <c r="E174" s="36">
-        <v>80</v>
-      </c>
-      <c r="F174" s="36">
-        <v>80</v>
+        <v>402</v>
+      </c>
+      <c r="D174" s="12">
+        <v>2</v>
+      </c>
+      <c r="E174" s="12">
+        <v>2</v>
+      </c>
+      <c r="F174" s="12">
+        <v>2</v>
       </c>
       <c r="G174" s="11" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="H174" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I174" s="13" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
         <v>400</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="D175" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E175" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F175" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G175" s="11" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="H175" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -7168,19 +7151,19 @@
         <v>400</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="D176" s="12">
-        <v>0</v>
-      </c>
-      <c r="E176" s="12">
-        <v>0</v>
-      </c>
-      <c r="F176" s="12">
-        <v>0</v>
+        <v>407</v>
+      </c>
+      <c r="D176" s="36">
+        <v>80</v>
+      </c>
+      <c r="E176" s="36">
+        <v>80</v>
+      </c>
+      <c r="F176" s="36">
+        <v>80</v>
       </c>
       <c r="G176" s="11" t="s">
         <v>44</v>
@@ -7197,10 +7180,10 @@
         <v>400</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D177" s="12">
         <v>0</v>
@@ -7226,10 +7209,10 @@
         <v>400</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D178" s="12">
         <v>0</v>
@@ -7255,19 +7238,19 @@
         <v>400</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F179" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G179" s="11" t="s">
         <v>44</v>
@@ -7279,91 +7262,91 @@
         <v>419</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A180" s="27" t="s">
-        <v>428</v>
-      </c>
-      <c r="B180" s="27" t="s">
-        <v>429</v>
-      </c>
-      <c r="C180" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="D180" s="29">
-        <v>50</v>
-      </c>
-      <c r="E180" s="29">
-        <v>50</v>
-      </c>
-      <c r="F180" s="29">
-        <v>50</v>
-      </c>
-      <c r="G180" s="27" t="s">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A180" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B180" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="D180" s="12">
+        <v>0</v>
+      </c>
+      <c r="E180" s="12">
+        <v>0</v>
+      </c>
+      <c r="F180" s="12">
+        <v>0</v>
+      </c>
+      <c r="G180" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H180" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I180" s="28" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A181" s="27" t="s">
-        <v>428</v>
-      </c>
-      <c r="B181" s="27" t="s">
-        <v>430</v>
-      </c>
-      <c r="C181" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="D181" s="29">
-        <v>20</v>
-      </c>
-      <c r="E181" s="29">
-        <v>20</v>
-      </c>
-      <c r="F181" s="29">
-        <v>20</v>
-      </c>
-      <c r="G181" s="27" t="s">
+      <c r="H180" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I180" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A181" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="B181" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="D181" s="12">
+        <v>20</v>
+      </c>
+      <c r="E181" s="12">
+        <v>20</v>
+      </c>
+      <c r="F181" s="12">
+        <v>20</v>
+      </c>
+      <c r="G181" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H181" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I181" s="28" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H181" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I181" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A182" s="27" t="s">
         <v>428</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D182" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E182" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F182" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="G182" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H182" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I182" s="28" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -7371,135 +7354,135 @@
         <v>428</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>95</v>
+        <v>435</v>
       </c>
       <c r="D183" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E183" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F183" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G183" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H183" s="27" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="I183" s="28" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="27" t="s">
         <v>428</v>
       </c>
       <c r="B184" s="27" t="s">
+        <v>431</v>
+      </c>
+      <c r="C184" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="D184" s="29">
+        <v>7</v>
+      </c>
+      <c r="E184" s="29">
+        <v>7</v>
+      </c>
+      <c r="F184" s="29">
+        <v>7</v>
+      </c>
+      <c r="G184" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H184" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I184" s="28" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A185" s="27" t="s">
+        <v>428</v>
+      </c>
+      <c r="B185" s="27" t="s">
+        <v>432</v>
+      </c>
+      <c r="C185" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D185" s="29">
+        <v>0</v>
+      </c>
+      <c r="E185" s="29">
+        <v>0</v>
+      </c>
+      <c r="F185" s="29">
+        <v>0</v>
+      </c>
+      <c r="G185" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H185" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I185" s="28" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A186" s="27" t="s">
+        <v>428</v>
+      </c>
+      <c r="B186" s="27" t="s">
         <v>433</v>
       </c>
-      <c r="C184" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D184" s="29">
+      <c r="C186" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D186" s="29">
         <v>100</v>
       </c>
-      <c r="E184" s="29">
+      <c r="E186" s="29">
         <v>100</v>
       </c>
-      <c r="F184" s="29">
+      <c r="F186" s="29">
         <v>100</v>
       </c>
-      <c r="G184" s="27" t="s">
+      <c r="G186" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H184" s="27" t="s">
+      <c r="H186" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I184" s="28" t="s">
+      <c r="I186" s="28" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A185" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="B185" s="11" t="s">
-        <v>448</v>
-      </c>
-      <c r="C185" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="D185" s="36">
-        <v>100</v>
-      </c>
-      <c r="E185" s="36">
-        <v>100</v>
-      </c>
-      <c r="F185" s="36">
-        <v>100</v>
-      </c>
-      <c r="G185" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H185" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I185" s="13" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A186" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="B186" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="C186" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D186" s="12">
-        <v>80</v>
-      </c>
-      <c r="E186" s="12">
-        <v>80</v>
-      </c>
-      <c r="F186" s="12">
-        <v>80</v>
-      </c>
-      <c r="G186" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H186" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I186" s="13" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
         <v>446</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>451</v>
-      </c>
-      <c r="D187" s="12">
-        <v>0</v>
-      </c>
-      <c r="E187" s="12">
-        <v>0</v>
-      </c>
-      <c r="F187" s="12">
-        <v>0</v>
+        <v>447</v>
+      </c>
+      <c r="D187" s="36">
+        <v>100</v>
+      </c>
+      <c r="E187" s="36">
+        <v>100</v>
+      </c>
+      <c r="F187" s="36">
+        <v>100</v>
       </c>
       <c r="G187" s="11" t="s">
         <v>44</v>
@@ -7508,93 +7491,151 @@
         <v>22</v>
       </c>
       <c r="I187" s="13" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
         <v>446</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>451</v>
+        <v>95</v>
       </c>
       <c r="D188" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E188" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F188" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G188" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H188" s="11" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="I188" s="13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A189" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B189" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D189" s="12">
+        <v>0</v>
+      </c>
+      <c r="E189" s="12">
+        <v>0</v>
+      </c>
+      <c r="F189" s="12">
+        <v>0</v>
+      </c>
+      <c r="G189" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H189" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I189" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A190" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B190" s="11" t="s">
+        <v>452</v>
+      </c>
+      <c r="C190" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D190" s="12">
+        <v>0</v>
+      </c>
+      <c r="E190" s="12">
+        <v>0</v>
+      </c>
+      <c r="F190" s="12">
+        <v>0</v>
+      </c>
+      <c r="G190" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H190" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I190" s="13" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A189" s="27" t="s">
+    <row r="191" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A191" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="B189" s="27" t="s">
+      <c r="B191" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="C189" s="28" t="s">
+      <c r="C191" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="D189" s="29">
+      <c r="D191" s="29">
         <v>90</v>
       </c>
-      <c r="E189" s="29">
+      <c r="E191" s="29">
         <v>90</v>
       </c>
-      <c r="F189" s="29">
+      <c r="F191" s="29">
         <v>90</v>
       </c>
-      <c r="G189" s="27" t="s">
+      <c r="G191" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H189" s="27" t="s">
+      <c r="H191" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I189" s="28" t="s">
+      <c r="I191" s="28" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A190" s="27" t="s">
+    <row r="192" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A192" s="27" t="s">
         <v>455</v>
       </c>
-      <c r="B190" s="27" t="s">
+      <c r="B192" s="27" t="s">
         <v>458</v>
       </c>
-      <c r="C190" s="28" t="s">
+      <c r="C192" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="D190" s="29">
+      <c r="D192" s="29">
         <v>50</v>
       </c>
-      <c r="E190" s="29">
+      <c r="E192" s="29">
         <v>50</v>
       </c>
-      <c r="F190" s="29">
+      <c r="F192" s="29">
         <v>50</v>
       </c>
-      <c r="G190" s="27" t="s">
+      <c r="G192" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H190" s="27" t="s">
+      <c r="H192" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="I190" s="28" t="s">
+      <c r="I192" s="28" t="s">
         <v>462</v>
       </c>
     </row>

</xml_diff>

<commit_message>
with parameters dea_radix and dea_age_at
</commit_message>
<xml_diff>
--- a/2020phase2/2_Data/3_Parameter/parameter.xlsx
+++ b/2020phase2/2_Data/3_Parameter/parameter.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C5AE2F-B315-4A4A-9740-59AB0AAA299A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="477">
   <si>
     <t>parameter</t>
   </si>
@@ -1437,12 +1436,27 @@
   </si>
   <si>
     <t>proportion of data points used in the loess regressions of proportion by year; groups: district, age, sex, origin (immigration* by district, year, age, sex, origin)</t>
+  </si>
+  <si>
+    <t>dea_radix</t>
+  </si>
+  <si>
+    <t>dea_age_at</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>radix (starting population) for life expectancy calcuation (no effect on result)</t>
+  </si>
+  <si>
+    <t>life expectancy at certain age (usually at birth; i.e. age zero)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1671,7 +1685,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1776,23 +1790,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1828,23 +1825,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2020,12 +2000,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I186"/>
+  <dimension ref="A1:I188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2034,9 +2014,9 @@
     <col min="1" max="1" width="27.5703125" style="21" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="21" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="23" customWidth="1"/>
     <col min="7" max="7" width="18" style="21" customWidth="1"/>
     <col min="8" max="8" width="19" style="21" customWidth="1"/>
     <col min="9" max="9" width="89.7109375" style="24" customWidth="1"/>
@@ -4136,28 +4116,28 @@
         <v>90</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>100</v>
+        <v>472</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D73" s="19">
-        <v>120</v>
+        <v>100000</v>
       </c>
       <c r="E73" s="19">
-        <v>120</v>
+        <v>100000</v>
       </c>
       <c r="F73" s="19">
-        <v>120</v>
+        <v>100000</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I73" s="20" t="s">
-        <v>101</v>
+        <v>474</v>
+      </c>
+      <c r="I73" s="15" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -4165,28 +4145,28 @@
         <v>90</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>109</v>
+        <v>473</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D74" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E74" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F74" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I74" s="20" t="s">
-        <v>458</v>
+        <v>474</v>
+      </c>
+      <c r="I74" s="15" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -4194,144 +4174,144 @@
         <v>90</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D75" s="19">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="E75" s="19">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="F75" s="19">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I75" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D76" s="19">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="E76" s="19">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="F76" s="19">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="I76" s="20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>454</v>
+        <v>110</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D77" s="19">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="E77" s="19">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="F77" s="19">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="G77" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="I77" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="E78" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="F78" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I78" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A79" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D79" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="E79" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="F79" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I79" s="20" t="s">
         <v>455</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A78" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D78" s="12">
-        <v>20</v>
-      </c>
-      <c r="E78" s="12">
-        <v>20</v>
-      </c>
-      <c r="F78" s="12">
-        <v>20</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H78" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I78" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D79" s="12">
-        <v>20</v>
-      </c>
-      <c r="E79" s="12">
-        <v>20</v>
-      </c>
-      <c r="F79" s="12">
-        <v>20</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I79" s="13" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4339,57 +4319,57 @@
         <v>142</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D80" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E80" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F80" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H80" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I80" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="D81" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E81" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F81" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4397,144 +4377,144 @@
         <v>142</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D82" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E82" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F82" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H82" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="D83" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E83" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F83" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G83" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D84" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E84" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F84" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H84" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="D85" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E85" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F85" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G85" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>93</v>
+        <v>148</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="D86" s="12">
-        <v>0.3</v>
+        <v>13</v>
       </c>
       <c r="E86" s="12">
-        <v>0.3</v>
+        <v>13</v>
       </c>
       <c r="F86" s="12">
-        <v>0.3</v>
+        <v>13</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="H86" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>471</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4542,28 +4522,28 @@
         <v>142</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="C87" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D87" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E87" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F87" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>467</v>
+        <v>140</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4571,57 +4551,57 @@
         <v>142</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C88" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="C88" s="13" t="s">
         <v>93</v>
       </c>
       <c r="D88" s="12">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="E88" s="12">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="F88" s="12">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H88" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C89" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C89" s="13" t="s">
         <v>93</v>
       </c>
       <c r="D89" s="12">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E89" s="12">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="F89" s="12">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>154</v>
+        <v>467</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -4629,115 +4609,115 @@
         <v>142</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D90" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E90" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F90" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I90" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>142</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D91" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E91" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F91" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G91" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H91" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D92" s="12">
+        <v>13</v>
+      </c>
+      <c r="E92" s="12">
+        <v>13</v>
+      </c>
+      <c r="F92" s="12">
+        <v>13</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H92" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I92" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D93" s="12">
+        <v>0</v>
+      </c>
+      <c r="E93" s="12">
+        <v>0</v>
+      </c>
+      <c r="F93" s="12">
+        <v>0</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H93" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="I91" s="13" t="s">
+      <c r="I93" s="13" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B92" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="D92" s="26">
-        <v>20</v>
-      </c>
-      <c r="E92" s="26">
-        <v>20</v>
-      </c>
-      <c r="F92" s="26">
-        <v>20</v>
-      </c>
-      <c r="G92" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H92" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I92" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B93" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="D93" s="26">
-        <v>20</v>
-      </c>
-      <c r="E93" s="26">
-        <v>20</v>
-      </c>
-      <c r="F93" s="26">
-        <v>20</v>
-      </c>
-      <c r="G93" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H93" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I93" s="30" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4745,57 +4725,57 @@
         <v>171</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D94" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E94" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F94" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G94" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H94" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I94" s="30" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>93</v>
+        <v>192</v>
       </c>
       <c r="D95" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E95" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F95" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G95" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H95" s="25" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I95" s="30" t="s">
-        <v>82</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4803,57 +4783,57 @@
         <v>171</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D96" s="26">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E96" s="26">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F96" s="26">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G96" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H96" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I96" s="30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>195</v>
+        <v>93</v>
       </c>
       <c r="D97" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E97" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F97" s="26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G97" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H97" s="25" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="I97" s="30" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4861,173 +4841,173 @@
         <v>171</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="C98" s="31" t="s">
-        <v>196</v>
+        <v>176</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>194</v>
       </c>
       <c r="D98" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E98" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F98" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H98" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I98" s="30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>93</v>
+        <v>195</v>
       </c>
       <c r="D99" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E99" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F99" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G99" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H99" s="25" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I99" s="30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>468</v>
-      </c>
-      <c r="C100" s="30" t="s">
-        <v>93</v>
+        <v>178</v>
+      </c>
+      <c r="C100" s="31" t="s">
+        <v>196</v>
       </c>
       <c r="D100" s="26">
-        <v>0.3</v>
+        <v>13</v>
       </c>
       <c r="E100" s="26">
-        <v>0.3</v>
+        <v>13</v>
       </c>
       <c r="F100" s="26">
-        <v>0.3</v>
+        <v>13</v>
       </c>
       <c r="G100" s="25" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="H100" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I100" s="30" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>469</v>
-      </c>
-      <c r="C101" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="C101" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D101" s="26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E101" s="26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F101" s="26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="H101" s="25" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="I101" s="30" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="C102" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="C102" s="30" t="s">
         <v>93</v>
       </c>
       <c r="D102" s="26">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="E102" s="26">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="F102" s="26">
-        <v>20</v>
+        <v>0.3</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H102" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I102" s="30" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C103" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="C103" s="30" t="s">
         <v>93</v>
       </c>
       <c r="D103" s="26">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E103" s="26">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="F103" s="26">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H103" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I103" s="30" t="s">
-        <v>188</v>
+        <v>467</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -5035,144 +5015,144 @@
         <v>171</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D104" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E104" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F104" s="26">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G104" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H104" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I104" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
         <v>171</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>93</v>
       </c>
       <c r="D105" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E105" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F105" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G105" s="25" t="s">
         <v>44</v>
       </c>
       <c r="H105" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I105" s="30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A106" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B106" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C106" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D106" s="26">
+        <v>13</v>
+      </c>
+      <c r="E106" s="26">
+        <v>13</v>
+      </c>
+      <c r="F106" s="26">
+        <v>13</v>
+      </c>
+      <c r="G106" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H106" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I106" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A107" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B107" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D107" s="26">
+        <v>0</v>
+      </c>
+      <c r="E107" s="26">
+        <v>0</v>
+      </c>
+      <c r="F107" s="26">
+        <v>0</v>
+      </c>
+      <c r="G107" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H107" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I105" s="30" t="s">
+      <c r="I107" s="30" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A106" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C106" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D106" s="12">
-        <v>70</v>
-      </c>
-      <c r="E106" s="12">
-        <v>70</v>
-      </c>
-      <c r="F106" s="12">
-        <v>70</v>
-      </c>
-      <c r="G106" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H106" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I106" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D107" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E107" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F107" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="G107" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H107" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I107" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B108" s="11" t="s">
-        <v>224</v>
+      <c r="B108" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D108" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E108" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="F108" s="6">
-        <v>0.2</v>
+        <v>202</v>
+      </c>
+      <c r="D108" s="12">
+        <v>70</v>
+      </c>
+      <c r="E108" s="12">
+        <v>70</v>
+      </c>
+      <c r="F108" s="12">
+        <v>70</v>
       </c>
       <c r="G108" s="11" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="H108" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I108" s="11" t="s">
-        <v>210</v>
+        <v>22</v>
+      </c>
+      <c r="I108" s="13" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5180,19 +5160,19 @@
         <v>203</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>300</v>
+        <v>223</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>208</v>
       </c>
       <c r="D109" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E109" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F109" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G109" s="11" t="s">
         <v>83</v>
@@ -5201,7 +5181,7 @@
         <v>57</v>
       </c>
       <c r="I109" s="11" t="s">
-        <v>302</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5209,19 +5189,19 @@
         <v>203</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>301</v>
+        <v>224</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>208</v>
       </c>
       <c r="D110" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E110" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F110" s="6">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G110" s="11" t="s">
         <v>83</v>
@@ -5230,7 +5210,7 @@
         <v>57</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>303</v>
+        <v>210</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5238,28 +5218,28 @@
         <v>203</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D111" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E111" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F111" s="6">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>213</v>
+        <v>83</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5267,19 +5247,19 @@
         <v>203</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>225</v>
+        <v>301</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>208</v>
       </c>
       <c r="D112" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E112" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="F112" s="6">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="G112" s="11" t="s">
         <v>83</v>
@@ -5288,65 +5268,65 @@
         <v>57</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>226</v>
+        <v>304</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D113" s="12">
-        <v>20</v>
-      </c>
-      <c r="E113" s="12">
-        <v>20</v>
-      </c>
-      <c r="F113" s="12">
-        <v>20</v>
+        <v>212</v>
+      </c>
+      <c r="D113" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="E113" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F113" s="6">
+        <v>0.4</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="H113" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I113" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I113" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D114" s="12">
-        <v>20</v>
-      </c>
-      <c r="E114" s="12">
-        <v>20</v>
-      </c>
-      <c r="F114" s="12">
-        <v>20</v>
+        <v>208</v>
+      </c>
+      <c r="D114" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E114" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F114" s="6">
+        <v>0.3</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I114" s="13" t="s">
-        <v>216</v>
+        <v>57</v>
+      </c>
+      <c r="I114" s="11" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5354,57 +5334,57 @@
         <v>203</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>93</v>
+        <v>219</v>
       </c>
       <c r="D115" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E115" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F115" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H115" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I115" s="13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D116" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E116" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F116" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H116" s="11" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I116" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5412,144 +5392,144 @@
         <v>203</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D117" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="E117" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F117" s="12">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G117" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H117" s="11" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I117" s="13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B118" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D118" s="12">
+        <v>0</v>
+      </c>
+      <c r="E118" s="12">
+        <v>0</v>
+      </c>
+      <c r="F118" s="12">
+        <v>0</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H118" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I118" s="13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A119" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D119" s="12">
+        <v>100</v>
+      </c>
+      <c r="E119" s="12">
+        <v>100</v>
+      </c>
+      <c r="F119" s="12">
+        <v>100</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H119" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I119" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B120" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="C118" s="6" t="s">
+      <c r="C120" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D120" s="6">
         <v>0.15</v>
       </c>
-      <c r="E118" s="6">
+      <c r="E120" s="6">
         <v>0.15</v>
       </c>
-      <c r="F118" s="6">
+      <c r="F120" s="6">
         <v>0.15</v>
       </c>
-      <c r="G118" s="11" t="s">
+      <c r="G120" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H118" s="11" t="s">
+      <c r="H120" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="I118" s="11" t="s">
+      <c r="I120" s="11" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A119" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="B119" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="D119" s="29">
-        <v>70</v>
-      </c>
-      <c r="E119" s="29">
-        <v>70</v>
-      </c>
-      <c r="F119" s="29">
-        <v>70</v>
-      </c>
-      <c r="G119" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H119" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I119" s="28" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A120" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="B120" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D120" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E120" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F120" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="G120" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="H120" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I120" s="27" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="B121" s="27" t="s">
-        <v>233</v>
+      <c r="B121" s="14" t="s">
+        <v>241</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D121" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="E121" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="F121" s="14">
-        <v>0.2</v>
+        <v>202</v>
+      </c>
+      <c r="D121" s="29">
+        <v>70</v>
+      </c>
+      <c r="E121" s="29">
+        <v>70</v>
+      </c>
+      <c r="F121" s="29">
+        <v>70</v>
       </c>
       <c r="G121" s="27" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="H121" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I121" s="27" t="s">
-        <v>210</v>
+        <v>22</v>
+      </c>
+      <c r="I121" s="28" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -5557,19 +5537,19 @@
         <v>232</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>306</v>
+        <v>244</v>
       </c>
       <c r="C122" s="14" t="s">
         <v>208</v>
       </c>
       <c r="D122" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E122" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F122" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G122" s="27" t="s">
         <v>83</v>
@@ -5578,7 +5558,7 @@
         <v>57</v>
       </c>
       <c r="I122" s="27" t="s">
-        <v>308</v>
+        <v>243</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.2">
@@ -5586,19 +5566,19 @@
         <v>232</v>
       </c>
       <c r="B123" s="27" t="s">
-        <v>307</v>
+        <v>233</v>
       </c>
       <c r="C123" s="14" t="s">
         <v>208</v>
       </c>
       <c r="D123" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="E123" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="F123" s="14">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="G123" s="27" t="s">
         <v>83</v>
@@ -5607,7 +5587,7 @@
         <v>57</v>
       </c>
       <c r="I123" s="27" t="s">
-        <v>303</v>
+        <v>210</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -5615,28 +5595,28 @@
         <v>232</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D124" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="E124" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="F124" s="14">
-        <v>0.4</v>
+        <v>0.12</v>
       </c>
       <c r="G124" s="27" t="s">
-        <v>213</v>
+        <v>83</v>
       </c>
       <c r="H124" s="27" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="I124" s="27" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -5644,19 +5624,19 @@
         <v>232</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>234</v>
+        <v>307</v>
       </c>
       <c r="C125" s="14" t="s">
         <v>208</v>
       </c>
       <c r="D125" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="E125" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="F125" s="14">
-        <v>0.3</v>
+        <v>0.12</v>
       </c>
       <c r="G125" s="27" t="s">
         <v>83</v>
@@ -5665,65 +5645,65 @@
         <v>57</v>
       </c>
       <c r="I125" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="27" t="s">
         <v>232</v>
       </c>
       <c r="B126" s="27" t="s">
-        <v>235</v>
+        <v>309</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="D126" s="29">
-        <v>20</v>
-      </c>
-      <c r="E126" s="29">
-        <v>20</v>
-      </c>
-      <c r="F126" s="29">
-        <v>20</v>
+        <v>211</v>
+      </c>
+      <c r="D126" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="E126" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F126" s="14">
+        <v>0.4</v>
       </c>
       <c r="G126" s="27" t="s">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="H126" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="I126" s="28" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="I126" s="27" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="27" t="s">
         <v>232</v>
       </c>
       <c r="B127" s="27" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D127" s="29">
-        <v>20</v>
-      </c>
-      <c r="E127" s="29">
-        <v>20</v>
-      </c>
-      <c r="F127" s="29">
-        <v>20</v>
+        <v>208</v>
+      </c>
+      <c r="D127" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="E127" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F127" s="14">
+        <v>0.3</v>
       </c>
       <c r="G127" s="27" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H127" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I127" s="28" t="s">
-        <v>246</v>
+        <v>57</v>
+      </c>
+      <c r="I127" s="27" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5731,57 +5711,57 @@
         <v>232</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>93</v>
+        <v>219</v>
       </c>
       <c r="D128" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E128" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F128" s="29">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H128" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I128" s="28" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A129" s="27" t="s">
         <v>232</v>
       </c>
       <c r="B129" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>93</v>
       </c>
       <c r="D129" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E129" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F129" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G129" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H129" s="27" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I129" s="28" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -5789,173 +5769,173 @@
         <v>232</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C130" s="14" t="s">
         <v>93</v>
       </c>
       <c r="D130" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="E130" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F130" s="29">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="G130" s="27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H130" s="27" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I130" s="28" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" s="27" t="s">
         <v>232</v>
       </c>
       <c r="B131" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C131" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D131" s="29">
+        <v>0</v>
+      </c>
+      <c r="E131" s="29">
+        <v>0</v>
+      </c>
+      <c r="F131" s="29">
+        <v>0</v>
+      </c>
+      <c r="G131" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H131" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I131" s="28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A132" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D132" s="29">
+        <v>100</v>
+      </c>
+      <c r="E132" s="29">
+        <v>100</v>
+      </c>
+      <c r="F132" s="29">
+        <v>100</v>
+      </c>
+      <c r="G132" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H132" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I132" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B133" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="C131" s="14" t="s">
+      <c r="C133" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="D131" s="14">
+      <c r="D133" s="14">
         <v>0.15</v>
       </c>
-      <c r="E131" s="14">
+      <c r="E133" s="14">
         <v>0.15</v>
       </c>
-      <c r="F131" s="14">
+      <c r="F133" s="14">
         <v>0.15</v>
       </c>
-      <c r="G131" s="27" t="s">
+      <c r="G133" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="H131" s="27" t="s">
+      <c r="H133" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="I131" s="27" t="s">
+      <c r="I133" s="27" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="B132" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D132" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="E132" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F132" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="G132" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H132" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I132" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A133" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="B133" s="35" t="s">
-        <v>262</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D133" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="E133" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="F133" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="G133" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H133" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I133" s="11" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="B134" s="11" t="s">
-        <v>263</v>
+      <c r="B134" s="35" t="s">
+        <v>261</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D134" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E134" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F134" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="H134" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="B135" s="11" t="s">
-        <v>264</v>
+      <c r="B135" s="35" t="s">
+        <v>262</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="D135" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E135" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F135" s="6">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>266</v>
+        <v>83</v>
       </c>
       <c r="H135" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I135" s="11" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -5963,28 +5943,28 @@
         <v>258</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D136" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E136" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F136" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G136" s="11" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="H136" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I136" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -5992,28 +5972,28 @@
         <v>258</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>259</v>
+        <v>93</v>
       </c>
       <c r="D137" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E137" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F137" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G137" s="11" t="s">
-        <v>83</v>
+        <v>266</v>
       </c>
       <c r="H137" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
@@ -6021,19 +6001,19 @@
         <v>258</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C138" s="6" t="s">
         <v>259</v>
       </c>
       <c r="D138" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E138" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F138" s="6">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G138" s="11" t="s">
         <v>83</v>
@@ -6042,7 +6022,7 @@
         <v>22</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -6050,7 +6030,7 @@
         <v>258</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C139" s="6" t="s">
         <v>259</v>
@@ -6071,7 +6051,7 @@
         <v>22</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -6079,28 +6059,28 @@
         <v>258</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="D140" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="E140" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="F140" s="6">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H140" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -6108,28 +6088,28 @@
         <v>258</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="D141" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="E141" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="F141" s="6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H141" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6137,28 +6117,28 @@
         <v>258</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>93</v>
+        <v>279</v>
       </c>
       <c r="D142" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E142" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F142" s="6">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G142" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H142" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6166,19 +6146,19 @@
         <v>258</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D143" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E143" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F143" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G143" s="11" t="s">
         <v>44</v>
@@ -6187,7 +6167,7 @@
         <v>22</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6195,28 +6175,28 @@
         <v>258</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>259</v>
+        <v>93</v>
       </c>
       <c r="D144" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="E144" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="F144" s="6">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="G144" s="11" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="H144" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6224,28 +6204,28 @@
         <v>258</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>259</v>
+        <v>93</v>
       </c>
       <c r="D145" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E145" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F145" s="6">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G145" s="11" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="H145" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.2">
@@ -6253,7 +6233,7 @@
         <v>258</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C146" s="6" t="s">
         <v>259</v>
@@ -6274,7 +6254,7 @@
         <v>22</v>
       </c>
       <c r="I146" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6282,28 +6262,28 @@
         <v>258</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="D147" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="E147" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="F147" s="6">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G147" s="11" t="s">
-        <v>295</v>
+        <v>83</v>
       </c>
       <c r="H147" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
@@ -6311,19 +6291,19 @@
         <v>258</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="D148" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E148" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F148" s="6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G148" s="11" t="s">
         <v>83</v>
@@ -6332,7 +6312,7 @@
         <v>22</v>
       </c>
       <c r="I148" s="11" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.2">
@@ -6340,86 +6320,86 @@
         <v>258</v>
       </c>
       <c r="B149" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D149" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E149" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F149" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G149" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="H149" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I149" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A150" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D150" s="6">
+        <v>0</v>
+      </c>
+      <c r="E150" s="6">
+        <v>0</v>
+      </c>
+      <c r="F150" s="6">
+        <v>0</v>
+      </c>
+      <c r="G150" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H150" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I150" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A151" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B151" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="C149" s="6" t="s">
+      <c r="C151" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="D149" s="6">
+      <c r="D151" s="6">
         <v>0.1</v>
       </c>
-      <c r="E149" s="6">
+      <c r="E151" s="6">
         <v>0.1</v>
       </c>
-      <c r="F149" s="6">
+      <c r="F151" s="6">
         <v>0.1</v>
       </c>
-      <c r="G149" s="11" t="s">
+      <c r="G151" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H149" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I149" s="11" t="s">
+      <c r="H151" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I151" s="11" t="s">
         <v>299</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A150" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B150" s="27" t="s">
-        <v>312</v>
-      </c>
-      <c r="C150" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="D150" s="29">
-        <v>25</v>
-      </c>
-      <c r="E150" s="29">
-        <v>25</v>
-      </c>
-      <c r="F150" s="29">
-        <v>25</v>
-      </c>
-      <c r="G150" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H150" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I150" s="28" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A151" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B151" s="27" t="s">
-        <v>317</v>
-      </c>
-      <c r="C151" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="D151" s="29">
-        <v>-25</v>
-      </c>
-      <c r="E151" s="29">
-        <v>0</v>
-      </c>
-      <c r="F151" s="29">
-        <v>25</v>
-      </c>
-      <c r="G151" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="H151" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I151" s="28" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.2">
@@ -6427,48 +6407,48 @@
         <v>310</v>
       </c>
       <c r="B152" s="27" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D152" s="29">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E152" s="29">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F152" s="29">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G152" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H152" s="27" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="I152" s="28" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A153" s="27" t="s">
         <v>310</v>
       </c>
       <c r="B153" s="27" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>93</v>
+        <v>313</v>
       </c>
       <c r="D153" s="29">
-        <v>85</v>
+        <v>-25</v>
       </c>
       <c r="E153" s="29">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="F153" s="29">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="G153" s="27" t="s">
         <v>44</v>
@@ -6477,7 +6457,7 @@
         <v>46</v>
       </c>
       <c r="I153" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.2">
@@ -6485,19 +6465,19 @@
         <v>310</v>
       </c>
       <c r="B154" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D154" s="29">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="E154" s="29">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="F154" s="29">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G154" s="27" t="s">
         <v>44</v>
@@ -6506,7 +6486,7 @@
         <v>46</v>
       </c>
       <c r="I154" s="28" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">
@@ -6514,28 +6494,28 @@
         <v>310</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>316</v>
+        <v>93</v>
       </c>
       <c r="D155" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="E155" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F155" s="29">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="G155" s="27" t="s">
-        <v>325</v>
+        <v>44</v>
       </c>
       <c r="H155" s="27" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="I155" s="28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.2">
@@ -6543,173 +6523,173 @@
         <v>310</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D156" s="29">
-        <v>2044</v>
+        <v>75</v>
       </c>
       <c r="E156" s="29">
-        <v>2044</v>
+        <v>85</v>
       </c>
       <c r="F156" s="29">
-        <v>2044</v>
+        <v>90</v>
       </c>
       <c r="G156" s="27" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H156" s="27" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I156" s="28" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="27" t="s">
         <v>310</v>
       </c>
       <c r="B157" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="C157" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D157" s="29">
+        <v>0</v>
+      </c>
+      <c r="E157" s="29">
+        <v>0</v>
+      </c>
+      <c r="F157" s="29">
+        <v>0</v>
+      </c>
+      <c r="G157" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="H157" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I157" s="28" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A158" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B158" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C158" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D158" s="29">
+        <v>2044</v>
+      </c>
+      <c r="E158" s="29">
+        <v>2044</v>
+      </c>
+      <c r="F158" s="29">
+        <v>2044</v>
+      </c>
+      <c r="G158" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H158" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I158" s="28" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A159" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B159" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="C157" s="14" t="s">
+      <c r="C159" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="D157" s="29">
+      <c r="D159" s="29">
         <v>-0.04</v>
       </c>
-      <c r="E157" s="29">
+      <c r="E159" s="29">
         <v>-0.04</v>
       </c>
-      <c r="F157" s="29">
+      <c r="F159" s="29">
         <v>-0.04</v>
       </c>
-      <c r="G157" s="27" t="s">
+      <c r="G159" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="H157" s="27" t="s">
+      <c r="H159" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="I157" s="28" t="s">
+      <c r="I159" s="28" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A158" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="B158" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="D158" s="6">
-        <v>500</v>
-      </c>
-      <c r="E158" s="6">
-        <v>500</v>
-      </c>
-      <c r="F158" s="6">
-        <v>500</v>
-      </c>
-      <c r="G158" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="H158" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I158" s="11" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A159" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="B159" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="D159" s="12">
-        <v>20</v>
-      </c>
-      <c r="E159" s="12">
-        <v>20</v>
-      </c>
-      <c r="F159" s="12">
-        <v>20</v>
-      </c>
-      <c r="G159" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H159" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I159" s="13" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
         <v>343</v>
       </c>
       <c r="B160" s="11" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="D160" s="12">
-        <v>20</v>
-      </c>
-      <c r="E160" s="12">
-        <v>20</v>
-      </c>
-      <c r="F160" s="12">
-        <v>20</v>
+        <v>345</v>
+      </c>
+      <c r="D160" s="6">
+        <v>500</v>
+      </c>
+      <c r="E160" s="6">
+        <v>500</v>
+      </c>
+      <c r="F160" s="6">
+        <v>500</v>
       </c>
       <c r="G160" s="11" t="s">
-        <v>44</v>
+        <v>346</v>
       </c>
       <c r="H160" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I160" s="13" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I160" s="11" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
         <v>343</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D161" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E161" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F161" s="12">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G161" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H161" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I161" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -6717,19 +6697,19 @@
         <v>343</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>93</v>
+        <v>352</v>
       </c>
       <c r="D162" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E162" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F162" s="12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G162" s="11" t="s">
         <v>44</v>
@@ -6738,143 +6718,143 @@
         <v>22</v>
       </c>
       <c r="I162" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A163" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B163" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="D163" s="12">
+        <v>7</v>
+      </c>
+      <c r="E163" s="12">
+        <v>7</v>
+      </c>
+      <c r="F163" s="12">
+        <v>7</v>
+      </c>
+      <c r="G163" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H163" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I163" s="13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A164" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B164" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D164" s="12">
+        <v>0</v>
+      </c>
+      <c r="E164" s="12">
+        <v>0</v>
+      </c>
+      <c r="F164" s="12">
+        <v>0</v>
+      </c>
+      <c r="G164" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H164" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I164" s="13" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="163" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="25" t="s">
-        <v>359</v>
-      </c>
-      <c r="B163" s="25" t="s">
-        <v>361</v>
-      </c>
-      <c r="C163" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="D163" s="10">
-        <v>500</v>
-      </c>
-      <c r="E163" s="10">
-        <v>500</v>
-      </c>
-      <c r="F163" s="10">
-        <v>500</v>
-      </c>
-      <c r="G163" s="25" t="s">
-        <v>346</v>
-      </c>
-      <c r="H163" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I163" s="25" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A164" s="25" t="s">
-        <v>359</v>
-      </c>
-      <c r="B164" s="25" t="s">
-        <v>362</v>
-      </c>
-      <c r="C164" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="D164" s="26">
-        <v>20</v>
-      </c>
-      <c r="E164" s="26">
-        <v>20</v>
-      </c>
-      <c r="F164" s="26">
-        <v>20</v>
-      </c>
-      <c r="G164" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H164" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I164" s="30" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="25" t="s">
         <v>359</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="D165" s="26">
-        <v>20</v>
-      </c>
-      <c r="E165" s="26">
-        <v>20</v>
-      </c>
-      <c r="F165" s="26">
-        <v>20</v>
+        <v>360</v>
+      </c>
+      <c r="D165" s="10">
+        <v>500</v>
+      </c>
+      <c r="E165" s="10">
+        <v>500</v>
+      </c>
+      <c r="F165" s="10">
+        <v>500</v>
       </c>
       <c r="G165" s="25" t="s">
-        <v>44</v>
+        <v>346</v>
       </c>
       <c r="H165" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="I165" s="30" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I165" s="25" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A166" s="25" t="s">
         <v>359</v>
       </c>
       <c r="B166" s="25" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C166" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D166" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E166" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F166" s="26">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G166" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H166" s="25" t="s">
         <v>22</v>
       </c>
       <c r="I166" s="30" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A167" s="25" t="s">
         <v>359</v>
       </c>
       <c r="B167" s="25" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>93</v>
+        <v>368</v>
       </c>
       <c r="D167" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E167" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F167" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G167" s="25" t="s">
         <v>44</v>
@@ -6883,123 +6863,123 @@
         <v>22</v>
       </c>
       <c r="I167" s="30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="B168" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="C168" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="D168" s="26">
+        <v>7</v>
+      </c>
+      <c r="E168" s="26">
+        <v>7</v>
+      </c>
+      <c r="F168" s="26">
+        <v>7</v>
+      </c>
+      <c r="G168" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H168" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I168" s="30" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A169" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="B169" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C169" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D169" s="26">
+        <v>0</v>
+      </c>
+      <c r="E169" s="26">
+        <v>0</v>
+      </c>
+      <c r="F169" s="26">
+        <v>0</v>
+      </c>
+      <c r="G169" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H169" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I169" s="30" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A168" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="B168" s="11" t="s">
-        <v>383</v>
-      </c>
-      <c r="C168" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="D168" s="12">
-        <v>2</v>
-      </c>
-      <c r="E168" s="12">
-        <v>2</v>
-      </c>
-      <c r="F168" s="12">
-        <v>2</v>
-      </c>
-      <c r="G168" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="H168" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I168" s="13" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A169" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="B169" s="11" t="s">
-        <v>386</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="D169" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="E169" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="F169" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="G169" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="H169" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I169" s="13" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
         <v>382</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="D170" s="34">
-        <v>80</v>
-      </c>
-      <c r="E170" s="34">
-        <v>80</v>
-      </c>
-      <c r="F170" s="34">
-        <v>80</v>
+        <v>384</v>
+      </c>
+      <c r="D170" s="12">
+        <v>2</v>
+      </c>
+      <c r="E170" s="12">
+        <v>2</v>
+      </c>
+      <c r="F170" s="12">
+        <v>2</v>
       </c>
       <c r="G170" s="11" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="H170" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I170" s="13" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A171" s="11" t="s">
         <v>382</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="D171" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E171" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F171" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G171" s="11" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="H171" s="11" t="s">
         <v>22</v>
       </c>
       <c r="I171" s="13" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
@@ -7007,19 +6987,19 @@
         <v>382</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="D172" s="12">
-        <v>0</v>
-      </c>
-      <c r="E172" s="12">
-        <v>0</v>
-      </c>
-      <c r="F172" s="12">
-        <v>0</v>
+        <v>389</v>
+      </c>
+      <c r="D172" s="34">
+        <v>80</v>
+      </c>
+      <c r="E172" s="34">
+        <v>80</v>
+      </c>
+      <c r="F172" s="34">
+        <v>80</v>
       </c>
       <c r="G172" s="11" t="s">
         <v>44</v>
@@ -7036,10 +7016,10 @@
         <v>382</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D173" s="12">
         <v>0</v>
@@ -7065,10 +7045,10 @@
         <v>382</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D174" s="12">
         <v>0</v>
@@ -7094,19 +7074,19 @@
         <v>382</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D175" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E175" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F175" s="12">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G175" s="11" t="s">
         <v>44</v>
@@ -7118,91 +7098,91 @@
         <v>401</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A176" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="B176" s="27" t="s">
-        <v>411</v>
-      </c>
-      <c r="C176" s="14" t="s">
-        <v>416</v>
-      </c>
-      <c r="D176" s="29">
-        <v>50</v>
-      </c>
-      <c r="E176" s="29">
-        <v>50</v>
-      </c>
-      <c r="F176" s="29">
-        <v>50</v>
-      </c>
-      <c r="G176" s="27" t="s">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A176" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B176" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="D176" s="12">
+        <v>0</v>
+      </c>
+      <c r="E176" s="12">
+        <v>0</v>
+      </c>
+      <c r="F176" s="12">
+        <v>0</v>
+      </c>
+      <c r="G176" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H176" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I176" s="28" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A177" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="B177" s="27" t="s">
-        <v>412</v>
-      </c>
-      <c r="C177" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="D177" s="29">
-        <v>20</v>
-      </c>
-      <c r="E177" s="29">
-        <v>20</v>
-      </c>
-      <c r="F177" s="29">
-        <v>20</v>
-      </c>
-      <c r="G177" s="27" t="s">
+      <c r="H176" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I176" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A177" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B177" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D177" s="12">
+        <v>20</v>
+      </c>
+      <c r="E177" s="12">
+        <v>20</v>
+      </c>
+      <c r="F177" s="12">
+        <v>20</v>
+      </c>
+      <c r="G177" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="H177" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I177" s="28" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H177" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I177" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A178" s="27" t="s">
         <v>410</v>
       </c>
       <c r="B178" s="27" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D178" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E178" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="F178" s="29">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="G178" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H178" s="27" t="s">
         <v>22</v>
       </c>
       <c r="I178" s="28" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -7210,135 +7190,135 @@
         <v>410</v>
       </c>
       <c r="B179" s="27" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>93</v>
+        <v>417</v>
       </c>
       <c r="D179" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E179" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F179" s="29">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G179" s="27" t="s">
         <v>44</v>
       </c>
       <c r="H179" s="27" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="I179" s="28" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="27" t="s">
         <v>410</v>
       </c>
       <c r="B180" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="C180" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="D180" s="29">
+        <v>7</v>
+      </c>
+      <c r="E180" s="29">
+        <v>7</v>
+      </c>
+      <c r="F180" s="29">
+        <v>7</v>
+      </c>
+      <c r="G180" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H180" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="I180" s="28" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A181" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="B181" s="27" t="s">
+        <v>414</v>
+      </c>
+      <c r="C181" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D181" s="29">
+        <v>0</v>
+      </c>
+      <c r="E181" s="29">
+        <v>0</v>
+      </c>
+      <c r="F181" s="29">
+        <v>0</v>
+      </c>
+      <c r="G181" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H181" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I181" s="28" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A182" s="27" t="s">
+        <v>410</v>
+      </c>
+      <c r="B182" s="27" t="s">
         <v>415</v>
       </c>
-      <c r="C180" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D180" s="29">
+      <c r="C182" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D182" s="29">
         <v>100</v>
       </c>
-      <c r="E180" s="29">
+      <c r="E182" s="29">
         <v>100</v>
       </c>
-      <c r="F180" s="29">
+      <c r="F182" s="29">
         <v>100</v>
       </c>
-      <c r="G180" s="27" t="s">
+      <c r="G182" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H180" s="27" t="s">
+      <c r="H182" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="I180" s="28" t="s">
+      <c r="I182" s="28" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A181" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="B181" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="C181" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="D181" s="34">
-        <v>100</v>
-      </c>
-      <c r="E181" s="34">
-        <v>100</v>
-      </c>
-      <c r="F181" s="34">
-        <v>100</v>
-      </c>
-      <c r="G181" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H181" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I181" s="13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A182" s="11" t="s">
-        <v>428</v>
-      </c>
-      <c r="B182" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="C182" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D182" s="12">
-        <v>80</v>
-      </c>
-      <c r="E182" s="12">
-        <v>80</v>
-      </c>
-      <c r="F182" s="12">
-        <v>80</v>
-      </c>
-      <c r="G182" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H182" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I182" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
         <v>428</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="D183" s="12">
-        <v>0</v>
-      </c>
-      <c r="E183" s="12">
-        <v>0</v>
-      </c>
-      <c r="F183" s="12">
-        <v>0</v>
+        <v>429</v>
+      </c>
+      <c r="D183" s="34">
+        <v>100</v>
+      </c>
+      <c r="E183" s="34">
+        <v>100</v>
+      </c>
+      <c r="F183" s="34">
+        <v>100</v>
       </c>
       <c r="G183" s="11" t="s">
         <v>44</v>
@@ -7347,93 +7327,151 @@
         <v>22</v>
       </c>
       <c r="I183" s="13" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A184" s="11" t="s">
         <v>428</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>433</v>
+        <v>93</v>
       </c>
       <c r="D184" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E184" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F184" s="12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G184" s="11" t="s">
         <v>44</v>
       </c>
       <c r="H184" s="11" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="I184" s="13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A185" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="B185" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="C185" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D185" s="12">
+        <v>0</v>
+      </c>
+      <c r="E185" s="12">
+        <v>0</v>
+      </c>
+      <c r="F185" s="12">
+        <v>0</v>
+      </c>
+      <c r="G185" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H185" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I185" s="13" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A186" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="B186" s="11" t="s">
+        <v>434</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="D186" s="12">
+        <v>0</v>
+      </c>
+      <c r="E186" s="12">
+        <v>0</v>
+      </c>
+      <c r="F186" s="12">
+        <v>0</v>
+      </c>
+      <c r="G186" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H186" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I186" s="13" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A185" s="27" t="s">
+    <row r="187" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A187" s="27" t="s">
         <v>437</v>
       </c>
-      <c r="B185" s="27" t="s">
+      <c r="B187" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="C185" s="28" t="s">
+      <c r="C187" s="28" t="s">
         <v>438</v>
       </c>
-      <c r="D185" s="29">
+      <c r="D187" s="29">
         <v>90</v>
       </c>
-      <c r="E185" s="29">
+      <c r="E187" s="29">
         <v>90</v>
       </c>
-      <c r="F185" s="29">
+      <c r="F187" s="29">
         <v>90</v>
       </c>
-      <c r="G185" s="27" t="s">
+      <c r="G187" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H185" s="27" t="s">
+      <c r="H187" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="I185" s="28" t="s">
+      <c r="I187" s="28" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A186" s="27" t="s">
+    <row r="188" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A188" s="27" t="s">
         <v>437</v>
       </c>
-      <c r="B186" s="27" t="s">
+      <c r="B188" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C186" s="28" t="s">
+      <c r="C188" s="28" t="s">
         <v>438</v>
       </c>
-      <c r="D186" s="29">
+      <c r="D188" s="29">
         <v>50</v>
       </c>
-      <c r="E186" s="29">
+      <c r="E188" s="29">
         <v>50</v>
       </c>
-      <c r="F186" s="29">
+      <c r="F188" s="29">
         <v>50</v>
       </c>
-      <c r="G186" s="27" t="s">
+      <c r="G188" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H186" s="27" t="s">
+      <c r="H188" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="I186" s="28" t="s">
+      <c r="I188" s="28" t="s">
         <v>444</v>
       </c>
     </row>

</xml_diff>